<commit_message>
[Add] Protocol : Sign Up
- Making Sign Up Protorol.
</commit_message>
<xml_diff>
--- a/T_Design.xlsx
+++ b/T_Design.xlsx
@@ -5,17 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wave\010_Project\010_Game\Tetris\Commom\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wave\010_Project\010_Game\Tetris\Server\010_Source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E387A904-0DA4-4255-B49E-43D8EFF8D0F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{217C42DC-C76D-47B8-8995-AFE8979CD0FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CBDAA684-FC25-4649-B038-1CECF5D4149C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{CBDAA684-FC25-4649-B038-1CECF5D4149C}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="1" r:id="rId1"/>
     <sheet name="Type" sheetId="5" r:id="rId2"/>
     <sheet name="Protocol_Default" sheetId="2" r:id="rId3"/>
+    <sheet name="SignUp(SC)" sheetId="6" r:id="rId4"/>
+    <sheet name="SignUp(CS)" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="106">
   <si>
     <t>Byte</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -192,6 +194,218 @@
   </si>
   <si>
     <t>Escape Game Room</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Message Secure Code(StoC : 0x59)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User Name #0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User Name #1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User Name #2</t>
+  </si>
+  <si>
+    <t>User Name #3</t>
+  </si>
+  <si>
+    <t>User Name #4</t>
+  </si>
+  <si>
+    <t>User Name #5</t>
+  </si>
+  <si>
+    <t>User Name #6</t>
+  </si>
+  <si>
+    <t>User Name #7</t>
+  </si>
+  <si>
+    <t>User Name #8</t>
+  </si>
+  <si>
+    <t>User Name #9</t>
+  </si>
+  <si>
+    <t>User Name #10</t>
+  </si>
+  <si>
+    <t>User Name #11</t>
+  </si>
+  <si>
+    <t>User Name #12</t>
+  </si>
+  <si>
+    <t>User Name #13</t>
+  </si>
+  <si>
+    <t>User Name #14</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User Name #15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User Name #16</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>spare</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User Name #17(NULL)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User Name #18(NULL)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User ID #1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User ID #2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User ID #3</t>
+  </si>
+  <si>
+    <t>User ID #4</t>
+  </si>
+  <si>
+    <t>User ID #5</t>
+  </si>
+  <si>
+    <t>User ID #6</t>
+  </si>
+  <si>
+    <t>User ID #7</t>
+  </si>
+  <si>
+    <t>User ID #8</t>
+  </si>
+  <si>
+    <t>User ID #9</t>
+  </si>
+  <si>
+    <t>User ID #10</t>
+  </si>
+  <si>
+    <t>User ID #11</t>
+  </si>
+  <si>
+    <t>User ID #12</t>
+  </si>
+  <si>
+    <t>User ID #13</t>
+  </si>
+  <si>
+    <t>User ID #14</t>
+  </si>
+  <si>
+    <t>User ID #15</t>
+  </si>
+  <si>
+    <t>User ID #16</t>
+  </si>
+  <si>
+    <t>User ID #17(NULL)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User ID #18(NULL)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Password #1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Password #2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Password #3</t>
+  </si>
+  <si>
+    <t>Password #4</t>
+  </si>
+  <si>
+    <t>Password #5</t>
+  </si>
+  <si>
+    <t>Password #6</t>
+  </si>
+  <si>
+    <t>Password #7</t>
+  </si>
+  <si>
+    <t>Password #8</t>
+  </si>
+  <si>
+    <t>Password #9</t>
+  </si>
+  <si>
+    <t>Password #10</t>
+  </si>
+  <si>
+    <t>Password #11</t>
+  </si>
+  <si>
+    <t>Password #12</t>
+  </si>
+  <si>
+    <t>Password #13</t>
+  </si>
+  <si>
+    <t>Password #14</t>
+  </si>
+  <si>
+    <t>Password #15</t>
+  </si>
+  <si>
+    <t>Password #16</t>
+  </si>
+  <si>
+    <t>Password #17(NULL)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Password #18(NULL)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Message Size (126 BYTE)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Message Type (0x01 : Sign Up)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Message Secure CodeCtoS : 0x47)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Message Type (0x01 Sign Up)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Message Size(5 BYTE)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Result (0x00 : OK, 0x01 : USER ID Already Exists, 0x02 : ETC Error)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -390,7 +604,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -408,6 +622,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -449,6 +669,33 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -782,8 +1029,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3CD6B57-0370-464C-92D1-8CCB08728235}">
   <dimension ref="C2:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -796,16 +1043,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="G2" s="7" t="s">
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="G2" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
     </row>
     <row r="3" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C3" s="3" t="s">
@@ -1062,18 +1309,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="N2" s="8" t="str">
+      <c r="N2" s="10" t="str">
         <f>Type!C2</f>
         <v>Server -&gt; Client</v>
       </c>
-      <c r="O2" s="8"/>
-      <c r="P2" s="8"/>
-      <c r="R2" s="8" t="str">
+      <c r="O2" s="10"/>
+      <c r="P2" s="10"/>
+      <c r="R2" s="10" t="str">
         <f>Type!G2</f>
         <v>Client -&gt; Server</v>
       </c>
-      <c r="S2" s="8"/>
-      <c r="T2" s="8"/>
+      <c r="S2" s="10"/>
+      <c r="T2" s="10"/>
     </row>
     <row r="3" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="6" t="s">
@@ -1135,16 +1382,16 @@
       <c r="B4" s="4">
         <v>0</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
       <c r="K4" s="4" t="s">
         <v>11</v>
       </c>
@@ -1177,17 +1424,17 @@
       <c r="B5" s="4">
         <v>1</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="18"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="20"/>
       <c r="N5" s="2" t="str">
         <f>IF(ISBLANK(Type!C5),"",Type!C5)</f>
         <v>0x02</v>
@@ -1217,15 +1464,15 @@
       <c r="B6" s="4">
         <v>2</v>
       </c>
-      <c r="C6" s="12"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="19"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="21"/>
       <c r="N6" s="2" t="str">
         <f>IF(ISBLANK(Type!C6),"",Type!C6)</f>
         <v>0x03</v>
@@ -1255,16 +1502,16 @@
       <c r="B7" s="4">
         <v>3</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="17"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="19"/>
       <c r="K7" s="5"/>
       <c r="N7" s="2" t="str">
         <f>IF(ISBLANK(Type!C7),"",Type!C7)</f>
@@ -1949,4 +2196,3298 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EFC3663-0FC5-4A8A-9C01-6D666EC91148}">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
+  <dimension ref="B2:T24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2.625" customWidth="1"/>
+    <col min="2" max="2" width="4.625" style="1" customWidth="1"/>
+    <col min="3" max="10" width="8.625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="25.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="2.625" customWidth="1"/>
+    <col min="14" max="14" width="14.625" customWidth="1"/>
+    <col min="15" max="15" width="20.625" customWidth="1"/>
+    <col min="17" max="17" width="2.625" customWidth="1"/>
+    <col min="18" max="18" width="14.625" customWidth="1"/>
+    <col min="19" max="19" width="20.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="N2" s="10" t="str">
+        <f>Type!C2</f>
+        <v>Server -&gt; Client</v>
+      </c>
+      <c r="O2" s="10"/>
+      <c r="P2" s="10"/>
+      <c r="R2" s="10" t="str">
+        <f>Type!G2</f>
+        <v>Client -&gt; Server</v>
+      </c>
+      <c r="S2" s="10"/>
+      <c r="T2" s="10"/>
+    </row>
+    <row r="3" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="N3" s="8" t="str">
+        <f>Type!C3</f>
+        <v>Message Type</v>
+      </c>
+      <c r="O3" s="8" t="str">
+        <f>Type!D3</f>
+        <v>Description</v>
+      </c>
+      <c r="P3" s="8" t="str">
+        <f>Type!E3</f>
+        <v>Size</v>
+      </c>
+      <c r="R3" s="8" t="str">
+        <f>Type!G3</f>
+        <v>Message Type</v>
+      </c>
+      <c r="S3" s="8" t="str">
+        <f>Type!H3</f>
+        <v>Description</v>
+      </c>
+      <c r="T3" s="8" t="str">
+        <f>Type!I3</f>
+        <v>Size</v>
+      </c>
+    </row>
+    <row r="4" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B4" s="7">
+        <v>0</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="N4" s="2" t="str">
+        <f>IF(ISBLANK(Type!C4),"",Type!C4)</f>
+        <v>0x01</v>
+      </c>
+      <c r="O4" s="2" t="str">
+        <f>IF(ISBLANK(Type!D4),"",Type!D4)</f>
+        <v>Sign Up</v>
+      </c>
+      <c r="P4" s="2" t="str">
+        <f>IF(ISBLANK(Type!E4),"",Type!E4)</f>
+        <v>Variable</v>
+      </c>
+      <c r="R4" s="2" t="str">
+        <f>IF(ISBLANK(Type!G4),"",Type!G4)</f>
+        <v>0x01</v>
+      </c>
+      <c r="S4" s="2" t="str">
+        <f>IF(ISBLANK(Type!H4),"",Type!H4)</f>
+        <v>Sign Up</v>
+      </c>
+      <c r="T4" s="2" t="str">
+        <f>IF(ISBLANK(Type!I4),"",Type!I4)</f>
+        <v>Variable</v>
+      </c>
+    </row>
+    <row r="5" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B5" s="7">
+        <v>1</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="20"/>
+      <c r="N5" s="2" t="str">
+        <f>IF(ISBLANK(Type!C5),"",Type!C5)</f>
+        <v>0x02</v>
+      </c>
+      <c r="O5" s="2" t="str">
+        <f>IF(ISBLANK(Type!D5),"",Type!D5)</f>
+        <v>Sign In</v>
+      </c>
+      <c r="P5" s="2" t="str">
+        <f>IF(ISBLANK(Type!E5),"",Type!E5)</f>
+        <v>Variable</v>
+      </c>
+      <c r="R5" s="2" t="str">
+        <f>IF(ISBLANK(Type!G5),"",Type!G5)</f>
+        <v>0x02</v>
+      </c>
+      <c r="S5" s="2" t="str">
+        <f>IF(ISBLANK(Type!H5),"",Type!H5)</f>
+        <v>Sign In</v>
+      </c>
+      <c r="T5" s="2" t="str">
+        <f>IF(ISBLANK(Type!I5),"",Type!I5)</f>
+        <v>Variable</v>
+      </c>
+    </row>
+    <row r="6" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B6" s="7">
+        <v>2</v>
+      </c>
+      <c r="C6" s="14"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="21"/>
+      <c r="N6" s="2" t="str">
+        <f>IF(ISBLANK(Type!C6),"",Type!C6)</f>
+        <v>0x03</v>
+      </c>
+      <c r="O6" s="2" t="str">
+        <f>IF(ISBLANK(Type!D6),"",Type!D6)</f>
+        <v>Sign Out</v>
+      </c>
+      <c r="P6" s="2" t="str">
+        <f>IF(ISBLANK(Type!E6),"",Type!E6)</f>
+        <v>Variable</v>
+      </c>
+      <c r="R6" s="2" t="str">
+        <f>IF(ISBLANK(Type!G6),"",Type!G6)</f>
+        <v>0x03</v>
+      </c>
+      <c r="S6" s="2" t="str">
+        <f>IF(ISBLANK(Type!H6),"",Type!H6)</f>
+        <v>Sign Out</v>
+      </c>
+      <c r="T6" s="2" t="str">
+        <f>IF(ISBLANK(Type!I6),"",Type!I6)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B7" s="7">
+        <v>3</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="5"/>
+      <c r="N7" s="2" t="str">
+        <f>IF(ISBLANK(Type!C7),"",Type!C7)</f>
+        <v>0x04</v>
+      </c>
+      <c r="O7" s="2" t="str">
+        <f>IF(ISBLANK(Type!D7),"",Type!D7)</f>
+        <v>Lobby Chat</v>
+      </c>
+      <c r="P7" s="2" t="str">
+        <f>IF(ISBLANK(Type!E7),"",Type!E7)</f>
+        <v>Variable</v>
+      </c>
+      <c r="R7" s="2" t="str">
+        <f>IF(ISBLANK(Type!G7),"",Type!G7)</f>
+        <v>0x04</v>
+      </c>
+      <c r="S7" s="2" t="str">
+        <f>IF(ISBLANK(Type!H7),"",Type!H7)</f>
+        <v>Lobby Chat</v>
+      </c>
+      <c r="T7" s="2" t="str">
+        <f>IF(ISBLANK(Type!I7),"",Type!I7)</f>
+        <v>Variable</v>
+      </c>
+    </row>
+    <row r="8" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B8" s="2">
+        <v>4</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="30"/>
+      <c r="K8" s="2"/>
+      <c r="N8" s="2" t="str">
+        <f>IF(ISBLANK(Type!C8),"",Type!C8)</f>
+        <v>0x05</v>
+      </c>
+      <c r="O8" s="2" t="str">
+        <f>IF(ISBLANK(Type!D8),"",Type!D8)</f>
+        <v>Ingame Chat</v>
+      </c>
+      <c r="P8" s="2" t="str">
+        <f>IF(ISBLANK(Type!E8),"",Type!E8)</f>
+        <v>Variable</v>
+      </c>
+      <c r="R8" s="2" t="str">
+        <f>IF(ISBLANK(Type!G8),"",Type!G8)</f>
+        <v>0x05</v>
+      </c>
+      <c r="S8" s="2" t="str">
+        <f>IF(ISBLANK(Type!H8),"",Type!H8)</f>
+        <v>Ingame Chat</v>
+      </c>
+      <c r="T8" s="2" t="str">
+        <f>IF(ISBLANK(Type!I8),"",Type!I8)</f>
+        <v>Variable</v>
+      </c>
+    </row>
+    <row r="9" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="N9" s="2" t="str">
+        <f>IF(ISBLANK(Type!C9),"",Type!C9)</f>
+        <v>0x06</v>
+      </c>
+      <c r="O9" s="2" t="str">
+        <f>IF(ISBLANK(Type!D9),"",Type!D9)</f>
+        <v>Change User Info</v>
+      </c>
+      <c r="P9" s="2" t="str">
+        <f>IF(ISBLANK(Type!E9),"",Type!E9)</f>
+        <v>Variable</v>
+      </c>
+      <c r="R9" s="2" t="str">
+        <f>IF(ISBLANK(Type!G9),"",Type!G9)</f>
+        <v>0x06</v>
+      </c>
+      <c r="S9" s="2" t="str">
+        <f>IF(ISBLANK(Type!H9),"",Type!H9)</f>
+        <v>Change User Info</v>
+      </c>
+      <c r="T9" s="2" t="str">
+        <f>IF(ISBLANK(Type!I9),"",Type!I9)</f>
+        <v>Variable</v>
+      </c>
+    </row>
+    <row r="10" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="N10" s="2" t="str">
+        <f>IF(ISBLANK(Type!C10),"",Type!C10)</f>
+        <v>0x07</v>
+      </c>
+      <c r="O10" s="2" t="str">
+        <f>IF(ISBLANK(Type!D10),"",Type!D10)</f>
+        <v>Ingame Cmd(S-&gt;C)</v>
+      </c>
+      <c r="P10" s="2" t="str">
+        <f>IF(ISBLANK(Type!E10),"",Type!E10)</f>
+        <v/>
+      </c>
+      <c r="R10" s="2" t="str">
+        <f>IF(ISBLANK(Type!G10),"",Type!G10)</f>
+        <v>0x07</v>
+      </c>
+      <c r="S10" s="2" t="str">
+        <f>IF(ISBLANK(Type!H10),"",Type!H10)</f>
+        <v>Ingame Cmd(C-&gt;S)</v>
+      </c>
+      <c r="T10" s="2" t="str">
+        <f>IF(ISBLANK(Type!I10),"",Type!I10)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="N11" s="2" t="str">
+        <f>IF(ISBLANK(Type!C11),"",Type!C11)</f>
+        <v>0x08</v>
+      </c>
+      <c r="O11" s="2" t="str">
+        <f>IF(ISBLANK(Type!D11),"",Type!D11)</f>
+        <v>Enter Game Room</v>
+      </c>
+      <c r="P11" s="2" t="str">
+        <f>IF(ISBLANK(Type!E11),"",Type!E11)</f>
+        <v/>
+      </c>
+      <c r="R11" s="2" t="str">
+        <f>IF(ISBLANK(Type!G11),"",Type!G11)</f>
+        <v>0x08</v>
+      </c>
+      <c r="S11" s="2" t="str">
+        <f>IF(ISBLANK(Type!H11),"",Type!H11)</f>
+        <v>Enter Game Room</v>
+      </c>
+      <c r="T11" s="2" t="str">
+        <f>IF(ISBLANK(Type!I11),"",Type!I11)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="N12" s="2" t="str">
+        <f>IF(ISBLANK(Type!C12),"",Type!C12)</f>
+        <v>0x09</v>
+      </c>
+      <c r="O12" s="2" t="str">
+        <f>IF(ISBLANK(Type!D12),"",Type!D12)</f>
+        <v>Escape Game Room</v>
+      </c>
+      <c r="P12" s="2" t="str">
+        <f>IF(ISBLANK(Type!E12),"",Type!E12)</f>
+        <v/>
+      </c>
+      <c r="R12" s="2" t="str">
+        <f>IF(ISBLANK(Type!G12),"",Type!G12)</f>
+        <v>0x09</v>
+      </c>
+      <c r="S12" s="2" t="str">
+        <f>IF(ISBLANK(Type!H12),"",Type!H12)</f>
+        <v>Escape Game Room</v>
+      </c>
+      <c r="T12" s="2" t="str">
+        <f>IF(ISBLANK(Type!I12),"",Type!I12)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="N13" s="2" t="str">
+        <f>IF(ISBLANK(Type!C13),"",Type!C13)</f>
+        <v>0x0A</v>
+      </c>
+      <c r="O13" s="2" t="str">
+        <f>IF(ISBLANK(Type!D13),"",Type!D13)</f>
+        <v>Heart Beat</v>
+      </c>
+      <c r="P13" s="2" t="str">
+        <f>IF(ISBLANK(Type!E13),"",Type!E13)</f>
+        <v/>
+      </c>
+      <c r="R13" s="2" t="str">
+        <f>IF(ISBLANK(Type!G13),"",Type!G13)</f>
+        <v>0x0A</v>
+      </c>
+      <c r="S13" s="2" t="str">
+        <f>IF(ISBLANK(Type!H13),"",Type!H13)</f>
+        <v>Heart Beat</v>
+      </c>
+      <c r="T13" s="2" t="str">
+        <f>IF(ISBLANK(Type!I13),"",Type!I13)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="N14" s="2" t="str">
+        <f>IF(ISBLANK(Type!C14),"",Type!C14)</f>
+        <v>0x0B</v>
+      </c>
+      <c r="O14" s="2" t="str">
+        <f>IF(ISBLANK(Type!D14),"",Type!D14)</f>
+        <v>In Game Whole Data</v>
+      </c>
+      <c r="P14" s="2">
+        <f>IF(ISBLANK(Type!E14),"",Type!E14)</f>
+        <v>1300</v>
+      </c>
+      <c r="R14" s="2" t="str">
+        <f>IF(ISBLANK(Type!G14),"",Type!G14)</f>
+        <v>0x0B</v>
+      </c>
+      <c r="S14" s="2" t="str">
+        <f>IF(ISBLANK(Type!H14),"",Type!H14)</f>
+        <v>In Game My Data</v>
+      </c>
+      <c r="T14" s="2">
+        <f>IF(ISBLANK(Type!I14),"",Type!I14)</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="15" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="N15" s="2" t="str">
+        <f>IF(ISBLANK(Type!C15),"",Type!C15)</f>
+        <v/>
+      </c>
+      <c r="O15" s="2" t="str">
+        <f>IF(ISBLANK(Type!D15),"",Type!D15)</f>
+        <v/>
+      </c>
+      <c r="P15" s="2" t="str">
+        <f>IF(ISBLANK(Type!E15),"",Type!E15)</f>
+        <v/>
+      </c>
+      <c r="R15" s="2" t="str">
+        <f>IF(ISBLANK(Type!G15),"",Type!G15)</f>
+        <v/>
+      </c>
+      <c r="S15" s="2" t="str">
+        <f>IF(ISBLANK(Type!H15),"",Type!H15)</f>
+        <v/>
+      </c>
+      <c r="T15" s="2" t="str">
+        <f>IF(ISBLANK(Type!I15),"",Type!I15)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="N16" s="2" t="str">
+        <f>IF(ISBLANK(Type!C16),"",Type!C16)</f>
+        <v/>
+      </c>
+      <c r="O16" s="2" t="str">
+        <f>IF(ISBLANK(Type!D16),"",Type!D16)</f>
+        <v/>
+      </c>
+      <c r="P16" s="2" t="str">
+        <f>IF(ISBLANK(Type!E16),"",Type!E16)</f>
+        <v/>
+      </c>
+      <c r="R16" s="2" t="str">
+        <f>IF(ISBLANK(Type!G16),"",Type!G16)</f>
+        <v/>
+      </c>
+      <c r="S16" s="2" t="str">
+        <f>IF(ISBLANK(Type!H16),"",Type!H16)</f>
+        <v/>
+      </c>
+      <c r="T16" s="2" t="str">
+        <f>IF(ISBLANK(Type!I16),"",Type!I16)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="14:20" x14ac:dyDescent="0.3">
+      <c r="N17" s="2" t="str">
+        <f>IF(ISBLANK(Type!C17),"",Type!C17)</f>
+        <v/>
+      </c>
+      <c r="O17" s="2" t="str">
+        <f>IF(ISBLANK(Type!D17),"",Type!D17)</f>
+        <v/>
+      </c>
+      <c r="P17" s="2" t="str">
+        <f>IF(ISBLANK(Type!E17),"",Type!E17)</f>
+        <v/>
+      </c>
+      <c r="R17" s="2" t="str">
+        <f>IF(ISBLANK(Type!G17),"",Type!G17)</f>
+        <v/>
+      </c>
+      <c r="S17" s="2" t="str">
+        <f>IF(ISBLANK(Type!H17),"",Type!H17)</f>
+        <v/>
+      </c>
+      <c r="T17" s="2" t="str">
+        <f>IF(ISBLANK(Type!I17),"",Type!I17)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="14:20" x14ac:dyDescent="0.3">
+      <c r="N18" s="2" t="str">
+        <f>IF(ISBLANK(Type!C18),"",Type!C18)</f>
+        <v/>
+      </c>
+      <c r="O18" s="2" t="str">
+        <f>IF(ISBLANK(Type!D18),"",Type!D18)</f>
+        <v/>
+      </c>
+      <c r="P18" s="2" t="str">
+        <f>IF(ISBLANK(Type!E18),"",Type!E18)</f>
+        <v/>
+      </c>
+      <c r="R18" s="2" t="str">
+        <f>IF(ISBLANK(Type!G18),"",Type!G18)</f>
+        <v/>
+      </c>
+      <c r="S18" s="2" t="str">
+        <f>IF(ISBLANK(Type!H18),"",Type!H18)</f>
+        <v/>
+      </c>
+      <c r="T18" s="2" t="str">
+        <f>IF(ISBLANK(Type!I18),"",Type!I18)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="14:20" x14ac:dyDescent="0.3">
+      <c r="N19" s="2" t="str">
+        <f>IF(ISBLANK(Type!C19),"",Type!C19)</f>
+        <v/>
+      </c>
+      <c r="O19" s="2" t="str">
+        <f>IF(ISBLANK(Type!D19),"",Type!D19)</f>
+        <v/>
+      </c>
+      <c r="P19" s="2" t="str">
+        <f>IF(ISBLANK(Type!E19),"",Type!E19)</f>
+        <v/>
+      </c>
+      <c r="R19" s="2" t="str">
+        <f>IF(ISBLANK(Type!G19),"",Type!G19)</f>
+        <v/>
+      </c>
+      <c r="S19" s="2" t="str">
+        <f>IF(ISBLANK(Type!H19),"",Type!H19)</f>
+        <v/>
+      </c>
+      <c r="T19" s="2" t="str">
+        <f>IF(ISBLANK(Type!I19),"",Type!I19)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="14:20" x14ac:dyDescent="0.3">
+      <c r="N20" s="2" t="str">
+        <f>IF(ISBLANK(Type!C20),"",Type!C20)</f>
+        <v/>
+      </c>
+      <c r="O20" s="2" t="str">
+        <f>IF(ISBLANK(Type!D20),"",Type!D20)</f>
+        <v/>
+      </c>
+      <c r="P20" s="2" t="str">
+        <f>IF(ISBLANK(Type!E20),"",Type!E20)</f>
+        <v/>
+      </c>
+      <c r="R20" s="2" t="str">
+        <f>IF(ISBLANK(Type!G20),"",Type!G20)</f>
+        <v/>
+      </c>
+      <c r="S20" s="2" t="str">
+        <f>IF(ISBLANK(Type!H20),"",Type!H20)</f>
+        <v/>
+      </c>
+      <c r="T20" s="2" t="str">
+        <f>IF(ISBLANK(Type!I20),"",Type!I20)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="14:20" x14ac:dyDescent="0.3">
+      <c r="N21" s="2" t="str">
+        <f>IF(ISBLANK(Type!C21),"",Type!C21)</f>
+        <v/>
+      </c>
+      <c r="O21" s="2" t="str">
+        <f>IF(ISBLANK(Type!D21),"",Type!D21)</f>
+        <v/>
+      </c>
+      <c r="P21" s="2" t="str">
+        <f>IF(ISBLANK(Type!E21),"",Type!E21)</f>
+        <v/>
+      </c>
+      <c r="R21" s="2" t="str">
+        <f>IF(ISBLANK(Type!G21),"",Type!G21)</f>
+        <v/>
+      </c>
+      <c r="S21" s="2" t="str">
+        <f>IF(ISBLANK(Type!H21),"",Type!H21)</f>
+        <v/>
+      </c>
+      <c r="T21" s="2" t="str">
+        <f>IF(ISBLANK(Type!I21),"",Type!I21)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="14:20" x14ac:dyDescent="0.3">
+      <c r="N22" s="2" t="str">
+        <f>IF(ISBLANK(Type!C22),"",Type!C22)</f>
+        <v/>
+      </c>
+      <c r="O22" s="2" t="str">
+        <f>IF(ISBLANK(Type!D22),"",Type!D22)</f>
+        <v/>
+      </c>
+      <c r="P22" s="2" t="str">
+        <f>IF(ISBLANK(Type!E22),"",Type!E22)</f>
+        <v/>
+      </c>
+      <c r="R22" s="2" t="str">
+        <f>IF(ISBLANK(Type!G22),"",Type!G22)</f>
+        <v/>
+      </c>
+      <c r="S22" s="2" t="str">
+        <f>IF(ISBLANK(Type!H22),"",Type!H22)</f>
+        <v/>
+      </c>
+      <c r="T22" s="2" t="str">
+        <f>IF(ISBLANK(Type!I22),"",Type!I22)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="14:20" x14ac:dyDescent="0.3">
+      <c r="N23" s="2" t="str">
+        <f>IF(ISBLANK(Type!C23),"",Type!C23)</f>
+        <v/>
+      </c>
+      <c r="O23" s="2" t="str">
+        <f>IF(ISBLANK(Type!D23),"",Type!D23)</f>
+        <v/>
+      </c>
+      <c r="P23" s="2" t="str">
+        <f>IF(ISBLANK(Type!E23),"",Type!E23)</f>
+        <v/>
+      </c>
+      <c r="R23" s="2" t="str">
+        <f>IF(ISBLANK(Type!G23),"",Type!G23)</f>
+        <v/>
+      </c>
+      <c r="S23" s="2" t="str">
+        <f>IF(ISBLANK(Type!H23),"",Type!H23)</f>
+        <v/>
+      </c>
+      <c r="T23" s="2" t="str">
+        <f>IF(ISBLANK(Type!I23),"",Type!I23)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="14:20" x14ac:dyDescent="0.3">
+      <c r="N24" s="2" t="str">
+        <f>IF(ISBLANK(Type!C24),"",Type!C24)</f>
+        <v/>
+      </c>
+      <c r="O24" s="2" t="str">
+        <f>IF(ISBLANK(Type!D24),"",Type!D24)</f>
+        <v/>
+      </c>
+      <c r="P24" s="2" t="str">
+        <f>IF(ISBLANK(Type!E24),"",Type!E24)</f>
+        <v/>
+      </c>
+      <c r="R24" s="2" t="str">
+        <f>IF(ISBLANK(Type!G24),"",Type!G24)</f>
+        <v/>
+      </c>
+      <c r="S24" s="2" t="str">
+        <f>IF(ISBLANK(Type!H24),"",Type!H24)</f>
+        <v/>
+      </c>
+      <c r="T24" s="2" t="str">
+        <f>IF(ISBLANK(Type!I24),"",Type!I24)</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="C8:J8"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="R2:T2"/>
+    <mergeCell ref="C4:J4"/>
+    <mergeCell ref="C5:J6"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="C7:J7"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E24A41A-84D0-4ECE-B49A-FE464E02F847}">
+  <sheetPr>
+    <tabColor rgb="FF0070C0"/>
+  </sheetPr>
+  <dimension ref="B2:T129"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22:J23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2.625" customWidth="1"/>
+    <col min="2" max="2" width="4.625" style="1" customWidth="1"/>
+    <col min="3" max="10" width="8.625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="25.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="2.625" customWidth="1"/>
+    <col min="14" max="14" width="14.625" customWidth="1"/>
+    <col min="15" max="15" width="20.625" customWidth="1"/>
+    <col min="17" max="17" width="2.625" customWidth="1"/>
+    <col min="18" max="18" width="14.625" customWidth="1"/>
+    <col min="19" max="19" width="20.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="N2" s="10" t="str">
+        <f>Type!C2</f>
+        <v>Server -&gt; Client</v>
+      </c>
+      <c r="O2" s="10"/>
+      <c r="P2" s="10"/>
+      <c r="R2" s="10" t="str">
+        <f>Type!G2</f>
+        <v>Client -&gt; Server</v>
+      </c>
+      <c r="S2" s="10"/>
+      <c r="T2" s="10"/>
+    </row>
+    <row r="3" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="N3" s="8" t="str">
+        <f>Type!C3</f>
+        <v>Message Type</v>
+      </c>
+      <c r="O3" s="8" t="str">
+        <f>Type!D3</f>
+        <v>Description</v>
+      </c>
+      <c r="P3" s="8" t="str">
+        <f>Type!E3</f>
+        <v>Size</v>
+      </c>
+      <c r="R3" s="8" t="str">
+        <f>Type!G3</f>
+        <v>Message Type</v>
+      </c>
+      <c r="S3" s="8" t="str">
+        <f>Type!H3</f>
+        <v>Description</v>
+      </c>
+      <c r="T3" s="8" t="str">
+        <f>Type!I3</f>
+        <v>Size</v>
+      </c>
+    </row>
+    <row r="4" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B4" s="7">
+        <v>0</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="N4" s="2" t="str">
+        <f>IF(ISBLANK(Type!C4),"",Type!C4)</f>
+        <v>0x01</v>
+      </c>
+      <c r="O4" s="2" t="str">
+        <f>IF(ISBLANK(Type!D4),"",Type!D4)</f>
+        <v>Sign Up</v>
+      </c>
+      <c r="P4" s="2" t="str">
+        <f>IF(ISBLANK(Type!E4),"",Type!E4)</f>
+        <v>Variable</v>
+      </c>
+      <c r="R4" s="2" t="str">
+        <f>IF(ISBLANK(Type!G4),"",Type!G4)</f>
+        <v>0x01</v>
+      </c>
+      <c r="S4" s="2" t="str">
+        <f>IF(ISBLANK(Type!H4),"",Type!H4)</f>
+        <v>Sign Up</v>
+      </c>
+      <c r="T4" s="2" t="str">
+        <f>IF(ISBLANK(Type!I4),"",Type!I4)</f>
+        <v>Variable</v>
+      </c>
+    </row>
+    <row r="5" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B5" s="7">
+        <v>1</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="20"/>
+      <c r="N5" s="2" t="str">
+        <f>IF(ISBLANK(Type!C5),"",Type!C5)</f>
+        <v>0x02</v>
+      </c>
+      <c r="O5" s="2" t="str">
+        <f>IF(ISBLANK(Type!D5),"",Type!D5)</f>
+        <v>Sign In</v>
+      </c>
+      <c r="P5" s="2" t="str">
+        <f>IF(ISBLANK(Type!E5),"",Type!E5)</f>
+        <v>Variable</v>
+      </c>
+      <c r="R5" s="2" t="str">
+        <f>IF(ISBLANK(Type!G5),"",Type!G5)</f>
+        <v>0x02</v>
+      </c>
+      <c r="S5" s="2" t="str">
+        <f>IF(ISBLANK(Type!H5),"",Type!H5)</f>
+        <v>Sign In</v>
+      </c>
+      <c r="T5" s="2" t="str">
+        <f>IF(ISBLANK(Type!I5),"",Type!I5)</f>
+        <v>Variable</v>
+      </c>
+    </row>
+    <row r="6" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B6" s="7">
+        <v>2</v>
+      </c>
+      <c r="C6" s="14"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="21"/>
+      <c r="N6" s="2" t="str">
+        <f>IF(ISBLANK(Type!C6),"",Type!C6)</f>
+        <v>0x03</v>
+      </c>
+      <c r="O6" s="2" t="str">
+        <f>IF(ISBLANK(Type!D6),"",Type!D6)</f>
+        <v>Sign Out</v>
+      </c>
+      <c r="P6" s="2" t="str">
+        <f>IF(ISBLANK(Type!E6),"",Type!E6)</f>
+        <v>Variable</v>
+      </c>
+      <c r="R6" s="2" t="str">
+        <f>IF(ISBLANK(Type!G6),"",Type!G6)</f>
+        <v>0x03</v>
+      </c>
+      <c r="S6" s="2" t="str">
+        <f>IF(ISBLANK(Type!H6),"",Type!H6)</f>
+        <v>Sign Out</v>
+      </c>
+      <c r="T6" s="2" t="str">
+        <f>IF(ISBLANK(Type!I6),"",Type!I6)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B7" s="7">
+        <v>3</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="5"/>
+      <c r="N7" s="2" t="str">
+        <f>IF(ISBLANK(Type!C7),"",Type!C7)</f>
+        <v>0x04</v>
+      </c>
+      <c r="O7" s="2" t="str">
+        <f>IF(ISBLANK(Type!D7),"",Type!D7)</f>
+        <v>Lobby Chat</v>
+      </c>
+      <c r="P7" s="2" t="str">
+        <f>IF(ISBLANK(Type!E7),"",Type!E7)</f>
+        <v>Variable</v>
+      </c>
+      <c r="R7" s="2" t="str">
+        <f>IF(ISBLANK(Type!G7),"",Type!G7)</f>
+        <v>0x04</v>
+      </c>
+      <c r="S7" s="2" t="str">
+        <f>IF(ISBLANK(Type!H7),"",Type!H7)</f>
+        <v>Lobby Chat</v>
+      </c>
+      <c r="T7" s="2" t="str">
+        <f>IF(ISBLANK(Type!I7),"",Type!I7)</f>
+        <v>Variable</v>
+      </c>
+    </row>
+    <row r="8" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B8" s="2">
+        <v>4</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="2"/>
+      <c r="N8" s="2" t="str">
+        <f>IF(ISBLANK(Type!C8),"",Type!C8)</f>
+        <v>0x05</v>
+      </c>
+      <c r="O8" s="2" t="str">
+        <f>IF(ISBLANK(Type!D8),"",Type!D8)</f>
+        <v>Ingame Chat</v>
+      </c>
+      <c r="P8" s="2" t="str">
+        <f>IF(ISBLANK(Type!E8),"",Type!E8)</f>
+        <v>Variable</v>
+      </c>
+      <c r="R8" s="2" t="str">
+        <f>IF(ISBLANK(Type!G8),"",Type!G8)</f>
+        <v>0x05</v>
+      </c>
+      <c r="S8" s="2" t="str">
+        <f>IF(ISBLANK(Type!H8),"",Type!H8)</f>
+        <v>Ingame Chat</v>
+      </c>
+      <c r="T8" s="2" t="str">
+        <f>IF(ISBLANK(Type!I8),"",Type!I8)</f>
+        <v>Variable</v>
+      </c>
+    </row>
+    <row r="9" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B9" s="2">
+        <v>5</v>
+      </c>
+      <c r="C9" s="25"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="2"/>
+      <c r="N9" s="2" t="str">
+        <f>IF(ISBLANK(Type!C9),"",Type!C9)</f>
+        <v>0x06</v>
+      </c>
+      <c r="O9" s="2" t="str">
+        <f>IF(ISBLANK(Type!D9),"",Type!D9)</f>
+        <v>Change User Info</v>
+      </c>
+      <c r="P9" s="2" t="str">
+        <f>IF(ISBLANK(Type!E9),"",Type!E9)</f>
+        <v>Variable</v>
+      </c>
+      <c r="R9" s="2" t="str">
+        <f>IF(ISBLANK(Type!G9),"",Type!G9)</f>
+        <v>0x06</v>
+      </c>
+      <c r="S9" s="2" t="str">
+        <f>IF(ISBLANK(Type!H9),"",Type!H9)</f>
+        <v>Change User Info</v>
+      </c>
+      <c r="T9" s="2" t="str">
+        <f>IF(ISBLANK(Type!I9),"",Type!I9)</f>
+        <v>Variable</v>
+      </c>
+    </row>
+    <row r="10" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B10" s="2">
+        <v>6</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="2"/>
+      <c r="N10" s="2" t="str">
+        <f>IF(ISBLANK(Type!C10),"",Type!C10)</f>
+        <v>0x07</v>
+      </c>
+      <c r="O10" s="2" t="str">
+        <f>IF(ISBLANK(Type!D10),"",Type!D10)</f>
+        <v>Ingame Cmd(S-&gt;C)</v>
+      </c>
+      <c r="P10" s="2" t="str">
+        <f>IF(ISBLANK(Type!E10),"",Type!E10)</f>
+        <v/>
+      </c>
+      <c r="R10" s="2" t="str">
+        <f>IF(ISBLANK(Type!G10),"",Type!G10)</f>
+        <v>0x07</v>
+      </c>
+      <c r="S10" s="2" t="str">
+        <f>IF(ISBLANK(Type!H10),"",Type!H10)</f>
+        <v>Ingame Cmd(C-&gt;S)</v>
+      </c>
+      <c r="T10" s="2" t="str">
+        <f>IF(ISBLANK(Type!I10),"",Type!I10)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B11" s="2">
+        <v>7</v>
+      </c>
+      <c r="C11" s="25"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="2"/>
+      <c r="N11" s="2" t="str">
+        <f>IF(ISBLANK(Type!C11),"",Type!C11)</f>
+        <v>0x08</v>
+      </c>
+      <c r="O11" s="2" t="str">
+        <f>IF(ISBLANK(Type!D11),"",Type!D11)</f>
+        <v>Enter Game Room</v>
+      </c>
+      <c r="P11" s="2" t="str">
+        <f>IF(ISBLANK(Type!E11),"",Type!E11)</f>
+        <v/>
+      </c>
+      <c r="R11" s="2" t="str">
+        <f>IF(ISBLANK(Type!G11),"",Type!G11)</f>
+        <v>0x08</v>
+      </c>
+      <c r="S11" s="2" t="str">
+        <f>IF(ISBLANK(Type!H11),"",Type!H11)</f>
+        <v>Enter Game Room</v>
+      </c>
+      <c r="T11" s="2" t="str">
+        <f>IF(ISBLANK(Type!I11),"",Type!I11)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B12" s="2">
+        <v>8</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="2"/>
+      <c r="N12" s="2" t="str">
+        <f>IF(ISBLANK(Type!C12),"",Type!C12)</f>
+        <v>0x09</v>
+      </c>
+      <c r="O12" s="2" t="str">
+        <f>IF(ISBLANK(Type!D12),"",Type!D12)</f>
+        <v>Escape Game Room</v>
+      </c>
+      <c r="P12" s="2" t="str">
+        <f>IF(ISBLANK(Type!E12),"",Type!E12)</f>
+        <v/>
+      </c>
+      <c r="R12" s="2" t="str">
+        <f>IF(ISBLANK(Type!G12),"",Type!G12)</f>
+        <v>0x09</v>
+      </c>
+      <c r="S12" s="2" t="str">
+        <f>IF(ISBLANK(Type!H12),"",Type!H12)</f>
+        <v>Escape Game Room</v>
+      </c>
+      <c r="T12" s="2" t="str">
+        <f>IF(ISBLANK(Type!I12),"",Type!I12)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B13" s="2">
+        <v>9</v>
+      </c>
+      <c r="C13" s="25"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="2"/>
+      <c r="N13" s="2" t="str">
+        <f>IF(ISBLANK(Type!C13),"",Type!C13)</f>
+        <v>0x0A</v>
+      </c>
+      <c r="O13" s="2" t="str">
+        <f>IF(ISBLANK(Type!D13),"",Type!D13)</f>
+        <v>Heart Beat</v>
+      </c>
+      <c r="P13" s="2" t="str">
+        <f>IF(ISBLANK(Type!E13),"",Type!E13)</f>
+        <v/>
+      </c>
+      <c r="R13" s="2" t="str">
+        <f>IF(ISBLANK(Type!G13),"",Type!G13)</f>
+        <v>0x0A</v>
+      </c>
+      <c r="S13" s="2" t="str">
+        <f>IF(ISBLANK(Type!H13),"",Type!H13)</f>
+        <v>Heart Beat</v>
+      </c>
+      <c r="T13" s="2" t="str">
+        <f>IF(ISBLANK(Type!I13),"",Type!I13)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B14" s="2">
+        <v>10</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="24"/>
+      <c r="K14" s="2"/>
+      <c r="N14" s="2" t="str">
+        <f>IF(ISBLANK(Type!C14),"",Type!C14)</f>
+        <v>0x0B</v>
+      </c>
+      <c r="O14" s="2" t="str">
+        <f>IF(ISBLANK(Type!D14),"",Type!D14)</f>
+        <v>In Game Whole Data</v>
+      </c>
+      <c r="P14" s="2">
+        <f>IF(ISBLANK(Type!E14),"",Type!E14)</f>
+        <v>1300</v>
+      </c>
+      <c r="R14" s="2" t="str">
+        <f>IF(ISBLANK(Type!G14),"",Type!G14)</f>
+        <v>0x0B</v>
+      </c>
+      <c r="S14" s="2" t="str">
+        <f>IF(ISBLANK(Type!H14),"",Type!H14)</f>
+        <v>In Game My Data</v>
+      </c>
+      <c r="T14" s="2">
+        <f>IF(ISBLANK(Type!I14),"",Type!I14)</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="15" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B15" s="2">
+        <v>11</v>
+      </c>
+      <c r="C15" s="25"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="2"/>
+      <c r="N15" s="2" t="str">
+        <f>IF(ISBLANK(Type!C15),"",Type!C15)</f>
+        <v/>
+      </c>
+      <c r="O15" s="2" t="str">
+        <f>IF(ISBLANK(Type!D15),"",Type!D15)</f>
+        <v/>
+      </c>
+      <c r="P15" s="2" t="str">
+        <f>IF(ISBLANK(Type!E15),"",Type!E15)</f>
+        <v/>
+      </c>
+      <c r="R15" s="2" t="str">
+        <f>IF(ISBLANK(Type!G15),"",Type!G15)</f>
+        <v/>
+      </c>
+      <c r="S15" s="2" t="str">
+        <f>IF(ISBLANK(Type!H15),"",Type!H15)</f>
+        <v/>
+      </c>
+      <c r="T15" s="2" t="str">
+        <f>IF(ISBLANK(Type!I15),"",Type!I15)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B16" s="2">
+        <v>12</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="24"/>
+      <c r="K16" s="2"/>
+      <c r="N16" s="2" t="str">
+        <f>IF(ISBLANK(Type!C16),"",Type!C16)</f>
+        <v/>
+      </c>
+      <c r="O16" s="2" t="str">
+        <f>IF(ISBLANK(Type!D16),"",Type!D16)</f>
+        <v/>
+      </c>
+      <c r="P16" s="2" t="str">
+        <f>IF(ISBLANK(Type!E16),"",Type!E16)</f>
+        <v/>
+      </c>
+      <c r="R16" s="2" t="str">
+        <f>IF(ISBLANK(Type!G16),"",Type!G16)</f>
+        <v/>
+      </c>
+      <c r="S16" s="2" t="str">
+        <f>IF(ISBLANK(Type!H16),"",Type!H16)</f>
+        <v/>
+      </c>
+      <c r="T16" s="2" t="str">
+        <f>IF(ISBLANK(Type!I16),"",Type!I16)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B17" s="2">
+        <v>13</v>
+      </c>
+      <c r="C17" s="25"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="2"/>
+      <c r="N17" s="2" t="str">
+        <f>IF(ISBLANK(Type!C17),"",Type!C17)</f>
+        <v/>
+      </c>
+      <c r="O17" s="2" t="str">
+        <f>IF(ISBLANK(Type!D17),"",Type!D17)</f>
+        <v/>
+      </c>
+      <c r="P17" s="2" t="str">
+        <f>IF(ISBLANK(Type!E17),"",Type!E17)</f>
+        <v/>
+      </c>
+      <c r="R17" s="2" t="str">
+        <f>IF(ISBLANK(Type!G17),"",Type!G17)</f>
+        <v/>
+      </c>
+      <c r="S17" s="2" t="str">
+        <f>IF(ISBLANK(Type!H17),"",Type!H17)</f>
+        <v/>
+      </c>
+      <c r="T17" s="2" t="str">
+        <f>IF(ISBLANK(Type!I17),"",Type!I17)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B18" s="2">
+        <v>14</v>
+      </c>
+      <c r="C18" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="23"/>
+      <c r="I18" s="23"/>
+      <c r="J18" s="24"/>
+      <c r="K18" s="2"/>
+      <c r="N18" s="2" t="str">
+        <f>IF(ISBLANK(Type!C18),"",Type!C18)</f>
+        <v/>
+      </c>
+      <c r="O18" s="2" t="str">
+        <f>IF(ISBLANK(Type!D18),"",Type!D18)</f>
+        <v/>
+      </c>
+      <c r="P18" s="2" t="str">
+        <f>IF(ISBLANK(Type!E18),"",Type!E18)</f>
+        <v/>
+      </c>
+      <c r="R18" s="2" t="str">
+        <f>IF(ISBLANK(Type!G18),"",Type!G18)</f>
+        <v/>
+      </c>
+      <c r="S18" s="2" t="str">
+        <f>IF(ISBLANK(Type!H18),"",Type!H18)</f>
+        <v/>
+      </c>
+      <c r="T18" s="2" t="str">
+        <f>IF(ISBLANK(Type!I18),"",Type!I18)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B19" s="2">
+        <v>15</v>
+      </c>
+      <c r="C19" s="25"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="26"/>
+      <c r="I19" s="26"/>
+      <c r="J19" s="27"/>
+      <c r="K19" s="2"/>
+      <c r="N19" s="2" t="str">
+        <f>IF(ISBLANK(Type!C19),"",Type!C19)</f>
+        <v/>
+      </c>
+      <c r="O19" s="2" t="str">
+        <f>IF(ISBLANK(Type!D19),"",Type!D19)</f>
+        <v/>
+      </c>
+      <c r="P19" s="2" t="str">
+        <f>IF(ISBLANK(Type!E19),"",Type!E19)</f>
+        <v/>
+      </c>
+      <c r="R19" s="2" t="str">
+        <f>IF(ISBLANK(Type!G19),"",Type!G19)</f>
+        <v/>
+      </c>
+      <c r="S19" s="2" t="str">
+        <f>IF(ISBLANK(Type!H19),"",Type!H19)</f>
+        <v/>
+      </c>
+      <c r="T19" s="2" t="str">
+        <f>IF(ISBLANK(Type!I19),"",Type!I19)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B20" s="2">
+        <v>16</v>
+      </c>
+      <c r="C20" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="24"/>
+      <c r="K20" s="2"/>
+      <c r="N20" s="2" t="str">
+        <f>IF(ISBLANK(Type!C20),"",Type!C20)</f>
+        <v/>
+      </c>
+      <c r="O20" s="2" t="str">
+        <f>IF(ISBLANK(Type!D20),"",Type!D20)</f>
+        <v/>
+      </c>
+      <c r="P20" s="2" t="str">
+        <f>IF(ISBLANK(Type!E20),"",Type!E20)</f>
+        <v/>
+      </c>
+      <c r="R20" s="2" t="str">
+        <f>IF(ISBLANK(Type!G20),"",Type!G20)</f>
+        <v/>
+      </c>
+      <c r="S20" s="2" t="str">
+        <f>IF(ISBLANK(Type!H20),"",Type!H20)</f>
+        <v/>
+      </c>
+      <c r="T20" s="2" t="str">
+        <f>IF(ISBLANK(Type!I20),"",Type!I20)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B21" s="2">
+        <v>17</v>
+      </c>
+      <c r="C21" s="25"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="26"/>
+      <c r="J21" s="27"/>
+      <c r="K21" s="2"/>
+      <c r="N21" s="2" t="str">
+        <f>IF(ISBLANK(Type!C21),"",Type!C21)</f>
+        <v/>
+      </c>
+      <c r="O21" s="2" t="str">
+        <f>IF(ISBLANK(Type!D21),"",Type!D21)</f>
+        <v/>
+      </c>
+      <c r="P21" s="2" t="str">
+        <f>IF(ISBLANK(Type!E21),"",Type!E21)</f>
+        <v/>
+      </c>
+      <c r="R21" s="2" t="str">
+        <f>IF(ISBLANK(Type!G21),"",Type!G21)</f>
+        <v/>
+      </c>
+      <c r="S21" s="2" t="str">
+        <f>IF(ISBLANK(Type!H21),"",Type!H21)</f>
+        <v/>
+      </c>
+      <c r="T21" s="2" t="str">
+        <f>IF(ISBLANK(Type!I21),"",Type!I21)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B22" s="2">
+        <v>18</v>
+      </c>
+      <c r="C22" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="23"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="23"/>
+      <c r="I22" s="23"/>
+      <c r="J22" s="24"/>
+      <c r="K22" s="2"/>
+      <c r="N22" s="2" t="str">
+        <f>IF(ISBLANK(Type!C22),"",Type!C22)</f>
+        <v/>
+      </c>
+      <c r="O22" s="2" t="str">
+        <f>IF(ISBLANK(Type!D22),"",Type!D22)</f>
+        <v/>
+      </c>
+      <c r="P22" s="2" t="str">
+        <f>IF(ISBLANK(Type!E22),"",Type!E22)</f>
+        <v/>
+      </c>
+      <c r="R22" s="2" t="str">
+        <f>IF(ISBLANK(Type!G22),"",Type!G22)</f>
+        <v/>
+      </c>
+      <c r="S22" s="2" t="str">
+        <f>IF(ISBLANK(Type!H22),"",Type!H22)</f>
+        <v/>
+      </c>
+      <c r="T22" s="2" t="str">
+        <f>IF(ISBLANK(Type!I22),"",Type!I22)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B23" s="2">
+        <v>19</v>
+      </c>
+      <c r="C23" s="25"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="26"/>
+      <c r="I23" s="26"/>
+      <c r="J23" s="27"/>
+      <c r="K23" s="2"/>
+      <c r="N23" s="2" t="str">
+        <f>IF(ISBLANK(Type!C23),"",Type!C23)</f>
+        <v/>
+      </c>
+      <c r="O23" s="2" t="str">
+        <f>IF(ISBLANK(Type!D23),"",Type!D23)</f>
+        <v/>
+      </c>
+      <c r="P23" s="2" t="str">
+        <f>IF(ISBLANK(Type!E23),"",Type!E23)</f>
+        <v/>
+      </c>
+      <c r="R23" s="2" t="str">
+        <f>IF(ISBLANK(Type!G23),"",Type!G23)</f>
+        <v/>
+      </c>
+      <c r="S23" s="2" t="str">
+        <f>IF(ISBLANK(Type!H23),"",Type!H23)</f>
+        <v/>
+      </c>
+      <c r="T23" s="2" t="str">
+        <f>IF(ISBLANK(Type!I23),"",Type!I23)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B24" s="2">
+        <v>20</v>
+      </c>
+      <c r="C24" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="D24" s="23"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="23"/>
+      <c r="G24" s="23"/>
+      <c r="H24" s="23"/>
+      <c r="I24" s="23"/>
+      <c r="J24" s="24"/>
+      <c r="K24" s="2"/>
+      <c r="N24" s="2" t="str">
+        <f>IF(ISBLANK(Type!C24),"",Type!C24)</f>
+        <v/>
+      </c>
+      <c r="O24" s="2" t="str">
+        <f>IF(ISBLANK(Type!D24),"",Type!D24)</f>
+        <v/>
+      </c>
+      <c r="P24" s="2" t="str">
+        <f>IF(ISBLANK(Type!E24),"",Type!E24)</f>
+        <v/>
+      </c>
+      <c r="R24" s="2" t="str">
+        <f>IF(ISBLANK(Type!G24),"",Type!G24)</f>
+        <v/>
+      </c>
+      <c r="S24" s="2" t="str">
+        <f>IF(ISBLANK(Type!H24),"",Type!H24)</f>
+        <v/>
+      </c>
+      <c r="T24" s="2" t="str">
+        <f>IF(ISBLANK(Type!I24),"",Type!I24)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B25" s="2">
+        <v>21</v>
+      </c>
+      <c r="C25" s="25"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="26"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="26"/>
+      <c r="J25" s="27"/>
+      <c r="K25" s="2"/>
+    </row>
+    <row r="26" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B26" s="2">
+        <v>22</v>
+      </c>
+      <c r="C26" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="D26" s="23"/>
+      <c r="E26" s="23"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="23"/>
+      <c r="H26" s="23"/>
+      <c r="I26" s="23"/>
+      <c r="J26" s="24"/>
+      <c r="K26" s="2"/>
+    </row>
+    <row r="27" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B27" s="2">
+        <v>23</v>
+      </c>
+      <c r="C27" s="25"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="26"/>
+      <c r="G27" s="26"/>
+      <c r="H27" s="26"/>
+      <c r="I27" s="26"/>
+      <c r="J27" s="27"/>
+      <c r="K27" s="2"/>
+    </row>
+    <row r="28" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B28" s="2">
+        <v>24</v>
+      </c>
+      <c r="C28" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="23"/>
+      <c r="J28" s="24"/>
+      <c r="K28" s="2"/>
+    </row>
+    <row r="29" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B29" s="2">
+        <v>25</v>
+      </c>
+      <c r="C29" s="25"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="27"/>
+      <c r="K29" s="2"/>
+    </row>
+    <row r="30" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B30" s="2">
+        <v>26</v>
+      </c>
+      <c r="C30" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="D30" s="23"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="23"/>
+      <c r="G30" s="23"/>
+      <c r="H30" s="23"/>
+      <c r="I30" s="23"/>
+      <c r="J30" s="24"/>
+      <c r="K30" s="2"/>
+    </row>
+    <row r="31" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B31" s="2">
+        <v>27</v>
+      </c>
+      <c r="C31" s="25"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="26"/>
+      <c r="F31" s="26"/>
+      <c r="G31" s="26"/>
+      <c r="H31" s="26"/>
+      <c r="I31" s="26"/>
+      <c r="J31" s="27"/>
+      <c r="K31" s="2"/>
+    </row>
+    <row r="32" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B32" s="2">
+        <v>28</v>
+      </c>
+      <c r="C32" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="D32" s="23"/>
+      <c r="E32" s="23"/>
+      <c r="F32" s="23"/>
+      <c r="G32" s="23"/>
+      <c r="H32" s="23"/>
+      <c r="I32" s="23"/>
+      <c r="J32" s="24"/>
+      <c r="K32" s="2"/>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B33" s="2">
+        <v>29</v>
+      </c>
+      <c r="C33" s="25"/>
+      <c r="D33" s="26"/>
+      <c r="E33" s="26"/>
+      <c r="F33" s="26"/>
+      <c r="G33" s="26"/>
+      <c r="H33" s="26"/>
+      <c r="I33" s="26"/>
+      <c r="J33" s="27"/>
+      <c r="K33" s="2"/>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B34" s="2">
+        <v>30</v>
+      </c>
+      <c r="C34" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="D34" s="23"/>
+      <c r="E34" s="23"/>
+      <c r="F34" s="23"/>
+      <c r="G34" s="23"/>
+      <c r="H34" s="23"/>
+      <c r="I34" s="23"/>
+      <c r="J34" s="24"/>
+      <c r="K34" s="2"/>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B35" s="2">
+        <v>31</v>
+      </c>
+      <c r="C35" s="25"/>
+      <c r="D35" s="26"/>
+      <c r="E35" s="26"/>
+      <c r="F35" s="26"/>
+      <c r="G35" s="26"/>
+      <c r="H35" s="26"/>
+      <c r="I35" s="26"/>
+      <c r="J35" s="27"/>
+      <c r="K35" s="2"/>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B36" s="2">
+        <v>32</v>
+      </c>
+      <c r="C36" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="D36" s="23"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="23"/>
+      <c r="G36" s="23"/>
+      <c r="H36" s="23"/>
+      <c r="I36" s="23"/>
+      <c r="J36" s="24"/>
+      <c r="K36" s="2"/>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B37" s="2">
+        <v>33</v>
+      </c>
+      <c r="C37" s="25"/>
+      <c r="D37" s="26"/>
+      <c r="E37" s="26"/>
+      <c r="F37" s="26"/>
+      <c r="G37" s="26"/>
+      <c r="H37" s="26"/>
+      <c r="I37" s="26"/>
+      <c r="J37" s="27"/>
+      <c r="K37" s="2"/>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B38" s="2">
+        <v>34</v>
+      </c>
+      <c r="C38" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="D38" s="23"/>
+      <c r="E38" s="23"/>
+      <c r="F38" s="23"/>
+      <c r="G38" s="23"/>
+      <c r="H38" s="23"/>
+      <c r="I38" s="23"/>
+      <c r="J38" s="24"/>
+      <c r="K38" s="2"/>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B39" s="2">
+        <v>35</v>
+      </c>
+      <c r="C39" s="25"/>
+      <c r="D39" s="26"/>
+      <c r="E39" s="26"/>
+      <c r="F39" s="26"/>
+      <c r="G39" s="26"/>
+      <c r="H39" s="26"/>
+      <c r="I39" s="26"/>
+      <c r="J39" s="27"/>
+      <c r="K39" s="2"/>
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B40" s="2">
+        <v>36</v>
+      </c>
+      <c r="C40" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="D40" s="23"/>
+      <c r="E40" s="23"/>
+      <c r="F40" s="23"/>
+      <c r="G40" s="23"/>
+      <c r="H40" s="23"/>
+      <c r="I40" s="23"/>
+      <c r="J40" s="24"/>
+      <c r="K40" s="2"/>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B41" s="2">
+        <v>37</v>
+      </c>
+      <c r="C41" s="25"/>
+      <c r="D41" s="26"/>
+      <c r="E41" s="26"/>
+      <c r="F41" s="26"/>
+      <c r="G41" s="26"/>
+      <c r="H41" s="26"/>
+      <c r="I41" s="26"/>
+      <c r="J41" s="27"/>
+      <c r="K41" s="2"/>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B42" s="2">
+        <v>38</v>
+      </c>
+      <c r="C42" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="D42" s="23"/>
+      <c r="E42" s="23"/>
+      <c r="F42" s="23"/>
+      <c r="G42" s="23"/>
+      <c r="H42" s="23"/>
+      <c r="I42" s="23"/>
+      <c r="J42" s="24"/>
+      <c r="K42" s="2"/>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B43" s="2">
+        <v>39</v>
+      </c>
+      <c r="C43" s="25"/>
+      <c r="D43" s="26"/>
+      <c r="E43" s="26"/>
+      <c r="F43" s="26"/>
+      <c r="G43" s="26"/>
+      <c r="H43" s="26"/>
+      <c r="I43" s="26"/>
+      <c r="J43" s="27"/>
+      <c r="K43" s="2"/>
+    </row>
+    <row r="44" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B44" s="2">
+        <v>40</v>
+      </c>
+      <c r="C44" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="D44" s="23"/>
+      <c r="E44" s="23"/>
+      <c r="F44" s="23"/>
+      <c r="G44" s="23"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="24"/>
+      <c r="K44" s="2"/>
+    </row>
+    <row r="45" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B45" s="2">
+        <v>41</v>
+      </c>
+      <c r="C45" s="25"/>
+      <c r="D45" s="26"/>
+      <c r="E45" s="26"/>
+      <c r="F45" s="26"/>
+      <c r="G45" s="26"/>
+      <c r="H45" s="26"/>
+      <c r="I45" s="26"/>
+      <c r="J45" s="27"/>
+      <c r="K45" s="2"/>
+    </row>
+    <row r="46" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B46" s="2">
+        <v>42</v>
+      </c>
+      <c r="C46" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="D46" s="23"/>
+      <c r="E46" s="23"/>
+      <c r="F46" s="23"/>
+      <c r="G46" s="23"/>
+      <c r="H46" s="23"/>
+      <c r="I46" s="23"/>
+      <c r="J46" s="24"/>
+      <c r="K46" s="2"/>
+    </row>
+    <row r="47" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B47" s="2">
+        <v>43</v>
+      </c>
+      <c r="C47" s="25"/>
+      <c r="D47" s="26"/>
+      <c r="E47" s="26"/>
+      <c r="F47" s="26"/>
+      <c r="G47" s="26"/>
+      <c r="H47" s="26"/>
+      <c r="I47" s="26"/>
+      <c r="J47" s="27"/>
+      <c r="K47" s="2"/>
+    </row>
+    <row r="48" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B48" s="2">
+        <v>44</v>
+      </c>
+      <c r="C48" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="D48" s="23"/>
+      <c r="E48" s="23"/>
+      <c r="F48" s="23"/>
+      <c r="G48" s="23"/>
+      <c r="H48" s="23"/>
+      <c r="I48" s="23"/>
+      <c r="J48" s="24"/>
+      <c r="K48" s="2"/>
+    </row>
+    <row r="49" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B49" s="2">
+        <v>45</v>
+      </c>
+      <c r="C49" s="25"/>
+      <c r="D49" s="26"/>
+      <c r="E49" s="26"/>
+      <c r="F49" s="26"/>
+      <c r="G49" s="26"/>
+      <c r="H49" s="26"/>
+      <c r="I49" s="26"/>
+      <c r="J49" s="27"/>
+      <c r="K49" s="2"/>
+    </row>
+    <row r="50" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B50" s="2">
+        <v>46</v>
+      </c>
+      <c r="C50" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="D50" s="23"/>
+      <c r="E50" s="23"/>
+      <c r="F50" s="23"/>
+      <c r="G50" s="23"/>
+      <c r="H50" s="23"/>
+      <c r="I50" s="23"/>
+      <c r="J50" s="24"/>
+      <c r="K50" s="2"/>
+    </row>
+    <row r="51" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B51" s="2">
+        <v>47</v>
+      </c>
+      <c r="C51" s="25"/>
+      <c r="D51" s="26"/>
+      <c r="E51" s="26"/>
+      <c r="F51" s="26"/>
+      <c r="G51" s="26"/>
+      <c r="H51" s="26"/>
+      <c r="I51" s="26"/>
+      <c r="J51" s="27"/>
+      <c r="K51" s="2"/>
+    </row>
+    <row r="52" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B52" s="2">
+        <v>48</v>
+      </c>
+      <c r="C52" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="D52" s="23"/>
+      <c r="E52" s="23"/>
+      <c r="F52" s="23"/>
+      <c r="G52" s="23"/>
+      <c r="H52" s="23"/>
+      <c r="I52" s="23"/>
+      <c r="J52" s="24"/>
+      <c r="K52" s="2"/>
+    </row>
+    <row r="53" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B53" s="2">
+        <v>49</v>
+      </c>
+      <c r="C53" s="25"/>
+      <c r="D53" s="26"/>
+      <c r="E53" s="26"/>
+      <c r="F53" s="26"/>
+      <c r="G53" s="26"/>
+      <c r="H53" s="26"/>
+      <c r="I53" s="26"/>
+      <c r="J53" s="27"/>
+      <c r="K53" s="2"/>
+    </row>
+    <row r="54" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B54" s="2">
+        <v>50</v>
+      </c>
+      <c r="C54" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="D54" s="23"/>
+      <c r="E54" s="23"/>
+      <c r="F54" s="23"/>
+      <c r="G54" s="23"/>
+      <c r="H54" s="23"/>
+      <c r="I54" s="23"/>
+      <c r="J54" s="24"/>
+      <c r="K54" s="2"/>
+    </row>
+    <row r="55" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B55" s="2">
+        <v>51</v>
+      </c>
+      <c r="C55" s="25"/>
+      <c r="D55" s="26"/>
+      <c r="E55" s="26"/>
+      <c r="F55" s="26"/>
+      <c r="G55" s="26"/>
+      <c r="H55" s="26"/>
+      <c r="I55" s="26"/>
+      <c r="J55" s="27"/>
+      <c r="K55" s="2"/>
+    </row>
+    <row r="56" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B56" s="2">
+        <v>52</v>
+      </c>
+      <c r="C56" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="D56" s="23"/>
+      <c r="E56" s="23"/>
+      <c r="F56" s="23"/>
+      <c r="G56" s="23"/>
+      <c r="H56" s="23"/>
+      <c r="I56" s="23"/>
+      <c r="J56" s="24"/>
+      <c r="K56" s="2"/>
+    </row>
+    <row r="57" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B57" s="2">
+        <v>53</v>
+      </c>
+      <c r="C57" s="25"/>
+      <c r="D57" s="26"/>
+      <c r="E57" s="26"/>
+      <c r="F57" s="26"/>
+      <c r="G57" s="26"/>
+      <c r="H57" s="26"/>
+      <c r="I57" s="26"/>
+      <c r="J57" s="27"/>
+      <c r="K57" s="2"/>
+    </row>
+    <row r="58" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B58" s="2">
+        <v>54</v>
+      </c>
+      <c r="C58" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="D58" s="23"/>
+      <c r="E58" s="23"/>
+      <c r="F58" s="23"/>
+      <c r="G58" s="23"/>
+      <c r="H58" s="23"/>
+      <c r="I58" s="23"/>
+      <c r="J58" s="24"/>
+      <c r="K58" s="2"/>
+    </row>
+    <row r="59" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B59" s="2">
+        <v>55</v>
+      </c>
+      <c r="C59" s="25"/>
+      <c r="D59" s="26"/>
+      <c r="E59" s="26"/>
+      <c r="F59" s="26"/>
+      <c r="G59" s="26"/>
+      <c r="H59" s="26"/>
+      <c r="I59" s="26"/>
+      <c r="J59" s="27"/>
+      <c r="K59" s="2"/>
+    </row>
+    <row r="60" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B60" s="2">
+        <v>56</v>
+      </c>
+      <c r="C60" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="D60" s="23"/>
+      <c r="E60" s="23"/>
+      <c r="F60" s="23"/>
+      <c r="G60" s="23"/>
+      <c r="H60" s="23"/>
+      <c r="I60" s="23"/>
+      <c r="J60" s="24"/>
+      <c r="K60" s="2"/>
+    </row>
+    <row r="61" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B61" s="2">
+        <v>57</v>
+      </c>
+      <c r="C61" s="25"/>
+      <c r="D61" s="26"/>
+      <c r="E61" s="26"/>
+      <c r="F61" s="26"/>
+      <c r="G61" s="26"/>
+      <c r="H61" s="26"/>
+      <c r="I61" s="26"/>
+      <c r="J61" s="27"/>
+      <c r="K61" s="2"/>
+    </row>
+    <row r="62" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B62" s="2">
+        <v>58</v>
+      </c>
+      <c r="C62" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="D62" s="23"/>
+      <c r="E62" s="23"/>
+      <c r="F62" s="23"/>
+      <c r="G62" s="23"/>
+      <c r="H62" s="23"/>
+      <c r="I62" s="23"/>
+      <c r="J62" s="24"/>
+      <c r="K62" s="2"/>
+    </row>
+    <row r="63" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B63" s="2">
+        <v>59</v>
+      </c>
+      <c r="C63" s="25"/>
+      <c r="D63" s="26"/>
+      <c r="E63" s="26"/>
+      <c r="F63" s="26"/>
+      <c r="G63" s="26"/>
+      <c r="H63" s="26"/>
+      <c r="I63" s="26"/>
+      <c r="J63" s="27"/>
+      <c r="K63" s="2"/>
+    </row>
+    <row r="64" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B64" s="2">
+        <v>60</v>
+      </c>
+      <c r="C64" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="D64" s="23"/>
+      <c r="E64" s="23"/>
+      <c r="F64" s="23"/>
+      <c r="G64" s="23"/>
+      <c r="H64" s="23"/>
+      <c r="I64" s="23"/>
+      <c r="J64" s="24"/>
+      <c r="K64" s="2"/>
+    </row>
+    <row r="65" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B65" s="2">
+        <v>61</v>
+      </c>
+      <c r="C65" s="25"/>
+      <c r="D65" s="26"/>
+      <c r="E65" s="26"/>
+      <c r="F65" s="26"/>
+      <c r="G65" s="26"/>
+      <c r="H65" s="26"/>
+      <c r="I65" s="26"/>
+      <c r="J65" s="27"/>
+      <c r="K65" s="2"/>
+    </row>
+    <row r="66" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B66" s="2">
+        <v>62</v>
+      </c>
+      <c r="C66" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="D66" s="23"/>
+      <c r="E66" s="23"/>
+      <c r="F66" s="23"/>
+      <c r="G66" s="23"/>
+      <c r="H66" s="23"/>
+      <c r="I66" s="23"/>
+      <c r="J66" s="24"/>
+      <c r="K66" s="2"/>
+    </row>
+    <row r="67" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B67" s="2">
+        <v>63</v>
+      </c>
+      <c r="C67" s="25"/>
+      <c r="D67" s="26"/>
+      <c r="E67" s="26"/>
+      <c r="F67" s="26"/>
+      <c r="G67" s="26"/>
+      <c r="H67" s="26"/>
+      <c r="I67" s="26"/>
+      <c r="J67" s="27"/>
+      <c r="K67" s="2"/>
+    </row>
+    <row r="68" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B68" s="2">
+        <v>64</v>
+      </c>
+      <c r="C68" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="D68" s="23"/>
+      <c r="E68" s="23"/>
+      <c r="F68" s="23"/>
+      <c r="G68" s="23"/>
+      <c r="H68" s="23"/>
+      <c r="I68" s="23"/>
+      <c r="J68" s="24"/>
+      <c r="K68" s="2"/>
+    </row>
+    <row r="69" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B69" s="2">
+        <v>65</v>
+      </c>
+      <c r="C69" s="25"/>
+      <c r="D69" s="26"/>
+      <c r="E69" s="26"/>
+      <c r="F69" s="26"/>
+      <c r="G69" s="26"/>
+      <c r="H69" s="26"/>
+      <c r="I69" s="26"/>
+      <c r="J69" s="27"/>
+      <c r="K69" s="2"/>
+    </row>
+    <row r="70" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B70" s="2">
+        <v>66</v>
+      </c>
+      <c r="C70" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="D70" s="23"/>
+      <c r="E70" s="23"/>
+      <c r="F70" s="23"/>
+      <c r="G70" s="23"/>
+      <c r="H70" s="23"/>
+      <c r="I70" s="23"/>
+      <c r="J70" s="24"/>
+      <c r="K70" s="2"/>
+    </row>
+    <row r="71" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B71" s="2">
+        <v>67</v>
+      </c>
+      <c r="C71" s="25"/>
+      <c r="D71" s="26"/>
+      <c r="E71" s="26"/>
+      <c r="F71" s="26"/>
+      <c r="G71" s="26"/>
+      <c r="H71" s="26"/>
+      <c r="I71" s="26"/>
+      <c r="J71" s="27"/>
+      <c r="K71" s="2"/>
+    </row>
+    <row r="72" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B72" s="2">
+        <v>68</v>
+      </c>
+      <c r="C72" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="D72" s="23"/>
+      <c r="E72" s="23"/>
+      <c r="F72" s="23"/>
+      <c r="G72" s="23"/>
+      <c r="H72" s="23"/>
+      <c r="I72" s="23"/>
+      <c r="J72" s="24"/>
+      <c r="K72" s="2"/>
+    </row>
+    <row r="73" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B73" s="2">
+        <v>69</v>
+      </c>
+      <c r="C73" s="25"/>
+      <c r="D73" s="26"/>
+      <c r="E73" s="26"/>
+      <c r="F73" s="26"/>
+      <c r="G73" s="26"/>
+      <c r="H73" s="26"/>
+      <c r="I73" s="26"/>
+      <c r="J73" s="27"/>
+      <c r="K73" s="2"/>
+    </row>
+    <row r="74" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B74" s="2">
+        <v>70</v>
+      </c>
+      <c r="C74" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="D74" s="23"/>
+      <c r="E74" s="23"/>
+      <c r="F74" s="23"/>
+      <c r="G74" s="23"/>
+      <c r="H74" s="23"/>
+      <c r="I74" s="23"/>
+      <c r="J74" s="24"/>
+      <c r="K74" s="2"/>
+    </row>
+    <row r="75" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B75" s="2">
+        <v>71</v>
+      </c>
+      <c r="C75" s="25"/>
+      <c r="D75" s="26"/>
+      <c r="E75" s="26"/>
+      <c r="F75" s="26"/>
+      <c r="G75" s="26"/>
+      <c r="H75" s="26"/>
+      <c r="I75" s="26"/>
+      <c r="J75" s="27"/>
+      <c r="K75" s="2"/>
+    </row>
+    <row r="76" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B76" s="2">
+        <v>72</v>
+      </c>
+      <c r="C76" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="D76" s="23"/>
+      <c r="E76" s="23"/>
+      <c r="F76" s="23"/>
+      <c r="G76" s="23"/>
+      <c r="H76" s="23"/>
+      <c r="I76" s="23"/>
+      <c r="J76" s="24"/>
+      <c r="K76" s="2"/>
+    </row>
+    <row r="77" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B77" s="2">
+        <v>73</v>
+      </c>
+      <c r="C77" s="25"/>
+      <c r="D77" s="26"/>
+      <c r="E77" s="26"/>
+      <c r="F77" s="26"/>
+      <c r="G77" s="26"/>
+      <c r="H77" s="26"/>
+      <c r="I77" s="26"/>
+      <c r="J77" s="27"/>
+      <c r="K77" s="2"/>
+    </row>
+    <row r="78" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B78" s="2">
+        <v>74</v>
+      </c>
+      <c r="C78" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="D78" s="23"/>
+      <c r="E78" s="23"/>
+      <c r="F78" s="23"/>
+      <c r="G78" s="23"/>
+      <c r="H78" s="23"/>
+      <c r="I78" s="23"/>
+      <c r="J78" s="24"/>
+      <c r="K78" s="2"/>
+    </row>
+    <row r="79" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B79" s="2">
+        <v>75</v>
+      </c>
+      <c r="C79" s="25"/>
+      <c r="D79" s="26"/>
+      <c r="E79" s="26"/>
+      <c r="F79" s="26"/>
+      <c r="G79" s="26"/>
+      <c r="H79" s="26"/>
+      <c r="I79" s="26"/>
+      <c r="J79" s="27"/>
+      <c r="K79" s="2"/>
+    </row>
+    <row r="80" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B80" s="2">
+        <v>76</v>
+      </c>
+      <c r="C80" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="D80" s="23"/>
+      <c r="E80" s="23"/>
+      <c r="F80" s="23"/>
+      <c r="G80" s="23"/>
+      <c r="H80" s="23"/>
+      <c r="I80" s="23"/>
+      <c r="J80" s="24"/>
+      <c r="K80" s="2"/>
+    </row>
+    <row r="81" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B81" s="2">
+        <v>77</v>
+      </c>
+      <c r="C81" s="25"/>
+      <c r="D81" s="26"/>
+      <c r="E81" s="26"/>
+      <c r="F81" s="26"/>
+      <c r="G81" s="26"/>
+      <c r="H81" s="26"/>
+      <c r="I81" s="26"/>
+      <c r="J81" s="27"/>
+      <c r="K81" s="2"/>
+    </row>
+    <row r="82" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B82" s="2">
+        <v>78</v>
+      </c>
+      <c r="C82" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="D82" s="23"/>
+      <c r="E82" s="23"/>
+      <c r="F82" s="23"/>
+      <c r="G82" s="23"/>
+      <c r="H82" s="23"/>
+      <c r="I82" s="23"/>
+      <c r="J82" s="24"/>
+      <c r="K82" s="2"/>
+    </row>
+    <row r="83" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B83" s="2">
+        <v>79</v>
+      </c>
+      <c r="C83" s="25"/>
+      <c r="D83" s="26"/>
+      <c r="E83" s="26"/>
+      <c r="F83" s="26"/>
+      <c r="G83" s="26"/>
+      <c r="H83" s="26"/>
+      <c r="I83" s="26"/>
+      <c r="J83" s="27"/>
+      <c r="K83" s="2"/>
+    </row>
+    <row r="84" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B84" s="2">
+        <v>80</v>
+      </c>
+      <c r="C84" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="D84" s="23"/>
+      <c r="E84" s="23"/>
+      <c r="F84" s="23"/>
+      <c r="G84" s="23"/>
+      <c r="H84" s="23"/>
+      <c r="I84" s="23"/>
+      <c r="J84" s="24"/>
+      <c r="K84" s="2"/>
+    </row>
+    <row r="85" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B85" s="2">
+        <v>81</v>
+      </c>
+      <c r="C85" s="25"/>
+      <c r="D85" s="26"/>
+      <c r="E85" s="26"/>
+      <c r="F85" s="26"/>
+      <c r="G85" s="26"/>
+      <c r="H85" s="26"/>
+      <c r="I85" s="26"/>
+      <c r="J85" s="27"/>
+      <c r="K85" s="2"/>
+    </row>
+    <row r="86" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B86" s="2">
+        <v>82</v>
+      </c>
+      <c r="C86" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="D86" s="23"/>
+      <c r="E86" s="23"/>
+      <c r="F86" s="23"/>
+      <c r="G86" s="23"/>
+      <c r="H86" s="23"/>
+      <c r="I86" s="23"/>
+      <c r="J86" s="24"/>
+      <c r="K86" s="2"/>
+    </row>
+    <row r="87" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B87" s="2">
+        <v>83</v>
+      </c>
+      <c r="C87" s="25"/>
+      <c r="D87" s="26"/>
+      <c r="E87" s="26"/>
+      <c r="F87" s="26"/>
+      <c r="G87" s="26"/>
+      <c r="H87" s="26"/>
+      <c r="I87" s="26"/>
+      <c r="J87" s="27"/>
+      <c r="K87" s="2"/>
+    </row>
+    <row r="88" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B88" s="2">
+        <v>84</v>
+      </c>
+      <c r="C88" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="D88" s="23"/>
+      <c r="E88" s="23"/>
+      <c r="F88" s="23"/>
+      <c r="G88" s="23"/>
+      <c r="H88" s="23"/>
+      <c r="I88" s="23"/>
+      <c r="J88" s="24"/>
+      <c r="K88" s="2"/>
+    </row>
+    <row r="89" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B89" s="2">
+        <v>85</v>
+      </c>
+      <c r="C89" s="25"/>
+      <c r="D89" s="26"/>
+      <c r="E89" s="26"/>
+      <c r="F89" s="26"/>
+      <c r="G89" s="26"/>
+      <c r="H89" s="26"/>
+      <c r="I89" s="26"/>
+      <c r="J89" s="27"/>
+      <c r="K89" s="2"/>
+    </row>
+    <row r="90" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B90" s="2">
+        <v>86</v>
+      </c>
+      <c r="C90" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="D90" s="23"/>
+      <c r="E90" s="23"/>
+      <c r="F90" s="23"/>
+      <c r="G90" s="23"/>
+      <c r="H90" s="23"/>
+      <c r="I90" s="23"/>
+      <c r="J90" s="24"/>
+      <c r="K90" s="2"/>
+    </row>
+    <row r="91" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B91" s="2">
+        <v>87</v>
+      </c>
+      <c r="C91" s="25"/>
+      <c r="D91" s="26"/>
+      <c r="E91" s="26"/>
+      <c r="F91" s="26"/>
+      <c r="G91" s="26"/>
+      <c r="H91" s="26"/>
+      <c r="I91" s="26"/>
+      <c r="J91" s="27"/>
+      <c r="K91" s="2"/>
+    </row>
+    <row r="92" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B92" s="2">
+        <v>88</v>
+      </c>
+      <c r="C92" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="D92" s="23"/>
+      <c r="E92" s="23"/>
+      <c r="F92" s="23"/>
+      <c r="G92" s="23"/>
+      <c r="H92" s="23"/>
+      <c r="I92" s="23"/>
+      <c r="J92" s="24"/>
+      <c r="K92" s="2"/>
+    </row>
+    <row r="93" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B93" s="2">
+        <v>89</v>
+      </c>
+      <c r="C93" s="25"/>
+      <c r="D93" s="26"/>
+      <c r="E93" s="26"/>
+      <c r="F93" s="26"/>
+      <c r="G93" s="26"/>
+      <c r="H93" s="26"/>
+      <c r="I93" s="26"/>
+      <c r="J93" s="27"/>
+      <c r="K93" s="2"/>
+    </row>
+    <row r="94" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B94" s="2">
+        <v>90</v>
+      </c>
+      <c r="C94" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="D94" s="23"/>
+      <c r="E94" s="23"/>
+      <c r="F94" s="23"/>
+      <c r="G94" s="23"/>
+      <c r="H94" s="23"/>
+      <c r="I94" s="23"/>
+      <c r="J94" s="24"/>
+      <c r="K94" s="2"/>
+    </row>
+    <row r="95" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B95" s="2">
+        <v>91</v>
+      </c>
+      <c r="C95" s="25"/>
+      <c r="D95" s="26"/>
+      <c r="E95" s="26"/>
+      <c r="F95" s="26"/>
+      <c r="G95" s="26"/>
+      <c r="H95" s="26"/>
+      <c r="I95" s="26"/>
+      <c r="J95" s="27"/>
+      <c r="K95" s="2"/>
+    </row>
+    <row r="96" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B96" s="2">
+        <v>92</v>
+      </c>
+      <c r="C96" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="D96" s="23"/>
+      <c r="E96" s="23"/>
+      <c r="F96" s="23"/>
+      <c r="G96" s="23"/>
+      <c r="H96" s="23"/>
+      <c r="I96" s="23"/>
+      <c r="J96" s="24"/>
+      <c r="K96" s="2"/>
+    </row>
+    <row r="97" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B97" s="2">
+        <v>93</v>
+      </c>
+      <c r="C97" s="25"/>
+      <c r="D97" s="26"/>
+      <c r="E97" s="26"/>
+      <c r="F97" s="26"/>
+      <c r="G97" s="26"/>
+      <c r="H97" s="26"/>
+      <c r="I97" s="26"/>
+      <c r="J97" s="27"/>
+      <c r="K97" s="2"/>
+    </row>
+    <row r="98" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B98" s="2">
+        <v>94</v>
+      </c>
+      <c r="C98" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="D98" s="23"/>
+      <c r="E98" s="23"/>
+      <c r="F98" s="23"/>
+      <c r="G98" s="23"/>
+      <c r="H98" s="23"/>
+      <c r="I98" s="23"/>
+      <c r="J98" s="24"/>
+      <c r="K98" s="2"/>
+    </row>
+    <row r="99" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B99" s="2">
+        <v>95</v>
+      </c>
+      <c r="C99" s="25"/>
+      <c r="D99" s="26"/>
+      <c r="E99" s="26"/>
+      <c r="F99" s="26"/>
+      <c r="G99" s="26"/>
+      <c r="H99" s="26"/>
+      <c r="I99" s="26"/>
+      <c r="J99" s="27"/>
+      <c r="K99" s="2"/>
+    </row>
+    <row r="100" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B100" s="2">
+        <v>96</v>
+      </c>
+      <c r="C100" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="D100" s="23"/>
+      <c r="E100" s="23"/>
+      <c r="F100" s="23"/>
+      <c r="G100" s="23"/>
+      <c r="H100" s="23"/>
+      <c r="I100" s="23"/>
+      <c r="J100" s="24"/>
+      <c r="K100" s="2"/>
+    </row>
+    <row r="101" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B101" s="2">
+        <v>97</v>
+      </c>
+      <c r="C101" s="25"/>
+      <c r="D101" s="26"/>
+      <c r="E101" s="26"/>
+      <c r="F101" s="26"/>
+      <c r="G101" s="26"/>
+      <c r="H101" s="26"/>
+      <c r="I101" s="26"/>
+      <c r="J101" s="27"/>
+      <c r="K101" s="2"/>
+    </row>
+    <row r="102" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B102" s="2">
+        <v>98</v>
+      </c>
+      <c r="C102" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="D102" s="23"/>
+      <c r="E102" s="23"/>
+      <c r="F102" s="23"/>
+      <c r="G102" s="23"/>
+      <c r="H102" s="23"/>
+      <c r="I102" s="23"/>
+      <c r="J102" s="24"/>
+      <c r="K102" s="2"/>
+    </row>
+    <row r="103" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B103" s="2">
+        <v>99</v>
+      </c>
+      <c r="C103" s="25"/>
+      <c r="D103" s="26"/>
+      <c r="E103" s="26"/>
+      <c r="F103" s="26"/>
+      <c r="G103" s="26"/>
+      <c r="H103" s="26"/>
+      <c r="I103" s="26"/>
+      <c r="J103" s="27"/>
+      <c r="K103" s="2"/>
+    </row>
+    <row r="104" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B104" s="2">
+        <v>100</v>
+      </c>
+      <c r="C104" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="D104" s="23"/>
+      <c r="E104" s="23"/>
+      <c r="F104" s="23"/>
+      <c r="G104" s="23"/>
+      <c r="H104" s="23"/>
+      <c r="I104" s="23"/>
+      <c r="J104" s="24"/>
+      <c r="K104" s="2"/>
+    </row>
+    <row r="105" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B105" s="2">
+        <v>101</v>
+      </c>
+      <c r="C105" s="25"/>
+      <c r="D105" s="26"/>
+      <c r="E105" s="26"/>
+      <c r="F105" s="26"/>
+      <c r="G105" s="26"/>
+      <c r="H105" s="26"/>
+      <c r="I105" s="26"/>
+      <c r="J105" s="27"/>
+      <c r="K105" s="2"/>
+    </row>
+    <row r="106" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B106" s="2">
+        <v>102</v>
+      </c>
+      <c r="C106" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="D106" s="23"/>
+      <c r="E106" s="23"/>
+      <c r="F106" s="23"/>
+      <c r="G106" s="23"/>
+      <c r="H106" s="23"/>
+      <c r="I106" s="23"/>
+      <c r="J106" s="24"/>
+      <c r="K106" s="2"/>
+    </row>
+    <row r="107" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B107" s="2">
+        <v>103</v>
+      </c>
+      <c r="C107" s="25"/>
+      <c r="D107" s="26"/>
+      <c r="E107" s="26"/>
+      <c r="F107" s="26"/>
+      <c r="G107" s="26"/>
+      <c r="H107" s="26"/>
+      <c r="I107" s="26"/>
+      <c r="J107" s="27"/>
+      <c r="K107" s="2"/>
+    </row>
+    <row r="108" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B108" s="2">
+        <v>104</v>
+      </c>
+      <c r="C108" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="D108" s="23"/>
+      <c r="E108" s="23"/>
+      <c r="F108" s="23"/>
+      <c r="G108" s="23"/>
+      <c r="H108" s="23"/>
+      <c r="I108" s="23"/>
+      <c r="J108" s="24"/>
+      <c r="K108" s="2"/>
+    </row>
+    <row r="109" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B109" s="2">
+        <v>105</v>
+      </c>
+      <c r="C109" s="25"/>
+      <c r="D109" s="26"/>
+      <c r="E109" s="26"/>
+      <c r="F109" s="26"/>
+      <c r="G109" s="26"/>
+      <c r="H109" s="26"/>
+      <c r="I109" s="26"/>
+      <c r="J109" s="27"/>
+      <c r="K109" s="2"/>
+    </row>
+    <row r="110" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B110" s="2">
+        <v>106</v>
+      </c>
+      <c r="C110" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="D110" s="23"/>
+      <c r="E110" s="23"/>
+      <c r="F110" s="23"/>
+      <c r="G110" s="23"/>
+      <c r="H110" s="23"/>
+      <c r="I110" s="23"/>
+      <c r="J110" s="24"/>
+      <c r="K110" s="2"/>
+    </row>
+    <row r="111" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B111" s="2">
+        <v>107</v>
+      </c>
+      <c r="C111" s="25"/>
+      <c r="D111" s="26"/>
+      <c r="E111" s="26"/>
+      <c r="F111" s="26"/>
+      <c r="G111" s="26"/>
+      <c r="H111" s="26"/>
+      <c r="I111" s="26"/>
+      <c r="J111" s="27"/>
+      <c r="K111" s="2"/>
+    </row>
+    <row r="112" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B112" s="2">
+        <v>108</v>
+      </c>
+      <c r="C112" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="D112" s="23"/>
+      <c r="E112" s="23"/>
+      <c r="F112" s="23"/>
+      <c r="G112" s="23"/>
+      <c r="H112" s="23"/>
+      <c r="I112" s="23"/>
+      <c r="J112" s="24"/>
+      <c r="K112" s="2"/>
+    </row>
+    <row r="113" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B113" s="2">
+        <v>109</v>
+      </c>
+      <c r="C113" s="25"/>
+      <c r="D113" s="26"/>
+      <c r="E113" s="26"/>
+      <c r="F113" s="26"/>
+      <c r="G113" s="26"/>
+      <c r="H113" s="26"/>
+      <c r="I113" s="26"/>
+      <c r="J113" s="27"/>
+      <c r="K113" s="2"/>
+    </row>
+    <row r="114" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B114" s="2">
+        <v>110</v>
+      </c>
+      <c r="C114" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="D114" s="23"/>
+      <c r="E114" s="23"/>
+      <c r="F114" s="23"/>
+      <c r="G114" s="23"/>
+      <c r="H114" s="23"/>
+      <c r="I114" s="23"/>
+      <c r="J114" s="24"/>
+      <c r="K114" s="2"/>
+    </row>
+    <row r="115" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B115" s="2">
+        <v>111</v>
+      </c>
+      <c r="C115" s="25"/>
+      <c r="D115" s="26"/>
+      <c r="E115" s="26"/>
+      <c r="F115" s="26"/>
+      <c r="G115" s="26"/>
+      <c r="H115" s="26"/>
+      <c r="I115" s="26"/>
+      <c r="J115" s="27"/>
+      <c r="K115" s="2"/>
+    </row>
+    <row r="116" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B116" s="2">
+        <v>112</v>
+      </c>
+      <c r="C116" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="D116" s="23"/>
+      <c r="E116" s="23"/>
+      <c r="F116" s="23"/>
+      <c r="G116" s="23"/>
+      <c r="H116" s="23"/>
+      <c r="I116" s="23"/>
+      <c r="J116" s="24"/>
+      <c r="K116" s="2"/>
+    </row>
+    <row r="117" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B117" s="2">
+        <v>113</v>
+      </c>
+      <c r="C117" s="25"/>
+      <c r="D117" s="26"/>
+      <c r="E117" s="26"/>
+      <c r="F117" s="26"/>
+      <c r="G117" s="26"/>
+      <c r="H117" s="26"/>
+      <c r="I117" s="26"/>
+      <c r="J117" s="27"/>
+      <c r="K117" s="2"/>
+    </row>
+    <row r="118" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B118" s="2">
+        <v>114</v>
+      </c>
+      <c r="C118" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="D118" s="23"/>
+      <c r="E118" s="23"/>
+      <c r="F118" s="23"/>
+      <c r="G118" s="23"/>
+      <c r="H118" s="23"/>
+      <c r="I118" s="23"/>
+      <c r="J118" s="24"/>
+      <c r="K118" s="2"/>
+    </row>
+    <row r="119" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B119" s="2">
+        <v>115</v>
+      </c>
+      <c r="C119" s="25"/>
+      <c r="D119" s="26"/>
+      <c r="E119" s="26"/>
+      <c r="F119" s="26"/>
+      <c r="G119" s="26"/>
+      <c r="H119" s="26"/>
+      <c r="I119" s="26"/>
+      <c r="J119" s="27"/>
+      <c r="K119" s="2"/>
+    </row>
+    <row r="120" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B120" s="2">
+        <v>116</v>
+      </c>
+      <c r="C120" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="D120" s="23"/>
+      <c r="E120" s="23"/>
+      <c r="F120" s="23"/>
+      <c r="G120" s="23"/>
+      <c r="H120" s="23"/>
+      <c r="I120" s="23"/>
+      <c r="J120" s="24"/>
+      <c r="K120" s="2"/>
+    </row>
+    <row r="121" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B121" s="2">
+        <v>117</v>
+      </c>
+      <c r="C121" s="25"/>
+      <c r="D121" s="26"/>
+      <c r="E121" s="26"/>
+      <c r="F121" s="26"/>
+      <c r="G121" s="26"/>
+      <c r="H121" s="26"/>
+      <c r="I121" s="26"/>
+      <c r="J121" s="27"/>
+      <c r="K121" s="2"/>
+    </row>
+    <row r="122" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B122" s="2">
+        <v>118</v>
+      </c>
+      <c r="C122" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="D122" s="23"/>
+      <c r="E122" s="23"/>
+      <c r="F122" s="23"/>
+      <c r="G122" s="23"/>
+      <c r="H122" s="23"/>
+      <c r="I122" s="23"/>
+      <c r="J122" s="24"/>
+      <c r="K122" s="2"/>
+    </row>
+    <row r="123" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B123" s="2">
+        <v>119</v>
+      </c>
+      <c r="C123" s="25"/>
+      <c r="D123" s="26"/>
+      <c r="E123" s="26"/>
+      <c r="F123" s="26"/>
+      <c r="G123" s="26"/>
+      <c r="H123" s="26"/>
+      <c r="I123" s="26"/>
+      <c r="J123" s="27"/>
+      <c r="K123" s="2"/>
+    </row>
+    <row r="124" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B124" s="2">
+        <v>120</v>
+      </c>
+      <c r="C124" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="D124" s="23"/>
+      <c r="E124" s="23"/>
+      <c r="F124" s="23"/>
+      <c r="G124" s="23"/>
+      <c r="H124" s="23"/>
+      <c r="I124" s="23"/>
+      <c r="J124" s="24"/>
+      <c r="K124" s="2"/>
+    </row>
+    <row r="125" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B125" s="2">
+        <v>121</v>
+      </c>
+      <c r="C125" s="25"/>
+      <c r="D125" s="26"/>
+      <c r="E125" s="26"/>
+      <c r="F125" s="26"/>
+      <c r="G125" s="26"/>
+      <c r="H125" s="26"/>
+      <c r="I125" s="26"/>
+      <c r="J125" s="27"/>
+      <c r="K125" s="2"/>
+    </row>
+    <row r="126" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B126" s="2">
+        <v>122</v>
+      </c>
+      <c r="C126" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="D126" s="23"/>
+      <c r="E126" s="23"/>
+      <c r="F126" s="23"/>
+      <c r="G126" s="23"/>
+      <c r="H126" s="23"/>
+      <c r="I126" s="23"/>
+      <c r="J126" s="24"/>
+      <c r="K126" s="2"/>
+    </row>
+    <row r="127" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B127" s="2">
+        <v>123</v>
+      </c>
+      <c r="C127" s="25"/>
+      <c r="D127" s="26"/>
+      <c r="E127" s="26"/>
+      <c r="F127" s="26"/>
+      <c r="G127" s="26"/>
+      <c r="H127" s="26"/>
+      <c r="I127" s="26"/>
+      <c r="J127" s="27"/>
+      <c r="K127" s="2"/>
+    </row>
+    <row r="128" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B128" s="2">
+        <v>124</v>
+      </c>
+      <c r="C128" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="D128" s="23"/>
+      <c r="E128" s="23"/>
+      <c r="F128" s="23"/>
+      <c r="G128" s="23"/>
+      <c r="H128" s="23"/>
+      <c r="I128" s="23"/>
+      <c r="J128" s="24"/>
+      <c r="K128" s="2"/>
+    </row>
+    <row r="129" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B129" s="2">
+        <v>125</v>
+      </c>
+      <c r="C129" s="25"/>
+      <c r="D129" s="26"/>
+      <c r="E129" s="26"/>
+      <c r="F129" s="26"/>
+      <c r="G129" s="26"/>
+      <c r="H129" s="26"/>
+      <c r="I129" s="26"/>
+      <c r="J129" s="27"/>
+      <c r="K129" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="67">
+    <mergeCell ref="C128:J129"/>
+    <mergeCell ref="C116:J117"/>
+    <mergeCell ref="C118:J119"/>
+    <mergeCell ref="C120:J121"/>
+    <mergeCell ref="C122:J123"/>
+    <mergeCell ref="C124:J125"/>
+    <mergeCell ref="C126:J127"/>
+    <mergeCell ref="C104:J105"/>
+    <mergeCell ref="C106:J107"/>
+    <mergeCell ref="C108:J109"/>
+    <mergeCell ref="C110:J111"/>
+    <mergeCell ref="C112:J113"/>
+    <mergeCell ref="C114:J115"/>
+    <mergeCell ref="C92:J93"/>
+    <mergeCell ref="C94:J95"/>
+    <mergeCell ref="C96:J97"/>
+    <mergeCell ref="C98:J99"/>
+    <mergeCell ref="C100:J101"/>
+    <mergeCell ref="C102:J103"/>
+    <mergeCell ref="C80:J81"/>
+    <mergeCell ref="C82:J83"/>
+    <mergeCell ref="C84:J85"/>
+    <mergeCell ref="C86:J87"/>
+    <mergeCell ref="C88:J89"/>
+    <mergeCell ref="C90:J91"/>
+    <mergeCell ref="C68:J69"/>
+    <mergeCell ref="C70:J71"/>
+    <mergeCell ref="C72:J73"/>
+    <mergeCell ref="C74:J75"/>
+    <mergeCell ref="C76:J77"/>
+    <mergeCell ref="C78:J79"/>
+    <mergeCell ref="C56:J57"/>
+    <mergeCell ref="C58:J59"/>
+    <mergeCell ref="C60:J61"/>
+    <mergeCell ref="C62:J63"/>
+    <mergeCell ref="C64:J65"/>
+    <mergeCell ref="C66:J67"/>
+    <mergeCell ref="C44:J45"/>
+    <mergeCell ref="C46:J47"/>
+    <mergeCell ref="C48:J49"/>
+    <mergeCell ref="C50:J51"/>
+    <mergeCell ref="C52:J53"/>
+    <mergeCell ref="C54:J55"/>
+    <mergeCell ref="C32:J33"/>
+    <mergeCell ref="C34:J35"/>
+    <mergeCell ref="C36:J37"/>
+    <mergeCell ref="C38:J39"/>
+    <mergeCell ref="C40:J41"/>
+    <mergeCell ref="C42:J43"/>
+    <mergeCell ref="C20:J21"/>
+    <mergeCell ref="C22:J23"/>
+    <mergeCell ref="C24:J25"/>
+    <mergeCell ref="C26:J27"/>
+    <mergeCell ref="C28:J29"/>
+    <mergeCell ref="C30:J31"/>
+    <mergeCell ref="C8:J9"/>
+    <mergeCell ref="C10:J11"/>
+    <mergeCell ref="C12:J13"/>
+    <mergeCell ref="C14:J15"/>
+    <mergeCell ref="C16:J17"/>
+    <mergeCell ref="C18:J19"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="R2:T2"/>
+    <mergeCell ref="C4:J4"/>
+    <mergeCell ref="C5:J6"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="C7:J7"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[Add] Sign Up Routine
- Sign Up Routine Test Complete with T_Simulator.
- Mod : Protocol : Sign Up
</commit_message>
<xml_diff>
--- a/T_Design.xlsx
+++ b/T_Design.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wave\010_Project\010_Game\Tetris\Server\010_Source\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wave\010_Project\010_Game\Tetris\Tetris_Server\020_SourceCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{217C42DC-C76D-47B8-8995-AFE8979CD0FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE537D43-36A8-4B38-9E6C-77775397E430}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{CBDAA684-FC25-4649-B038-1CECF5D4149C}"/>
   </bookViews>
@@ -24,12 +24,20 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="109">
   <si>
     <t>Byte</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -385,10 +393,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Message Size (126 BYTE)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Message Type (0x01 : Sign Up)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -406,6 +410,22 @@
   </si>
   <si>
     <t>Result (0x00 : OK, 0x01 : USER ID Already Exists, 0x02 : ETC Error)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User ID Text Size</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User Name Text Size</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User PW Text Size</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Message Size (129 BYTE)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -604,7 +624,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -671,6 +691,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -689,13 +718,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2340,7 +2363,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>
@@ -2418,7 +2441,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D7" s="18"/>
       <c r="E7" s="18"/>
@@ -2457,16 +2480,16 @@
       <c r="B8" s="2">
         <v>4</v>
       </c>
-      <c r="C8" s="28" t="s">
-        <v>105</v>
-      </c>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="29"/>
-      <c r="I8" s="29"/>
-      <c r="J8" s="30"/>
+      <c r="C8" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="24"/>
       <c r="K8" s="2"/>
       <c r="N8" s="2" t="str">
         <f>IF(ISBLANK(Type!C8),"",Type!C8)</f>
@@ -2921,6 +2944,7 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2929,10 +2953,10 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="B2:T129"/>
+  <dimension ref="B2:T132"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22:J23"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="K128" sqref="K128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3024,7 +3048,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
@@ -3066,7 +3090,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>
@@ -3144,7 +3168,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D7" s="18"/>
       <c r="E7" s="18"/>
@@ -3183,16 +3207,16 @@
       <c r="B8" s="2">
         <v>4</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="24"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="27"/>
       <c r="K8" s="2"/>
       <c r="N8" s="2" t="str">
         <f>IF(ISBLANK(Type!C8),"",Type!C8)</f>
@@ -3223,14 +3247,14 @@
       <c r="B9" s="2">
         <v>5</v>
       </c>
-      <c r="C9" s="25"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="26"/>
-      <c r="J9" s="27"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="30"/>
       <c r="K9" s="2"/>
       <c r="N9" s="2" t="str">
         <f>IF(ISBLANK(Type!C9),"",Type!C9)</f>
@@ -3261,16 +3285,16 @@
       <c r="B10" s="2">
         <v>6</v>
       </c>
-      <c r="C10" s="22" t="s">
+      <c r="C10" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="23"/>
-      <c r="J10" s="24"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="26"/>
+      <c r="J10" s="27"/>
       <c r="K10" s="2"/>
       <c r="N10" s="2" t="str">
         <f>IF(ISBLANK(Type!C10),"",Type!C10)</f>
@@ -3301,14 +3325,14 @@
       <c r="B11" s="2">
         <v>7</v>
       </c>
-      <c r="C11" s="25"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="26"/>
-      <c r="J11" s="27"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="29"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="30"/>
       <c r="K11" s="2"/>
       <c r="N11" s="2" t="str">
         <f>IF(ISBLANK(Type!C11),"",Type!C11)</f>
@@ -3339,16 +3363,16 @@
       <c r="B12" s="2">
         <v>8</v>
       </c>
-      <c r="C12" s="22" t="s">
+      <c r="C12" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
-      <c r="I12" s="23"/>
-      <c r="J12" s="24"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="26"/>
+      <c r="J12" s="27"/>
       <c r="K12" s="2"/>
       <c r="N12" s="2" t="str">
         <f>IF(ISBLANK(Type!C12),"",Type!C12)</f>
@@ -3379,14 +3403,14 @@
       <c r="B13" s="2">
         <v>9</v>
       </c>
-      <c r="C13" s="25"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="27"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="30"/>
       <c r="K13" s="2"/>
       <c r="N13" s="2" t="str">
         <f>IF(ISBLANK(Type!C13),"",Type!C13)</f>
@@ -3417,16 +3441,16 @@
       <c r="B14" s="2">
         <v>10</v>
       </c>
-      <c r="C14" s="22" t="s">
+      <c r="C14" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="23"/>
-      <c r="I14" s="23"/>
-      <c r="J14" s="24"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="27"/>
       <c r="K14" s="2"/>
       <c r="N14" s="2" t="str">
         <f>IF(ISBLANK(Type!C14),"",Type!C14)</f>
@@ -3457,14 +3481,14 @@
       <c r="B15" s="2">
         <v>11</v>
       </c>
-      <c r="C15" s="25"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="27"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="30"/>
       <c r="K15" s="2"/>
       <c r="N15" s="2" t="str">
         <f>IF(ISBLANK(Type!C15),"",Type!C15)</f>
@@ -3495,16 +3519,16 @@
       <c r="B16" s="2">
         <v>12</v>
       </c>
-      <c r="C16" s="22" t="s">
+      <c r="C16" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="23"/>
-      <c r="I16" s="23"/>
-      <c r="J16" s="24"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="27"/>
       <c r="K16" s="2"/>
       <c r="N16" s="2" t="str">
         <f>IF(ISBLANK(Type!C16),"",Type!C16)</f>
@@ -3535,14 +3559,14 @@
       <c r="B17" s="2">
         <v>13</v>
       </c>
-      <c r="C17" s="25"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="27"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="30"/>
       <c r="K17" s="2"/>
       <c r="N17" s="2" t="str">
         <f>IF(ISBLANK(Type!C17),"",Type!C17)</f>
@@ -3573,16 +3597,16 @@
       <c r="B18" s="2">
         <v>14</v>
       </c>
-      <c r="C18" s="22" t="s">
+      <c r="C18" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="23"/>
-      <c r="H18" s="23"/>
-      <c r="I18" s="23"/>
-      <c r="J18" s="24"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="27"/>
       <c r="K18" s="2"/>
       <c r="N18" s="2" t="str">
         <f>IF(ISBLANK(Type!C18),"",Type!C18)</f>
@@ -3613,14 +3637,14 @@
       <c r="B19" s="2">
         <v>15</v>
       </c>
-      <c r="C19" s="25"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="26"/>
-      <c r="J19" s="27"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="29"/>
+      <c r="J19" s="30"/>
       <c r="K19" s="2"/>
       <c r="N19" s="2" t="str">
         <f>IF(ISBLANK(Type!C19),"",Type!C19)</f>
@@ -3651,16 +3675,16 @@
       <c r="B20" s="2">
         <v>16</v>
       </c>
-      <c r="C20" s="22" t="s">
+      <c r="C20" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="23"/>
-      <c r="H20" s="23"/>
-      <c r="I20" s="23"/>
-      <c r="J20" s="24"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="26"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="27"/>
       <c r="K20" s="2"/>
       <c r="N20" s="2" t="str">
         <f>IF(ISBLANK(Type!C20),"",Type!C20)</f>
@@ -3691,14 +3715,14 @@
       <c r="B21" s="2">
         <v>17</v>
       </c>
-      <c r="C21" s="25"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="26"/>
-      <c r="G21" s="26"/>
-      <c r="H21" s="26"/>
-      <c r="I21" s="26"/>
-      <c r="J21" s="27"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="29"/>
+      <c r="I21" s="29"/>
+      <c r="J21" s="30"/>
       <c r="K21" s="2"/>
       <c r="N21" s="2" t="str">
         <f>IF(ISBLANK(Type!C21),"",Type!C21)</f>
@@ -3729,16 +3753,16 @@
       <c r="B22" s="2">
         <v>18</v>
       </c>
-      <c r="C22" s="22" t="s">
+      <c r="C22" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="D22" s="23"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="23"/>
-      <c r="G22" s="23"/>
-      <c r="H22" s="23"/>
-      <c r="I22" s="23"/>
-      <c r="J22" s="24"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="26"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="26"/>
+      <c r="J22" s="27"/>
       <c r="K22" s="2"/>
       <c r="N22" s="2" t="str">
         <f>IF(ISBLANK(Type!C22),"",Type!C22)</f>
@@ -3769,14 +3793,14 @@
       <c r="B23" s="2">
         <v>19</v>
       </c>
-      <c r="C23" s="25"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="26"/>
-      <c r="H23" s="26"/>
-      <c r="I23" s="26"/>
-      <c r="J23" s="27"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="29"/>
+      <c r="I23" s="29"/>
+      <c r="J23" s="30"/>
       <c r="K23" s="2"/>
       <c r="N23" s="2" t="str">
         <f>IF(ISBLANK(Type!C23),"",Type!C23)</f>
@@ -3807,16 +3831,16 @@
       <c r="B24" s="2">
         <v>20</v>
       </c>
-      <c r="C24" s="22" t="s">
+      <c r="C24" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="D24" s="23"/>
-      <c r="E24" s="23"/>
-      <c r="F24" s="23"/>
-      <c r="G24" s="23"/>
-      <c r="H24" s="23"/>
-      <c r="I24" s="23"/>
-      <c r="J24" s="24"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="26"/>
+      <c r="J24" s="27"/>
       <c r="K24" s="2"/>
       <c r="N24" s="2" t="str">
         <f>IF(ISBLANK(Type!C24),"",Type!C24)</f>
@@ -3847,1578 +3871,1689 @@
       <c r="B25" s="2">
         <v>21</v>
       </c>
-      <c r="C25" s="25"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="26"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="26"/>
-      <c r="H25" s="26"/>
-      <c r="I25" s="26"/>
-      <c r="J25" s="27"/>
+      <c r="C25" s="28"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="29"/>
+      <c r="I25" s="29"/>
+      <c r="J25" s="30"/>
       <c r="K25" s="2"/>
     </row>
     <row r="26" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B26" s="2">
         <v>22</v>
       </c>
-      <c r="C26" s="22" t="s">
+      <c r="C26" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="D26" s="23"/>
-      <c r="E26" s="23"/>
-      <c r="F26" s="23"/>
-      <c r="G26" s="23"/>
-      <c r="H26" s="23"/>
-      <c r="I26" s="23"/>
-      <c r="J26" s="24"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="26"/>
+      <c r="G26" s="26"/>
+      <c r="H26" s="26"/>
+      <c r="I26" s="26"/>
+      <c r="J26" s="27"/>
       <c r="K26" s="2"/>
     </row>
     <row r="27" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B27" s="2">
         <v>23</v>
       </c>
-      <c r="C27" s="25"/>
-      <c r="D27" s="26"/>
-      <c r="E27" s="26"/>
-      <c r="F27" s="26"/>
-      <c r="G27" s="26"/>
-      <c r="H27" s="26"/>
-      <c r="I27" s="26"/>
-      <c r="J27" s="27"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="29"/>
+      <c r="I27" s="29"/>
+      <c r="J27" s="30"/>
       <c r="K27" s="2"/>
     </row>
     <row r="28" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B28" s="2">
         <v>24</v>
       </c>
-      <c r="C28" s="22" t="s">
+      <c r="C28" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="D28" s="23"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="23"/>
-      <c r="H28" s="23"/>
-      <c r="I28" s="23"/>
-      <c r="J28" s="24"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="26"/>
+      <c r="H28" s="26"/>
+      <c r="I28" s="26"/>
+      <c r="J28" s="27"/>
       <c r="K28" s="2"/>
     </row>
     <row r="29" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B29" s="2">
         <v>25</v>
       </c>
-      <c r="C29" s="25"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="27"/>
+      <c r="C29" s="28"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="29"/>
+      <c r="I29" s="29"/>
+      <c r="J29" s="30"/>
       <c r="K29" s="2"/>
     </row>
     <row r="30" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B30" s="2">
         <v>26</v>
       </c>
-      <c r="C30" s="22" t="s">
+      <c r="C30" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="D30" s="23"/>
-      <c r="E30" s="23"/>
-      <c r="F30" s="23"/>
-      <c r="G30" s="23"/>
-      <c r="H30" s="23"/>
-      <c r="I30" s="23"/>
-      <c r="J30" s="24"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="27"/>
       <c r="K30" s="2"/>
     </row>
     <row r="31" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B31" s="2">
         <v>27</v>
       </c>
-      <c r="C31" s="25"/>
-      <c r="D31" s="26"/>
-      <c r="E31" s="26"/>
-      <c r="F31" s="26"/>
-      <c r="G31" s="26"/>
-      <c r="H31" s="26"/>
-      <c r="I31" s="26"/>
-      <c r="J31" s="27"/>
+      <c r="C31" s="28"/>
+      <c r="D31" s="29"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="29"/>
+      <c r="I31" s="29"/>
+      <c r="J31" s="30"/>
       <c r="K31" s="2"/>
     </row>
     <row r="32" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B32" s="2">
         <v>28</v>
       </c>
-      <c r="C32" s="22" t="s">
+      <c r="C32" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="D32" s="23"/>
-      <c r="E32" s="23"/>
-      <c r="F32" s="23"/>
-      <c r="G32" s="23"/>
-      <c r="H32" s="23"/>
-      <c r="I32" s="23"/>
-      <c r="J32" s="24"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="26"/>
+      <c r="F32" s="26"/>
+      <c r="G32" s="26"/>
+      <c r="H32" s="26"/>
+      <c r="I32" s="26"/>
+      <c r="J32" s="27"/>
       <c r="K32" s="2"/>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B33" s="2">
         <v>29</v>
       </c>
-      <c r="C33" s="25"/>
-      <c r="D33" s="26"/>
-      <c r="E33" s="26"/>
-      <c r="F33" s="26"/>
-      <c r="G33" s="26"/>
-      <c r="H33" s="26"/>
-      <c r="I33" s="26"/>
-      <c r="J33" s="27"/>
+      <c r="C33" s="28"/>
+      <c r="D33" s="29"/>
+      <c r="E33" s="29"/>
+      <c r="F33" s="29"/>
+      <c r="G33" s="29"/>
+      <c r="H33" s="29"/>
+      <c r="I33" s="29"/>
+      <c r="J33" s="30"/>
       <c r="K33" s="2"/>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B34" s="2">
         <v>30</v>
       </c>
-      <c r="C34" s="22" t="s">
+      <c r="C34" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="D34" s="23"/>
-      <c r="E34" s="23"/>
-      <c r="F34" s="23"/>
-      <c r="G34" s="23"/>
-      <c r="H34" s="23"/>
-      <c r="I34" s="23"/>
-      <c r="J34" s="24"/>
+      <c r="D34" s="26"/>
+      <c r="E34" s="26"/>
+      <c r="F34" s="26"/>
+      <c r="G34" s="26"/>
+      <c r="H34" s="26"/>
+      <c r="I34" s="26"/>
+      <c r="J34" s="27"/>
       <c r="K34" s="2"/>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B35" s="2">
         <v>31</v>
       </c>
-      <c r="C35" s="25"/>
-      <c r="D35" s="26"/>
-      <c r="E35" s="26"/>
-      <c r="F35" s="26"/>
-      <c r="G35" s="26"/>
-      <c r="H35" s="26"/>
-      <c r="I35" s="26"/>
-      <c r="J35" s="27"/>
+      <c r="C35" s="28"/>
+      <c r="D35" s="29"/>
+      <c r="E35" s="29"/>
+      <c r="F35" s="29"/>
+      <c r="G35" s="29"/>
+      <c r="H35" s="29"/>
+      <c r="I35" s="29"/>
+      <c r="J35" s="30"/>
       <c r="K35" s="2"/>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B36" s="2">
         <v>32</v>
       </c>
-      <c r="C36" s="22" t="s">
+      <c r="C36" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="D36" s="23"/>
-      <c r="E36" s="23"/>
-      <c r="F36" s="23"/>
-      <c r="G36" s="23"/>
-      <c r="H36" s="23"/>
-      <c r="I36" s="23"/>
-      <c r="J36" s="24"/>
+      <c r="D36" s="26"/>
+      <c r="E36" s="26"/>
+      <c r="F36" s="26"/>
+      <c r="G36" s="26"/>
+      <c r="H36" s="26"/>
+      <c r="I36" s="26"/>
+      <c r="J36" s="27"/>
       <c r="K36" s="2"/>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B37" s="2">
         <v>33</v>
       </c>
-      <c r="C37" s="25"/>
-      <c r="D37" s="26"/>
-      <c r="E37" s="26"/>
-      <c r="F37" s="26"/>
-      <c r="G37" s="26"/>
-      <c r="H37" s="26"/>
-      <c r="I37" s="26"/>
-      <c r="J37" s="27"/>
+      <c r="C37" s="28"/>
+      <c r="D37" s="29"/>
+      <c r="E37" s="29"/>
+      <c r="F37" s="29"/>
+      <c r="G37" s="29"/>
+      <c r="H37" s="29"/>
+      <c r="I37" s="29"/>
+      <c r="J37" s="30"/>
       <c r="K37" s="2"/>
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B38" s="2">
         <v>34</v>
       </c>
-      <c r="C38" s="22" t="s">
+      <c r="C38" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="D38" s="23"/>
-      <c r="E38" s="23"/>
-      <c r="F38" s="23"/>
-      <c r="G38" s="23"/>
-      <c r="H38" s="23"/>
-      <c r="I38" s="23"/>
-      <c r="J38" s="24"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="26"/>
+      <c r="F38" s="26"/>
+      <c r="G38" s="26"/>
+      <c r="H38" s="26"/>
+      <c r="I38" s="26"/>
+      <c r="J38" s="27"/>
       <c r="K38" s="2"/>
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B39" s="2">
         <v>35</v>
       </c>
-      <c r="C39" s="25"/>
-      <c r="D39" s="26"/>
-      <c r="E39" s="26"/>
-      <c r="F39" s="26"/>
-      <c r="G39" s="26"/>
-      <c r="H39" s="26"/>
-      <c r="I39" s="26"/>
-      <c r="J39" s="27"/>
+      <c r="C39" s="28"/>
+      <c r="D39" s="29"/>
+      <c r="E39" s="29"/>
+      <c r="F39" s="29"/>
+      <c r="G39" s="29"/>
+      <c r="H39" s="29"/>
+      <c r="I39" s="29"/>
+      <c r="J39" s="30"/>
       <c r="K39" s="2"/>
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B40" s="2">
         <v>36</v>
       </c>
-      <c r="C40" s="22" t="s">
+      <c r="C40" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="D40" s="23"/>
-      <c r="E40" s="23"/>
-      <c r="F40" s="23"/>
-      <c r="G40" s="23"/>
-      <c r="H40" s="23"/>
-      <c r="I40" s="23"/>
-      <c r="J40" s="24"/>
+      <c r="D40" s="26"/>
+      <c r="E40" s="26"/>
+      <c r="F40" s="26"/>
+      <c r="G40" s="26"/>
+      <c r="H40" s="26"/>
+      <c r="I40" s="26"/>
+      <c r="J40" s="27"/>
       <c r="K40" s="2"/>
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B41" s="2">
         <v>37</v>
       </c>
-      <c r="C41" s="25"/>
-      <c r="D41" s="26"/>
-      <c r="E41" s="26"/>
-      <c r="F41" s="26"/>
-      <c r="G41" s="26"/>
-      <c r="H41" s="26"/>
-      <c r="I41" s="26"/>
-      <c r="J41" s="27"/>
+      <c r="C41" s="28"/>
+      <c r="D41" s="29"/>
+      <c r="E41" s="29"/>
+      <c r="F41" s="29"/>
+      <c r="G41" s="29"/>
+      <c r="H41" s="29"/>
+      <c r="I41" s="29"/>
+      <c r="J41" s="30"/>
       <c r="K41" s="2"/>
     </row>
     <row r="42" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B42" s="2">
         <v>38</v>
       </c>
-      <c r="C42" s="22" t="s">
+      <c r="C42" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="D42" s="23"/>
-      <c r="E42" s="23"/>
-      <c r="F42" s="23"/>
-      <c r="G42" s="23"/>
-      <c r="H42" s="23"/>
-      <c r="I42" s="23"/>
-      <c r="J42" s="24"/>
+      <c r="D42" s="26"/>
+      <c r="E42" s="26"/>
+      <c r="F42" s="26"/>
+      <c r="G42" s="26"/>
+      <c r="H42" s="26"/>
+      <c r="I42" s="26"/>
+      <c r="J42" s="27"/>
       <c r="K42" s="2"/>
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B43" s="2">
         <v>39</v>
       </c>
-      <c r="C43" s="25"/>
-      <c r="D43" s="26"/>
-      <c r="E43" s="26"/>
-      <c r="F43" s="26"/>
-      <c r="G43" s="26"/>
-      <c r="H43" s="26"/>
-      <c r="I43" s="26"/>
-      <c r="J43" s="27"/>
+      <c r="C43" s="28"/>
+      <c r="D43" s="29"/>
+      <c r="E43" s="29"/>
+      <c r="F43" s="29"/>
+      <c r="G43" s="29"/>
+      <c r="H43" s="29"/>
+      <c r="I43" s="29"/>
+      <c r="J43" s="30"/>
       <c r="K43" s="2"/>
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B44" s="2">
         <v>40</v>
       </c>
-      <c r="C44" s="22" t="s">
+      <c r="C44" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="D44" s="23"/>
-      <c r="E44" s="23"/>
-      <c r="F44" s="23"/>
-      <c r="G44" s="23"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="24"/>
+      <c r="D44" s="26"/>
+      <c r="E44" s="26"/>
+      <c r="F44" s="26"/>
+      <c r="G44" s="26"/>
+      <c r="H44" s="26"/>
+      <c r="I44" s="26"/>
+      <c r="J44" s="27"/>
       <c r="K44" s="2"/>
     </row>
     <row r="45" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B45" s="2">
         <v>41</v>
       </c>
-      <c r="C45" s="25"/>
-      <c r="D45" s="26"/>
-      <c r="E45" s="26"/>
-      <c r="F45" s="26"/>
-      <c r="G45" s="26"/>
-      <c r="H45" s="26"/>
-      <c r="I45" s="26"/>
-      <c r="J45" s="27"/>
+      <c r="C45" s="28"/>
+      <c r="D45" s="29"/>
+      <c r="E45" s="29"/>
+      <c r="F45" s="29"/>
+      <c r="G45" s="29"/>
+      <c r="H45" s="29"/>
+      <c r="I45" s="29"/>
+      <c r="J45" s="30"/>
       <c r="K45" s="2"/>
     </row>
     <row r="46" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B46" s="2">
         <v>42</v>
       </c>
-      <c r="C46" s="22" t="s">
+      <c r="C46" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="D46" s="23"/>
-      <c r="E46" s="23"/>
-      <c r="F46" s="23"/>
-      <c r="G46" s="23"/>
-      <c r="H46" s="23"/>
-      <c r="I46" s="23"/>
-      <c r="J46" s="24"/>
+      <c r="D46" s="26"/>
+      <c r="E46" s="26"/>
+      <c r="F46" s="26"/>
+      <c r="G46" s="26"/>
+      <c r="H46" s="26"/>
+      <c r="I46" s="26"/>
+      <c r="J46" s="27"/>
       <c r="K46" s="2"/>
     </row>
     <row r="47" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B47" s="2">
         <v>43</v>
       </c>
-      <c r="C47" s="25"/>
-      <c r="D47" s="26"/>
-      <c r="E47" s="26"/>
-      <c r="F47" s="26"/>
-      <c r="G47" s="26"/>
-      <c r="H47" s="26"/>
-      <c r="I47" s="26"/>
-      <c r="J47" s="27"/>
+      <c r="C47" s="28"/>
+      <c r="D47" s="29"/>
+      <c r="E47" s="29"/>
+      <c r="F47" s="29"/>
+      <c r="G47" s="29"/>
+      <c r="H47" s="29"/>
+      <c r="I47" s="29"/>
+      <c r="J47" s="30"/>
       <c r="K47" s="2"/>
     </row>
     <row r="48" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B48" s="2">
         <v>44</v>
       </c>
-      <c r="C48" s="22" t="s">
+      <c r="C48" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="D48" s="23"/>
-      <c r="E48" s="23"/>
-      <c r="F48" s="23"/>
-      <c r="G48" s="23"/>
-      <c r="H48" s="23"/>
-      <c r="I48" s="23"/>
-      <c r="J48" s="24"/>
+      <c r="D48" s="26"/>
+      <c r="E48" s="26"/>
+      <c r="F48" s="26"/>
+      <c r="G48" s="26"/>
+      <c r="H48" s="26"/>
+      <c r="I48" s="26"/>
+      <c r="J48" s="27"/>
       <c r="K48" s="2"/>
     </row>
     <row r="49" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B49" s="2">
         <v>45</v>
       </c>
-      <c r="C49" s="25"/>
-      <c r="D49" s="26"/>
-      <c r="E49" s="26"/>
-      <c r="F49" s="26"/>
-      <c r="G49" s="26"/>
-      <c r="H49" s="26"/>
-      <c r="I49" s="26"/>
-      <c r="J49" s="27"/>
+      <c r="C49" s="28"/>
+      <c r="D49" s="29"/>
+      <c r="E49" s="29"/>
+      <c r="F49" s="29"/>
+      <c r="G49" s="29"/>
+      <c r="H49" s="29"/>
+      <c r="I49" s="29"/>
+      <c r="J49" s="30"/>
       <c r="K49" s="2"/>
     </row>
     <row r="50" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B50" s="2">
         <v>46</v>
       </c>
-      <c r="C50" s="22" t="s">
+      <c r="C50" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="D50" s="23"/>
-      <c r="E50" s="23"/>
-      <c r="F50" s="23"/>
-      <c r="G50" s="23"/>
-      <c r="H50" s="23"/>
-      <c r="I50" s="23"/>
-      <c r="J50" s="24"/>
+      <c r="D50" s="26"/>
+      <c r="E50" s="26"/>
+      <c r="F50" s="26"/>
+      <c r="G50" s="26"/>
+      <c r="H50" s="26"/>
+      <c r="I50" s="26"/>
+      <c r="J50" s="27"/>
       <c r="K50" s="2"/>
     </row>
     <row r="51" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B51" s="2">
         <v>47</v>
       </c>
-      <c r="C51" s="25"/>
-      <c r="D51" s="26"/>
-      <c r="E51" s="26"/>
-      <c r="F51" s="26"/>
-      <c r="G51" s="26"/>
-      <c r="H51" s="26"/>
-      <c r="I51" s="26"/>
-      <c r="J51" s="27"/>
+      <c r="C51" s="28"/>
+      <c r="D51" s="29"/>
+      <c r="E51" s="29"/>
+      <c r="F51" s="29"/>
+      <c r="G51" s="29"/>
+      <c r="H51" s="29"/>
+      <c r="I51" s="29"/>
+      <c r="J51" s="30"/>
       <c r="K51" s="2"/>
     </row>
     <row r="52" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B52" s="2">
         <v>48</v>
       </c>
-      <c r="C52" s="22" t="s">
+      <c r="C52" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="D52" s="23"/>
-      <c r="E52" s="23"/>
-      <c r="F52" s="23"/>
-      <c r="G52" s="23"/>
-      <c r="H52" s="23"/>
-      <c r="I52" s="23"/>
-      <c r="J52" s="24"/>
+      <c r="D52" s="26"/>
+      <c r="E52" s="26"/>
+      <c r="F52" s="26"/>
+      <c r="G52" s="26"/>
+      <c r="H52" s="26"/>
+      <c r="I52" s="26"/>
+      <c r="J52" s="27"/>
       <c r="K52" s="2"/>
     </row>
     <row r="53" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B53" s="2">
         <v>49</v>
       </c>
-      <c r="C53" s="25"/>
-      <c r="D53" s="26"/>
-      <c r="E53" s="26"/>
-      <c r="F53" s="26"/>
-      <c r="G53" s="26"/>
-      <c r="H53" s="26"/>
-      <c r="I53" s="26"/>
-      <c r="J53" s="27"/>
+      <c r="C53" s="28"/>
+      <c r="D53" s="29"/>
+      <c r="E53" s="29"/>
+      <c r="F53" s="29"/>
+      <c r="G53" s="29"/>
+      <c r="H53" s="29"/>
+      <c r="I53" s="29"/>
+      <c r="J53" s="30"/>
       <c r="K53" s="2"/>
     </row>
     <row r="54" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B54" s="2">
         <v>50</v>
       </c>
-      <c r="C54" s="22" t="s">
+      <c r="C54" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="D54" s="23"/>
-      <c r="E54" s="23"/>
-      <c r="F54" s="23"/>
-      <c r="G54" s="23"/>
-      <c r="H54" s="23"/>
-      <c r="I54" s="23"/>
-      <c r="J54" s="24"/>
+      <c r="D54" s="26"/>
+      <c r="E54" s="26"/>
+      <c r="F54" s="26"/>
+      <c r="G54" s="26"/>
+      <c r="H54" s="26"/>
+      <c r="I54" s="26"/>
+      <c r="J54" s="27"/>
       <c r="K54" s="2"/>
     </row>
     <row r="55" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B55" s="2">
         <v>51</v>
       </c>
-      <c r="C55" s="25"/>
-      <c r="D55" s="26"/>
-      <c r="E55" s="26"/>
-      <c r="F55" s="26"/>
-      <c r="G55" s="26"/>
-      <c r="H55" s="26"/>
-      <c r="I55" s="26"/>
-      <c r="J55" s="27"/>
+      <c r="C55" s="28"/>
+      <c r="D55" s="29"/>
+      <c r="E55" s="29"/>
+      <c r="F55" s="29"/>
+      <c r="G55" s="29"/>
+      <c r="H55" s="29"/>
+      <c r="I55" s="29"/>
+      <c r="J55" s="30"/>
       <c r="K55" s="2"/>
     </row>
     <row r="56" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B56" s="2">
         <v>52</v>
       </c>
-      <c r="C56" s="22" t="s">
+      <c r="C56" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="D56" s="23"/>
-      <c r="E56" s="23"/>
-      <c r="F56" s="23"/>
-      <c r="G56" s="23"/>
-      <c r="H56" s="23"/>
-      <c r="I56" s="23"/>
-      <c r="J56" s="24"/>
+      <c r="D56" s="26"/>
+      <c r="E56" s="26"/>
+      <c r="F56" s="26"/>
+      <c r="G56" s="26"/>
+      <c r="H56" s="26"/>
+      <c r="I56" s="26"/>
+      <c r="J56" s="27"/>
       <c r="K56" s="2"/>
     </row>
     <row r="57" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B57" s="2">
         <v>53</v>
       </c>
-      <c r="C57" s="25"/>
-      <c r="D57" s="26"/>
-      <c r="E57" s="26"/>
-      <c r="F57" s="26"/>
-      <c r="G57" s="26"/>
-      <c r="H57" s="26"/>
-      <c r="I57" s="26"/>
-      <c r="J57" s="27"/>
+      <c r="C57" s="28"/>
+      <c r="D57" s="29"/>
+      <c r="E57" s="29"/>
+      <c r="F57" s="29"/>
+      <c r="G57" s="29"/>
+      <c r="H57" s="29"/>
+      <c r="I57" s="29"/>
+      <c r="J57" s="30"/>
       <c r="K57" s="2"/>
     </row>
     <row r="58" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B58" s="2">
         <v>54</v>
       </c>
-      <c r="C58" s="22" t="s">
+      <c r="C58" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="D58" s="23"/>
-      <c r="E58" s="23"/>
-      <c r="F58" s="23"/>
-      <c r="G58" s="23"/>
-      <c r="H58" s="23"/>
-      <c r="I58" s="23"/>
-      <c r="J58" s="24"/>
+      <c r="D58" s="26"/>
+      <c r="E58" s="26"/>
+      <c r="F58" s="26"/>
+      <c r="G58" s="26"/>
+      <c r="H58" s="26"/>
+      <c r="I58" s="26"/>
+      <c r="J58" s="27"/>
       <c r="K58" s="2"/>
     </row>
     <row r="59" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B59" s="2">
         <v>55</v>
       </c>
-      <c r="C59" s="25"/>
-      <c r="D59" s="26"/>
-      <c r="E59" s="26"/>
-      <c r="F59" s="26"/>
-      <c r="G59" s="26"/>
-      <c r="H59" s="26"/>
-      <c r="I59" s="26"/>
-      <c r="J59" s="27"/>
+      <c r="C59" s="28"/>
+      <c r="D59" s="29"/>
+      <c r="E59" s="29"/>
+      <c r="F59" s="29"/>
+      <c r="G59" s="29"/>
+      <c r="H59" s="29"/>
+      <c r="I59" s="29"/>
+      <c r="J59" s="30"/>
       <c r="K59" s="2"/>
     </row>
     <row r="60" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B60" s="2">
         <v>56</v>
       </c>
-      <c r="C60" s="22" t="s">
+      <c r="C60" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="D60" s="23"/>
-      <c r="E60" s="23"/>
-      <c r="F60" s="23"/>
-      <c r="G60" s="23"/>
-      <c r="H60" s="23"/>
-      <c r="I60" s="23"/>
-      <c r="J60" s="24"/>
+      <c r="D60" s="26"/>
+      <c r="E60" s="26"/>
+      <c r="F60" s="26"/>
+      <c r="G60" s="26"/>
+      <c r="H60" s="26"/>
+      <c r="I60" s="26"/>
+      <c r="J60" s="27"/>
       <c r="K60" s="2"/>
     </row>
     <row r="61" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B61" s="2">
         <v>57</v>
       </c>
-      <c r="C61" s="25"/>
-      <c r="D61" s="26"/>
-      <c r="E61" s="26"/>
-      <c r="F61" s="26"/>
-      <c r="G61" s="26"/>
-      <c r="H61" s="26"/>
-      <c r="I61" s="26"/>
-      <c r="J61" s="27"/>
+      <c r="C61" s="28"/>
+      <c r="D61" s="29"/>
+      <c r="E61" s="29"/>
+      <c r="F61" s="29"/>
+      <c r="G61" s="29"/>
+      <c r="H61" s="29"/>
+      <c r="I61" s="29"/>
+      <c r="J61" s="30"/>
       <c r="K61" s="2"/>
     </row>
     <row r="62" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B62" s="2">
         <v>58</v>
       </c>
-      <c r="C62" s="22" t="s">
+      <c r="C62" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="D62" s="23"/>
-      <c r="E62" s="23"/>
-      <c r="F62" s="23"/>
-      <c r="G62" s="23"/>
-      <c r="H62" s="23"/>
-      <c r="I62" s="23"/>
-      <c r="J62" s="24"/>
+      <c r="D62" s="26"/>
+      <c r="E62" s="26"/>
+      <c r="F62" s="26"/>
+      <c r="G62" s="26"/>
+      <c r="H62" s="26"/>
+      <c r="I62" s="26"/>
+      <c r="J62" s="27"/>
       <c r="K62" s="2"/>
     </row>
     <row r="63" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B63" s="2">
         <v>59</v>
       </c>
-      <c r="C63" s="25"/>
-      <c r="D63" s="26"/>
-      <c r="E63" s="26"/>
-      <c r="F63" s="26"/>
-      <c r="G63" s="26"/>
-      <c r="H63" s="26"/>
-      <c r="I63" s="26"/>
-      <c r="J63" s="27"/>
+      <c r="C63" s="28"/>
+      <c r="D63" s="29"/>
+      <c r="E63" s="29"/>
+      <c r="F63" s="29"/>
+      <c r="G63" s="29"/>
+      <c r="H63" s="29"/>
+      <c r="I63" s="29"/>
+      <c r="J63" s="30"/>
       <c r="K63" s="2"/>
     </row>
     <row r="64" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B64" s="2">
         <v>60</v>
       </c>
-      <c r="C64" s="22" t="s">
+      <c r="C64" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="D64" s="23"/>
-      <c r="E64" s="23"/>
-      <c r="F64" s="23"/>
-      <c r="G64" s="23"/>
-      <c r="H64" s="23"/>
-      <c r="I64" s="23"/>
-      <c r="J64" s="24"/>
+      <c r="D64" s="26"/>
+      <c r="E64" s="26"/>
+      <c r="F64" s="26"/>
+      <c r="G64" s="26"/>
+      <c r="H64" s="26"/>
+      <c r="I64" s="26"/>
+      <c r="J64" s="27"/>
       <c r="K64" s="2"/>
     </row>
     <row r="65" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B65" s="2">
         <v>61</v>
       </c>
-      <c r="C65" s="25"/>
-      <c r="D65" s="26"/>
-      <c r="E65" s="26"/>
-      <c r="F65" s="26"/>
-      <c r="G65" s="26"/>
-      <c r="H65" s="26"/>
-      <c r="I65" s="26"/>
-      <c r="J65" s="27"/>
+      <c r="C65" s="28"/>
+      <c r="D65" s="29"/>
+      <c r="E65" s="29"/>
+      <c r="F65" s="29"/>
+      <c r="G65" s="29"/>
+      <c r="H65" s="29"/>
+      <c r="I65" s="29"/>
+      <c r="J65" s="30"/>
       <c r="K65" s="2"/>
     </row>
     <row r="66" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B66" s="2">
         <v>62</v>
       </c>
-      <c r="C66" s="22" t="s">
+      <c r="C66" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="D66" s="23"/>
-      <c r="E66" s="23"/>
-      <c r="F66" s="23"/>
-      <c r="G66" s="23"/>
-      <c r="H66" s="23"/>
-      <c r="I66" s="23"/>
-      <c r="J66" s="24"/>
+      <c r="D66" s="26"/>
+      <c r="E66" s="26"/>
+      <c r="F66" s="26"/>
+      <c r="G66" s="26"/>
+      <c r="H66" s="26"/>
+      <c r="I66" s="26"/>
+      <c r="J66" s="27"/>
       <c r="K66" s="2"/>
     </row>
     <row r="67" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B67" s="2">
         <v>63</v>
       </c>
-      <c r="C67" s="25"/>
-      <c r="D67" s="26"/>
-      <c r="E67" s="26"/>
-      <c r="F67" s="26"/>
-      <c r="G67" s="26"/>
-      <c r="H67" s="26"/>
-      <c r="I67" s="26"/>
-      <c r="J67" s="27"/>
+      <c r="C67" s="28"/>
+      <c r="D67" s="29"/>
+      <c r="E67" s="29"/>
+      <c r="F67" s="29"/>
+      <c r="G67" s="29"/>
+      <c r="H67" s="29"/>
+      <c r="I67" s="29"/>
+      <c r="J67" s="30"/>
       <c r="K67" s="2"/>
     </row>
     <row r="68" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B68" s="2">
         <v>64</v>
       </c>
-      <c r="C68" s="22" t="s">
+      <c r="C68" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="D68" s="23"/>
-      <c r="E68" s="23"/>
-      <c r="F68" s="23"/>
-      <c r="G68" s="23"/>
-      <c r="H68" s="23"/>
-      <c r="I68" s="23"/>
-      <c r="J68" s="24"/>
+      <c r="D68" s="26"/>
+      <c r="E68" s="26"/>
+      <c r="F68" s="26"/>
+      <c r="G68" s="26"/>
+      <c r="H68" s="26"/>
+      <c r="I68" s="26"/>
+      <c r="J68" s="27"/>
       <c r="K68" s="2"/>
     </row>
     <row r="69" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B69" s="2">
         <v>65</v>
       </c>
-      <c r="C69" s="25"/>
-      <c r="D69" s="26"/>
-      <c r="E69" s="26"/>
-      <c r="F69" s="26"/>
-      <c r="G69" s="26"/>
-      <c r="H69" s="26"/>
-      <c r="I69" s="26"/>
-      <c r="J69" s="27"/>
+      <c r="C69" s="28"/>
+      <c r="D69" s="29"/>
+      <c r="E69" s="29"/>
+      <c r="F69" s="29"/>
+      <c r="G69" s="29"/>
+      <c r="H69" s="29"/>
+      <c r="I69" s="29"/>
+      <c r="J69" s="30"/>
       <c r="K69" s="2"/>
     </row>
     <row r="70" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B70" s="2">
         <v>66</v>
       </c>
-      <c r="C70" s="22" t="s">
+      <c r="C70" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="D70" s="23"/>
-      <c r="E70" s="23"/>
-      <c r="F70" s="23"/>
-      <c r="G70" s="23"/>
-      <c r="H70" s="23"/>
-      <c r="I70" s="23"/>
-      <c r="J70" s="24"/>
+      <c r="D70" s="26"/>
+      <c r="E70" s="26"/>
+      <c r="F70" s="26"/>
+      <c r="G70" s="26"/>
+      <c r="H70" s="26"/>
+      <c r="I70" s="26"/>
+      <c r="J70" s="27"/>
       <c r="K70" s="2"/>
     </row>
     <row r="71" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B71" s="2">
         <v>67</v>
       </c>
-      <c r="C71" s="25"/>
-      <c r="D71" s="26"/>
-      <c r="E71" s="26"/>
-      <c r="F71" s="26"/>
-      <c r="G71" s="26"/>
-      <c r="H71" s="26"/>
-      <c r="I71" s="26"/>
-      <c r="J71" s="27"/>
+      <c r="C71" s="28"/>
+      <c r="D71" s="29"/>
+      <c r="E71" s="29"/>
+      <c r="F71" s="29"/>
+      <c r="G71" s="29"/>
+      <c r="H71" s="29"/>
+      <c r="I71" s="29"/>
+      <c r="J71" s="30"/>
       <c r="K71" s="2"/>
     </row>
     <row r="72" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B72" s="2">
         <v>68</v>
       </c>
-      <c r="C72" s="22" t="s">
+      <c r="C72" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="D72" s="23"/>
-      <c r="E72" s="23"/>
-      <c r="F72" s="23"/>
-      <c r="G72" s="23"/>
-      <c r="H72" s="23"/>
-      <c r="I72" s="23"/>
-      <c r="J72" s="24"/>
+      <c r="D72" s="26"/>
+      <c r="E72" s="26"/>
+      <c r="F72" s="26"/>
+      <c r="G72" s="26"/>
+      <c r="H72" s="26"/>
+      <c r="I72" s="26"/>
+      <c r="J72" s="27"/>
       <c r="K72" s="2"/>
     </row>
     <row r="73" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B73" s="2">
         <v>69</v>
       </c>
-      <c r="C73" s="25"/>
-      <c r="D73" s="26"/>
-      <c r="E73" s="26"/>
-      <c r="F73" s="26"/>
-      <c r="G73" s="26"/>
-      <c r="H73" s="26"/>
-      <c r="I73" s="26"/>
-      <c r="J73" s="27"/>
+      <c r="C73" s="28"/>
+      <c r="D73" s="29"/>
+      <c r="E73" s="29"/>
+      <c r="F73" s="29"/>
+      <c r="G73" s="29"/>
+      <c r="H73" s="29"/>
+      <c r="I73" s="29"/>
+      <c r="J73" s="30"/>
       <c r="K73" s="2"/>
     </row>
     <row r="74" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B74" s="2">
         <v>70</v>
       </c>
-      <c r="C74" s="22" t="s">
+      <c r="C74" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="D74" s="23"/>
-      <c r="E74" s="23"/>
-      <c r="F74" s="23"/>
-      <c r="G74" s="23"/>
-      <c r="H74" s="23"/>
-      <c r="I74" s="23"/>
-      <c r="J74" s="24"/>
+      <c r="D74" s="26"/>
+      <c r="E74" s="26"/>
+      <c r="F74" s="26"/>
+      <c r="G74" s="26"/>
+      <c r="H74" s="26"/>
+      <c r="I74" s="26"/>
+      <c r="J74" s="27"/>
       <c r="K74" s="2"/>
     </row>
     <row r="75" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B75" s="2">
         <v>71</v>
       </c>
-      <c r="C75" s="25"/>
-      <c r="D75" s="26"/>
-      <c r="E75" s="26"/>
-      <c r="F75" s="26"/>
-      <c r="G75" s="26"/>
-      <c r="H75" s="26"/>
-      <c r="I75" s="26"/>
-      <c r="J75" s="27"/>
+      <c r="C75" s="28"/>
+      <c r="D75" s="29"/>
+      <c r="E75" s="29"/>
+      <c r="F75" s="29"/>
+      <c r="G75" s="29"/>
+      <c r="H75" s="29"/>
+      <c r="I75" s="29"/>
+      <c r="J75" s="30"/>
       <c r="K75" s="2"/>
     </row>
     <row r="76" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B76" s="2">
         <v>72</v>
       </c>
-      <c r="C76" s="22" t="s">
+      <c r="C76" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="D76" s="23"/>
-      <c r="E76" s="23"/>
-      <c r="F76" s="23"/>
-      <c r="G76" s="23"/>
-      <c r="H76" s="23"/>
-      <c r="I76" s="23"/>
-      <c r="J76" s="24"/>
+      <c r="D76" s="26"/>
+      <c r="E76" s="26"/>
+      <c r="F76" s="26"/>
+      <c r="G76" s="26"/>
+      <c r="H76" s="26"/>
+      <c r="I76" s="26"/>
+      <c r="J76" s="27"/>
       <c r="K76" s="2"/>
     </row>
     <row r="77" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B77" s="2">
         <v>73</v>
       </c>
-      <c r="C77" s="25"/>
-      <c r="D77" s="26"/>
-      <c r="E77" s="26"/>
-      <c r="F77" s="26"/>
-      <c r="G77" s="26"/>
-      <c r="H77" s="26"/>
-      <c r="I77" s="26"/>
-      <c r="J77" s="27"/>
+      <c r="C77" s="28"/>
+      <c r="D77" s="29"/>
+      <c r="E77" s="29"/>
+      <c r="F77" s="29"/>
+      <c r="G77" s="29"/>
+      <c r="H77" s="29"/>
+      <c r="I77" s="29"/>
+      <c r="J77" s="30"/>
       <c r="K77" s="2"/>
     </row>
     <row r="78" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B78" s="2">
         <v>74</v>
       </c>
-      <c r="C78" s="22" t="s">
+      <c r="C78" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="D78" s="23"/>
-      <c r="E78" s="23"/>
-      <c r="F78" s="23"/>
-      <c r="G78" s="23"/>
-      <c r="H78" s="23"/>
-      <c r="I78" s="23"/>
-      <c r="J78" s="24"/>
+      <c r="D78" s="26"/>
+      <c r="E78" s="26"/>
+      <c r="F78" s="26"/>
+      <c r="G78" s="26"/>
+      <c r="H78" s="26"/>
+      <c r="I78" s="26"/>
+      <c r="J78" s="27"/>
       <c r="K78" s="2"/>
     </row>
     <row r="79" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B79" s="2">
         <v>75</v>
       </c>
-      <c r="C79" s="25"/>
-      <c r="D79" s="26"/>
-      <c r="E79" s="26"/>
-      <c r="F79" s="26"/>
-      <c r="G79" s="26"/>
-      <c r="H79" s="26"/>
-      <c r="I79" s="26"/>
-      <c r="J79" s="27"/>
+      <c r="C79" s="28"/>
+      <c r="D79" s="29"/>
+      <c r="E79" s="29"/>
+      <c r="F79" s="29"/>
+      <c r="G79" s="29"/>
+      <c r="H79" s="29"/>
+      <c r="I79" s="29"/>
+      <c r="J79" s="30"/>
       <c r="K79" s="2"/>
     </row>
     <row r="80" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B80" s="2">
         <v>76</v>
       </c>
-      <c r="C80" s="22" t="s">
+      <c r="C80" s="25" t="s">
         <v>79</v>
       </c>
-      <c r="D80" s="23"/>
-      <c r="E80" s="23"/>
-      <c r="F80" s="23"/>
-      <c r="G80" s="23"/>
-      <c r="H80" s="23"/>
-      <c r="I80" s="23"/>
-      <c r="J80" s="24"/>
+      <c r="D80" s="26"/>
+      <c r="E80" s="26"/>
+      <c r="F80" s="26"/>
+      <c r="G80" s="26"/>
+      <c r="H80" s="26"/>
+      <c r="I80" s="26"/>
+      <c r="J80" s="27"/>
       <c r="K80" s="2"/>
     </row>
     <row r="81" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B81" s="2">
         <v>77</v>
       </c>
-      <c r="C81" s="25"/>
-      <c r="D81" s="26"/>
-      <c r="E81" s="26"/>
-      <c r="F81" s="26"/>
-      <c r="G81" s="26"/>
-      <c r="H81" s="26"/>
-      <c r="I81" s="26"/>
-      <c r="J81" s="27"/>
+      <c r="C81" s="28"/>
+      <c r="D81" s="29"/>
+      <c r="E81" s="29"/>
+      <c r="F81" s="29"/>
+      <c r="G81" s="29"/>
+      <c r="H81" s="29"/>
+      <c r="I81" s="29"/>
+      <c r="J81" s="30"/>
       <c r="K81" s="2"/>
     </row>
     <row r="82" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B82" s="2">
         <v>78</v>
       </c>
-      <c r="C82" s="22" t="s">
+      <c r="C82" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="D82" s="23"/>
-      <c r="E82" s="23"/>
-      <c r="F82" s="23"/>
-      <c r="G82" s="23"/>
-      <c r="H82" s="23"/>
-      <c r="I82" s="23"/>
-      <c r="J82" s="24"/>
+      <c r="D82" s="26"/>
+      <c r="E82" s="26"/>
+      <c r="F82" s="26"/>
+      <c r="G82" s="26"/>
+      <c r="H82" s="26"/>
+      <c r="I82" s="26"/>
+      <c r="J82" s="27"/>
       <c r="K82" s="2"/>
     </row>
     <row r="83" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B83" s="2">
         <v>79</v>
       </c>
-      <c r="C83" s="25"/>
-      <c r="D83" s="26"/>
-      <c r="E83" s="26"/>
-      <c r="F83" s="26"/>
-      <c r="G83" s="26"/>
-      <c r="H83" s="26"/>
-      <c r="I83" s="26"/>
-      <c r="J83" s="27"/>
+      <c r="C83" s="28"/>
+      <c r="D83" s="29"/>
+      <c r="E83" s="29"/>
+      <c r="F83" s="29"/>
+      <c r="G83" s="29"/>
+      <c r="H83" s="29"/>
+      <c r="I83" s="29"/>
+      <c r="J83" s="30"/>
       <c r="K83" s="2"/>
     </row>
     <row r="84" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B84" s="2">
         <v>80</v>
       </c>
-      <c r="C84" s="22" t="s">
+      <c r="C84" s="25" t="s">
         <v>81</v>
       </c>
-      <c r="D84" s="23"/>
-      <c r="E84" s="23"/>
-      <c r="F84" s="23"/>
-      <c r="G84" s="23"/>
-      <c r="H84" s="23"/>
-      <c r="I84" s="23"/>
-      <c r="J84" s="24"/>
+      <c r="D84" s="26"/>
+      <c r="E84" s="26"/>
+      <c r="F84" s="26"/>
+      <c r="G84" s="26"/>
+      <c r="H84" s="26"/>
+      <c r="I84" s="26"/>
+      <c r="J84" s="27"/>
       <c r="K84" s="2"/>
     </row>
     <row r="85" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B85" s="2">
         <v>81</v>
       </c>
-      <c r="C85" s="25"/>
-      <c r="D85" s="26"/>
-      <c r="E85" s="26"/>
-      <c r="F85" s="26"/>
-      <c r="G85" s="26"/>
-      <c r="H85" s="26"/>
-      <c r="I85" s="26"/>
-      <c r="J85" s="27"/>
+      <c r="C85" s="28"/>
+      <c r="D85" s="29"/>
+      <c r="E85" s="29"/>
+      <c r="F85" s="29"/>
+      <c r="G85" s="29"/>
+      <c r="H85" s="29"/>
+      <c r="I85" s="29"/>
+      <c r="J85" s="30"/>
       <c r="K85" s="2"/>
     </row>
     <row r="86" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B86" s="2">
         <v>82</v>
       </c>
-      <c r="C86" s="22" t="s">
+      <c r="C86" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="D86" s="23"/>
-      <c r="E86" s="23"/>
-      <c r="F86" s="23"/>
-      <c r="G86" s="23"/>
-      <c r="H86" s="23"/>
-      <c r="I86" s="23"/>
-      <c r="J86" s="24"/>
+      <c r="D86" s="26"/>
+      <c r="E86" s="26"/>
+      <c r="F86" s="26"/>
+      <c r="G86" s="26"/>
+      <c r="H86" s="26"/>
+      <c r="I86" s="26"/>
+      <c r="J86" s="27"/>
       <c r="K86" s="2"/>
     </row>
     <row r="87" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B87" s="2">
         <v>83</v>
       </c>
-      <c r="C87" s="25"/>
-      <c r="D87" s="26"/>
-      <c r="E87" s="26"/>
-      <c r="F87" s="26"/>
-      <c r="G87" s="26"/>
-      <c r="H87" s="26"/>
-      <c r="I87" s="26"/>
-      <c r="J87" s="27"/>
+      <c r="C87" s="28"/>
+      <c r="D87" s="29"/>
+      <c r="E87" s="29"/>
+      <c r="F87" s="29"/>
+      <c r="G87" s="29"/>
+      <c r="H87" s="29"/>
+      <c r="I87" s="29"/>
+      <c r="J87" s="30"/>
       <c r="K87" s="2"/>
     </row>
     <row r="88" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B88" s="2">
         <v>84</v>
       </c>
-      <c r="C88" s="22" t="s">
+      <c r="C88" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="D88" s="23"/>
-      <c r="E88" s="23"/>
-      <c r="F88" s="23"/>
-      <c r="G88" s="23"/>
-      <c r="H88" s="23"/>
-      <c r="I88" s="23"/>
-      <c r="J88" s="24"/>
+      <c r="D88" s="26"/>
+      <c r="E88" s="26"/>
+      <c r="F88" s="26"/>
+      <c r="G88" s="26"/>
+      <c r="H88" s="26"/>
+      <c r="I88" s="26"/>
+      <c r="J88" s="27"/>
       <c r="K88" s="2"/>
     </row>
     <row r="89" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B89" s="2">
         <v>85</v>
       </c>
-      <c r="C89" s="25"/>
-      <c r="D89" s="26"/>
-      <c r="E89" s="26"/>
-      <c r="F89" s="26"/>
-      <c r="G89" s="26"/>
-      <c r="H89" s="26"/>
-      <c r="I89" s="26"/>
-      <c r="J89" s="27"/>
+      <c r="C89" s="28"/>
+      <c r="D89" s="29"/>
+      <c r="E89" s="29"/>
+      <c r="F89" s="29"/>
+      <c r="G89" s="29"/>
+      <c r="H89" s="29"/>
+      <c r="I89" s="29"/>
+      <c r="J89" s="30"/>
       <c r="K89" s="2"/>
     </row>
     <row r="90" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B90" s="2">
         <v>86</v>
       </c>
-      <c r="C90" s="22" t="s">
+      <c r="C90" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="D90" s="23"/>
-      <c r="E90" s="23"/>
-      <c r="F90" s="23"/>
-      <c r="G90" s="23"/>
-      <c r="H90" s="23"/>
-      <c r="I90" s="23"/>
-      <c r="J90" s="24"/>
+      <c r="D90" s="26"/>
+      <c r="E90" s="26"/>
+      <c r="F90" s="26"/>
+      <c r="G90" s="26"/>
+      <c r="H90" s="26"/>
+      <c r="I90" s="26"/>
+      <c r="J90" s="27"/>
       <c r="K90" s="2"/>
     </row>
     <row r="91" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B91" s="2">
         <v>87</v>
       </c>
-      <c r="C91" s="25"/>
-      <c r="D91" s="26"/>
-      <c r="E91" s="26"/>
-      <c r="F91" s="26"/>
-      <c r="G91" s="26"/>
-      <c r="H91" s="26"/>
-      <c r="I91" s="26"/>
-      <c r="J91" s="27"/>
+      <c r="C91" s="28"/>
+      <c r="D91" s="29"/>
+      <c r="E91" s="29"/>
+      <c r="F91" s="29"/>
+      <c r="G91" s="29"/>
+      <c r="H91" s="29"/>
+      <c r="I91" s="29"/>
+      <c r="J91" s="30"/>
       <c r="K91" s="2"/>
     </row>
     <row r="92" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B92" s="2">
         <v>88</v>
       </c>
-      <c r="C92" s="22" t="s">
+      <c r="C92" s="25" t="s">
         <v>83</v>
       </c>
-      <c r="D92" s="23"/>
-      <c r="E92" s="23"/>
-      <c r="F92" s="23"/>
-      <c r="G92" s="23"/>
-      <c r="H92" s="23"/>
-      <c r="I92" s="23"/>
-      <c r="J92" s="24"/>
+      <c r="D92" s="26"/>
+      <c r="E92" s="26"/>
+      <c r="F92" s="26"/>
+      <c r="G92" s="26"/>
+      <c r="H92" s="26"/>
+      <c r="I92" s="26"/>
+      <c r="J92" s="27"/>
       <c r="K92" s="2"/>
     </row>
     <row r="93" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B93" s="2">
         <v>89</v>
       </c>
-      <c r="C93" s="25"/>
-      <c r="D93" s="26"/>
-      <c r="E93" s="26"/>
-      <c r="F93" s="26"/>
-      <c r="G93" s="26"/>
-      <c r="H93" s="26"/>
-      <c r="I93" s="26"/>
-      <c r="J93" s="27"/>
+      <c r="C93" s="28"/>
+      <c r="D93" s="29"/>
+      <c r="E93" s="29"/>
+      <c r="F93" s="29"/>
+      <c r="G93" s="29"/>
+      <c r="H93" s="29"/>
+      <c r="I93" s="29"/>
+      <c r="J93" s="30"/>
       <c r="K93" s="2"/>
     </row>
     <row r="94" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B94" s="2">
         <v>90</v>
       </c>
-      <c r="C94" s="22" t="s">
+      <c r="C94" s="25" t="s">
         <v>84</v>
       </c>
-      <c r="D94" s="23"/>
-      <c r="E94" s="23"/>
-      <c r="F94" s="23"/>
-      <c r="G94" s="23"/>
-      <c r="H94" s="23"/>
-      <c r="I94" s="23"/>
-      <c r="J94" s="24"/>
+      <c r="D94" s="26"/>
+      <c r="E94" s="26"/>
+      <c r="F94" s="26"/>
+      <c r="G94" s="26"/>
+      <c r="H94" s="26"/>
+      <c r="I94" s="26"/>
+      <c r="J94" s="27"/>
       <c r="K94" s="2"/>
     </row>
     <row r="95" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B95" s="2">
         <v>91</v>
       </c>
-      <c r="C95" s="25"/>
-      <c r="D95" s="26"/>
-      <c r="E95" s="26"/>
-      <c r="F95" s="26"/>
-      <c r="G95" s="26"/>
-      <c r="H95" s="26"/>
-      <c r="I95" s="26"/>
-      <c r="J95" s="27"/>
+      <c r="C95" s="28"/>
+      <c r="D95" s="29"/>
+      <c r="E95" s="29"/>
+      <c r="F95" s="29"/>
+      <c r="G95" s="29"/>
+      <c r="H95" s="29"/>
+      <c r="I95" s="29"/>
+      <c r="J95" s="30"/>
       <c r="K95" s="2"/>
     </row>
     <row r="96" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B96" s="2">
         <v>92</v>
       </c>
-      <c r="C96" s="22" t="s">
+      <c r="C96" s="25" t="s">
         <v>85</v>
       </c>
-      <c r="D96" s="23"/>
-      <c r="E96" s="23"/>
-      <c r="F96" s="23"/>
-      <c r="G96" s="23"/>
-      <c r="H96" s="23"/>
-      <c r="I96" s="23"/>
-      <c r="J96" s="24"/>
+      <c r="D96" s="26"/>
+      <c r="E96" s="26"/>
+      <c r="F96" s="26"/>
+      <c r="G96" s="26"/>
+      <c r="H96" s="26"/>
+      <c r="I96" s="26"/>
+      <c r="J96" s="27"/>
       <c r="K96" s="2"/>
     </row>
     <row r="97" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B97" s="2">
         <v>93</v>
       </c>
-      <c r="C97" s="25"/>
-      <c r="D97" s="26"/>
-      <c r="E97" s="26"/>
-      <c r="F97" s="26"/>
-      <c r="G97" s="26"/>
-      <c r="H97" s="26"/>
-      <c r="I97" s="26"/>
-      <c r="J97" s="27"/>
+      <c r="C97" s="28"/>
+      <c r="D97" s="29"/>
+      <c r="E97" s="29"/>
+      <c r="F97" s="29"/>
+      <c r="G97" s="29"/>
+      <c r="H97" s="29"/>
+      <c r="I97" s="29"/>
+      <c r="J97" s="30"/>
       <c r="K97" s="2"/>
     </row>
     <row r="98" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B98" s="2">
         <v>94</v>
       </c>
-      <c r="C98" s="22" t="s">
+      <c r="C98" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="D98" s="23"/>
-      <c r="E98" s="23"/>
-      <c r="F98" s="23"/>
-      <c r="G98" s="23"/>
-      <c r="H98" s="23"/>
-      <c r="I98" s="23"/>
-      <c r="J98" s="24"/>
+      <c r="D98" s="26"/>
+      <c r="E98" s="26"/>
+      <c r="F98" s="26"/>
+      <c r="G98" s="26"/>
+      <c r="H98" s="26"/>
+      <c r="I98" s="26"/>
+      <c r="J98" s="27"/>
       <c r="K98" s="2"/>
     </row>
     <row r="99" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B99" s="2">
         <v>95</v>
       </c>
-      <c r="C99" s="25"/>
-      <c r="D99" s="26"/>
-      <c r="E99" s="26"/>
-      <c r="F99" s="26"/>
-      <c r="G99" s="26"/>
-      <c r="H99" s="26"/>
-      <c r="I99" s="26"/>
-      <c r="J99" s="27"/>
+      <c r="C99" s="28"/>
+      <c r="D99" s="29"/>
+      <c r="E99" s="29"/>
+      <c r="F99" s="29"/>
+      <c r="G99" s="29"/>
+      <c r="H99" s="29"/>
+      <c r="I99" s="29"/>
+      <c r="J99" s="30"/>
       <c r="K99" s="2"/>
     </row>
     <row r="100" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B100" s="2">
         <v>96</v>
       </c>
-      <c r="C100" s="22" t="s">
+      <c r="C100" s="25" t="s">
         <v>87</v>
       </c>
-      <c r="D100" s="23"/>
-      <c r="E100" s="23"/>
-      <c r="F100" s="23"/>
-      <c r="G100" s="23"/>
-      <c r="H100" s="23"/>
-      <c r="I100" s="23"/>
-      <c r="J100" s="24"/>
+      <c r="D100" s="26"/>
+      <c r="E100" s="26"/>
+      <c r="F100" s="26"/>
+      <c r="G100" s="26"/>
+      <c r="H100" s="26"/>
+      <c r="I100" s="26"/>
+      <c r="J100" s="27"/>
       <c r="K100" s="2"/>
     </row>
     <row r="101" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B101" s="2">
         <v>97</v>
       </c>
-      <c r="C101" s="25"/>
-      <c r="D101" s="26"/>
-      <c r="E101" s="26"/>
-      <c r="F101" s="26"/>
-      <c r="G101" s="26"/>
-      <c r="H101" s="26"/>
-      <c r="I101" s="26"/>
-      <c r="J101" s="27"/>
+      <c r="C101" s="28"/>
+      <c r="D101" s="29"/>
+      <c r="E101" s="29"/>
+      <c r="F101" s="29"/>
+      <c r="G101" s="29"/>
+      <c r="H101" s="29"/>
+      <c r="I101" s="29"/>
+      <c r="J101" s="30"/>
       <c r="K101" s="2"/>
     </row>
     <row r="102" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B102" s="2">
         <v>98</v>
       </c>
-      <c r="C102" s="22" t="s">
+      <c r="C102" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="D102" s="23"/>
-      <c r="E102" s="23"/>
-      <c r="F102" s="23"/>
-      <c r="G102" s="23"/>
-      <c r="H102" s="23"/>
-      <c r="I102" s="23"/>
-      <c r="J102" s="24"/>
+      <c r="D102" s="26"/>
+      <c r="E102" s="26"/>
+      <c r="F102" s="26"/>
+      <c r="G102" s="26"/>
+      <c r="H102" s="26"/>
+      <c r="I102" s="26"/>
+      <c r="J102" s="27"/>
       <c r="K102" s="2"/>
     </row>
     <row r="103" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B103" s="2">
         <v>99</v>
       </c>
-      <c r="C103" s="25"/>
-      <c r="D103" s="26"/>
-      <c r="E103" s="26"/>
-      <c r="F103" s="26"/>
-      <c r="G103" s="26"/>
-      <c r="H103" s="26"/>
-      <c r="I103" s="26"/>
-      <c r="J103" s="27"/>
+      <c r="C103" s="28"/>
+      <c r="D103" s="29"/>
+      <c r="E103" s="29"/>
+      <c r="F103" s="29"/>
+      <c r="G103" s="29"/>
+      <c r="H103" s="29"/>
+      <c r="I103" s="29"/>
+      <c r="J103" s="30"/>
       <c r="K103" s="2"/>
     </row>
     <row r="104" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B104" s="2">
         <v>100</v>
       </c>
-      <c r="C104" s="22" t="s">
+      <c r="C104" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="D104" s="23"/>
-      <c r="E104" s="23"/>
-      <c r="F104" s="23"/>
-      <c r="G104" s="23"/>
-      <c r="H104" s="23"/>
-      <c r="I104" s="23"/>
-      <c r="J104" s="24"/>
+      <c r="D104" s="26"/>
+      <c r="E104" s="26"/>
+      <c r="F104" s="26"/>
+      <c r="G104" s="26"/>
+      <c r="H104" s="26"/>
+      <c r="I104" s="26"/>
+      <c r="J104" s="27"/>
       <c r="K104" s="2"/>
     </row>
     <row r="105" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B105" s="2">
         <v>101</v>
       </c>
-      <c r="C105" s="25"/>
-      <c r="D105" s="26"/>
-      <c r="E105" s="26"/>
-      <c r="F105" s="26"/>
-      <c r="G105" s="26"/>
-      <c r="H105" s="26"/>
-      <c r="I105" s="26"/>
-      <c r="J105" s="27"/>
+      <c r="C105" s="28"/>
+      <c r="D105" s="29"/>
+      <c r="E105" s="29"/>
+      <c r="F105" s="29"/>
+      <c r="G105" s="29"/>
+      <c r="H105" s="29"/>
+      <c r="I105" s="29"/>
+      <c r="J105" s="30"/>
       <c r="K105" s="2"/>
     </row>
     <row r="106" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B106" s="2">
         <v>102</v>
       </c>
-      <c r="C106" s="22" t="s">
+      <c r="C106" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="D106" s="23"/>
-      <c r="E106" s="23"/>
-      <c r="F106" s="23"/>
-      <c r="G106" s="23"/>
-      <c r="H106" s="23"/>
-      <c r="I106" s="23"/>
-      <c r="J106" s="24"/>
+      <c r="D106" s="26"/>
+      <c r="E106" s="26"/>
+      <c r="F106" s="26"/>
+      <c r="G106" s="26"/>
+      <c r="H106" s="26"/>
+      <c r="I106" s="26"/>
+      <c r="J106" s="27"/>
       <c r="K106" s="2"/>
     </row>
     <row r="107" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B107" s="2">
         <v>103</v>
       </c>
-      <c r="C107" s="25"/>
-      <c r="D107" s="26"/>
-      <c r="E107" s="26"/>
-      <c r="F107" s="26"/>
-      <c r="G107" s="26"/>
-      <c r="H107" s="26"/>
-      <c r="I107" s="26"/>
-      <c r="J107" s="27"/>
+      <c r="C107" s="28"/>
+      <c r="D107" s="29"/>
+      <c r="E107" s="29"/>
+      <c r="F107" s="29"/>
+      <c r="G107" s="29"/>
+      <c r="H107" s="29"/>
+      <c r="I107" s="29"/>
+      <c r="J107" s="30"/>
       <c r="K107" s="2"/>
     </row>
     <row r="108" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B108" s="2">
         <v>104</v>
       </c>
-      <c r="C108" s="22" t="s">
+      <c r="C108" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="D108" s="23"/>
-      <c r="E108" s="23"/>
-      <c r="F108" s="23"/>
-      <c r="G108" s="23"/>
-      <c r="H108" s="23"/>
-      <c r="I108" s="23"/>
-      <c r="J108" s="24"/>
+      <c r="D108" s="26"/>
+      <c r="E108" s="26"/>
+      <c r="F108" s="26"/>
+      <c r="G108" s="26"/>
+      <c r="H108" s="26"/>
+      <c r="I108" s="26"/>
+      <c r="J108" s="27"/>
       <c r="K108" s="2"/>
     </row>
     <row r="109" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B109" s="2">
         <v>105</v>
       </c>
-      <c r="C109" s="25"/>
-      <c r="D109" s="26"/>
-      <c r="E109" s="26"/>
-      <c r="F109" s="26"/>
-      <c r="G109" s="26"/>
-      <c r="H109" s="26"/>
-      <c r="I109" s="26"/>
-      <c r="J109" s="27"/>
+      <c r="C109" s="28"/>
+      <c r="D109" s="29"/>
+      <c r="E109" s="29"/>
+      <c r="F109" s="29"/>
+      <c r="G109" s="29"/>
+      <c r="H109" s="29"/>
+      <c r="I109" s="29"/>
+      <c r="J109" s="30"/>
       <c r="K109" s="2"/>
     </row>
     <row r="110" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B110" s="2">
         <v>106</v>
       </c>
-      <c r="C110" s="22" t="s">
+      <c r="C110" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="D110" s="23"/>
-      <c r="E110" s="23"/>
-      <c r="F110" s="23"/>
-      <c r="G110" s="23"/>
-      <c r="H110" s="23"/>
-      <c r="I110" s="23"/>
-      <c r="J110" s="24"/>
+      <c r="D110" s="26"/>
+      <c r="E110" s="26"/>
+      <c r="F110" s="26"/>
+      <c r="G110" s="26"/>
+      <c r="H110" s="26"/>
+      <c r="I110" s="26"/>
+      <c r="J110" s="27"/>
       <c r="K110" s="2"/>
     </row>
     <row r="111" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B111" s="2">
         <v>107</v>
       </c>
-      <c r="C111" s="25"/>
-      <c r="D111" s="26"/>
-      <c r="E111" s="26"/>
-      <c r="F111" s="26"/>
-      <c r="G111" s="26"/>
-      <c r="H111" s="26"/>
-      <c r="I111" s="26"/>
-      <c r="J111" s="27"/>
+      <c r="C111" s="28"/>
+      <c r="D111" s="29"/>
+      <c r="E111" s="29"/>
+      <c r="F111" s="29"/>
+      <c r="G111" s="29"/>
+      <c r="H111" s="29"/>
+      <c r="I111" s="29"/>
+      <c r="J111" s="30"/>
       <c r="K111" s="2"/>
     </row>
     <row r="112" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B112" s="2">
         <v>108</v>
       </c>
-      <c r="C112" s="22" t="s">
+      <c r="C112" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="D112" s="23"/>
-      <c r="E112" s="23"/>
-      <c r="F112" s="23"/>
-      <c r="G112" s="23"/>
-      <c r="H112" s="23"/>
-      <c r="I112" s="23"/>
-      <c r="J112" s="24"/>
+      <c r="D112" s="26"/>
+      <c r="E112" s="26"/>
+      <c r="F112" s="26"/>
+      <c r="G112" s="26"/>
+      <c r="H112" s="26"/>
+      <c r="I112" s="26"/>
+      <c r="J112" s="27"/>
       <c r="K112" s="2"/>
     </row>
     <row r="113" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B113" s="2">
         <v>109</v>
       </c>
-      <c r="C113" s="25"/>
-      <c r="D113" s="26"/>
-      <c r="E113" s="26"/>
-      <c r="F113" s="26"/>
-      <c r="G113" s="26"/>
-      <c r="H113" s="26"/>
-      <c r="I113" s="26"/>
-      <c r="J113" s="27"/>
+      <c r="C113" s="28"/>
+      <c r="D113" s="29"/>
+      <c r="E113" s="29"/>
+      <c r="F113" s="29"/>
+      <c r="G113" s="29"/>
+      <c r="H113" s="29"/>
+      <c r="I113" s="29"/>
+      <c r="J113" s="30"/>
       <c r="K113" s="2"/>
     </row>
     <row r="114" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B114" s="2">
         <v>110</v>
       </c>
-      <c r="C114" s="22" t="s">
+      <c r="C114" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="D114" s="23"/>
-      <c r="E114" s="23"/>
-      <c r="F114" s="23"/>
-      <c r="G114" s="23"/>
-      <c r="H114" s="23"/>
-      <c r="I114" s="23"/>
-      <c r="J114" s="24"/>
+      <c r="D114" s="26"/>
+      <c r="E114" s="26"/>
+      <c r="F114" s="26"/>
+      <c r="G114" s="26"/>
+      <c r="H114" s="26"/>
+      <c r="I114" s="26"/>
+      <c r="J114" s="27"/>
       <c r="K114" s="2"/>
     </row>
     <row r="115" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B115" s="2">
         <v>111</v>
       </c>
-      <c r="C115" s="25"/>
-      <c r="D115" s="26"/>
-      <c r="E115" s="26"/>
-      <c r="F115" s="26"/>
-      <c r="G115" s="26"/>
-      <c r="H115" s="26"/>
-      <c r="I115" s="26"/>
-      <c r="J115" s="27"/>
+      <c r="C115" s="28"/>
+      <c r="D115" s="29"/>
+      <c r="E115" s="29"/>
+      <c r="F115" s="29"/>
+      <c r="G115" s="29"/>
+      <c r="H115" s="29"/>
+      <c r="I115" s="29"/>
+      <c r="J115" s="30"/>
       <c r="K115" s="2"/>
     </row>
     <row r="116" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B116" s="2">
         <v>112</v>
       </c>
-      <c r="C116" s="22" t="s">
+      <c r="C116" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="D116" s="23"/>
-      <c r="E116" s="23"/>
-      <c r="F116" s="23"/>
-      <c r="G116" s="23"/>
-      <c r="H116" s="23"/>
-      <c r="I116" s="23"/>
-      <c r="J116" s="24"/>
+      <c r="D116" s="26"/>
+      <c r="E116" s="26"/>
+      <c r="F116" s="26"/>
+      <c r="G116" s="26"/>
+      <c r="H116" s="26"/>
+      <c r="I116" s="26"/>
+      <c r="J116" s="27"/>
       <c r="K116" s="2"/>
     </row>
     <row r="117" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B117" s="2">
         <v>113</v>
       </c>
-      <c r="C117" s="25"/>
-      <c r="D117" s="26"/>
-      <c r="E117" s="26"/>
-      <c r="F117" s="26"/>
-      <c r="G117" s="26"/>
-      <c r="H117" s="26"/>
-      <c r="I117" s="26"/>
-      <c r="J117" s="27"/>
+      <c r="C117" s="28"/>
+      <c r="D117" s="29"/>
+      <c r="E117" s="29"/>
+      <c r="F117" s="29"/>
+      <c r="G117" s="29"/>
+      <c r="H117" s="29"/>
+      <c r="I117" s="29"/>
+      <c r="J117" s="30"/>
       <c r="K117" s="2"/>
     </row>
     <row r="118" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B118" s="2">
         <v>114</v>
       </c>
-      <c r="C118" s="22" t="s">
+      <c r="C118" s="25" t="s">
         <v>96</v>
       </c>
-      <c r="D118" s="23"/>
-      <c r="E118" s="23"/>
-      <c r="F118" s="23"/>
-      <c r="G118" s="23"/>
-      <c r="H118" s="23"/>
-      <c r="I118" s="23"/>
-      <c r="J118" s="24"/>
+      <c r="D118" s="26"/>
+      <c r="E118" s="26"/>
+      <c r="F118" s="26"/>
+      <c r="G118" s="26"/>
+      <c r="H118" s="26"/>
+      <c r="I118" s="26"/>
+      <c r="J118" s="27"/>
       <c r="K118" s="2"/>
     </row>
     <row r="119" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B119" s="2">
         <v>115</v>
       </c>
-      <c r="C119" s="25"/>
-      <c r="D119" s="26"/>
-      <c r="E119" s="26"/>
-      <c r="F119" s="26"/>
-      <c r="G119" s="26"/>
-      <c r="H119" s="26"/>
-      <c r="I119" s="26"/>
-      <c r="J119" s="27"/>
+      <c r="C119" s="28"/>
+      <c r="D119" s="29"/>
+      <c r="E119" s="29"/>
+      <c r="F119" s="29"/>
+      <c r="G119" s="29"/>
+      <c r="H119" s="29"/>
+      <c r="I119" s="29"/>
+      <c r="J119" s="30"/>
       <c r="K119" s="2"/>
     </row>
     <row r="120" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B120" s="2">
         <v>116</v>
       </c>
-      <c r="C120" s="22" t="s">
+      <c r="C120" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="D120" s="23"/>
-      <c r="E120" s="23"/>
-      <c r="F120" s="23"/>
-      <c r="G120" s="23"/>
-      <c r="H120" s="23"/>
-      <c r="I120" s="23"/>
-      <c r="J120" s="24"/>
+      <c r="D120" s="26"/>
+      <c r="E120" s="26"/>
+      <c r="F120" s="26"/>
+      <c r="G120" s="26"/>
+      <c r="H120" s="26"/>
+      <c r="I120" s="26"/>
+      <c r="J120" s="27"/>
       <c r="K120" s="2"/>
     </row>
     <row r="121" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B121" s="2">
         <v>117</v>
       </c>
-      <c r="C121" s="25"/>
-      <c r="D121" s="26"/>
-      <c r="E121" s="26"/>
-      <c r="F121" s="26"/>
-      <c r="G121" s="26"/>
-      <c r="H121" s="26"/>
-      <c r="I121" s="26"/>
-      <c r="J121" s="27"/>
+      <c r="C121" s="28"/>
+      <c r="D121" s="29"/>
+      <c r="E121" s="29"/>
+      <c r="F121" s="29"/>
+      <c r="G121" s="29"/>
+      <c r="H121" s="29"/>
+      <c r="I121" s="29"/>
+      <c r="J121" s="30"/>
       <c r="K121" s="2"/>
     </row>
     <row r="122" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B122" s="2">
         <v>118</v>
       </c>
-      <c r="C122" s="22" t="s">
+      <c r="C122" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="D122" s="23"/>
-      <c r="E122" s="23"/>
-      <c r="F122" s="23"/>
-      <c r="G122" s="23"/>
-      <c r="H122" s="23"/>
-      <c r="I122" s="23"/>
-      <c r="J122" s="24"/>
+      <c r="D122" s="26"/>
+      <c r="E122" s="26"/>
+      <c r="F122" s="26"/>
+      <c r="G122" s="26"/>
+      <c r="H122" s="26"/>
+      <c r="I122" s="26"/>
+      <c r="J122" s="27"/>
       <c r="K122" s="2"/>
     </row>
     <row r="123" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B123" s="2">
         <v>119</v>
       </c>
-      <c r="C123" s="25"/>
-      <c r="D123" s="26"/>
-      <c r="E123" s="26"/>
-      <c r="F123" s="26"/>
-      <c r="G123" s="26"/>
-      <c r="H123" s="26"/>
-      <c r="I123" s="26"/>
-      <c r="J123" s="27"/>
+      <c r="C123" s="28"/>
+      <c r="D123" s="29"/>
+      <c r="E123" s="29"/>
+      <c r="F123" s="29"/>
+      <c r="G123" s="29"/>
+      <c r="H123" s="29"/>
+      <c r="I123" s="29"/>
+      <c r="J123" s="30"/>
       <c r="K123" s="2"/>
     </row>
     <row r="124" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B124" s="2">
         <v>120</v>
       </c>
-      <c r="C124" s="22" t="s">
+      <c r="C124" s="25" t="s">
         <v>99</v>
       </c>
-      <c r="D124" s="23"/>
-      <c r="E124" s="23"/>
-      <c r="F124" s="23"/>
-      <c r="G124" s="23"/>
-      <c r="H124" s="23"/>
-      <c r="I124" s="23"/>
-      <c r="J124" s="24"/>
+      <c r="D124" s="26"/>
+      <c r="E124" s="26"/>
+      <c r="F124" s="26"/>
+      <c r="G124" s="26"/>
+      <c r="H124" s="26"/>
+      <c r="I124" s="26"/>
+      <c r="J124" s="27"/>
       <c r="K124" s="2"/>
     </row>
     <row r="125" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B125" s="2">
         <v>121</v>
       </c>
-      <c r="C125" s="25"/>
-      <c r="D125" s="26"/>
-      <c r="E125" s="26"/>
-      <c r="F125" s="26"/>
-      <c r="G125" s="26"/>
-      <c r="H125" s="26"/>
-      <c r="I125" s="26"/>
-      <c r="J125" s="27"/>
+      <c r="C125" s="28"/>
+      <c r="D125" s="29"/>
+      <c r="E125" s="29"/>
+      <c r="F125" s="29"/>
+      <c r="G125" s="29"/>
+      <c r="H125" s="29"/>
+      <c r="I125" s="29"/>
+      <c r="J125" s="30"/>
       <c r="K125" s="2"/>
     </row>
     <row r="126" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B126" s="2">
         <v>122</v>
       </c>
-      <c r="C126" s="22" t="s">
+      <c r="C126" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="D126" s="23"/>
-      <c r="E126" s="23"/>
-      <c r="F126" s="23"/>
-      <c r="G126" s="23"/>
-      <c r="H126" s="23"/>
-      <c r="I126" s="23"/>
-      <c r="J126" s="24"/>
+      <c r="D126" s="26"/>
+      <c r="E126" s="26"/>
+      <c r="F126" s="26"/>
+      <c r="G126" s="26"/>
+      <c r="H126" s="26"/>
+      <c r="I126" s="26"/>
+      <c r="J126" s="27"/>
       <c r="K126" s="2"/>
     </row>
     <row r="127" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B127" s="2">
         <v>123</v>
       </c>
-      <c r="C127" s="25"/>
-      <c r="D127" s="26"/>
-      <c r="E127" s="26"/>
-      <c r="F127" s="26"/>
-      <c r="G127" s="26"/>
-      <c r="H127" s="26"/>
-      <c r="I127" s="26"/>
-      <c r="J127" s="27"/>
+      <c r="C127" s="28"/>
+      <c r="D127" s="29"/>
+      <c r="E127" s="29"/>
+      <c r="F127" s="29"/>
+      <c r="G127" s="29"/>
+      <c r="H127" s="29"/>
+      <c r="I127" s="29"/>
+      <c r="J127" s="30"/>
       <c r="K127" s="2"/>
     </row>
     <row r="128" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B128" s="2">
         <v>124</v>
       </c>
-      <c r="C128" s="22" t="s">
+      <c r="C128" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="D128" s="23"/>
-      <c r="E128" s="23"/>
-      <c r="F128" s="23"/>
-      <c r="G128" s="23"/>
-      <c r="H128" s="23"/>
-      <c r="I128" s="23"/>
-      <c r="J128" s="24"/>
+      <c r="D128" s="26"/>
+      <c r="E128" s="26"/>
+      <c r="F128" s="26"/>
+      <c r="G128" s="26"/>
+      <c r="H128" s="26"/>
+      <c r="I128" s="26"/>
+      <c r="J128" s="27"/>
       <c r="K128" s="2"/>
     </row>
     <row r="129" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B129" s="2">
         <v>125</v>
       </c>
-      <c r="C129" s="25"/>
-      <c r="D129" s="26"/>
-      <c r="E129" s="26"/>
-      <c r="F129" s="26"/>
-      <c r="G129" s="26"/>
-      <c r="H129" s="26"/>
-      <c r="I129" s="26"/>
-      <c r="J129" s="27"/>
+      <c r="C129" s="28"/>
+      <c r="D129" s="29"/>
+      <c r="E129" s="29"/>
+      <c r="F129" s="29"/>
+      <c r="G129" s="29"/>
+      <c r="H129" s="29"/>
+      <c r="I129" s="29"/>
+      <c r="J129" s="30"/>
       <c r="K129" s="2"/>
     </row>
+    <row r="130" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B130" s="2">
+        <v>126</v>
+      </c>
+      <c r="C130" s="31" t="s">
+        <v>106</v>
+      </c>
+      <c r="D130" s="31"/>
+      <c r="E130" s="31"/>
+      <c r="F130" s="31"/>
+      <c r="G130" s="31"/>
+      <c r="H130" s="31"/>
+      <c r="I130" s="31"/>
+      <c r="J130" s="31"/>
+      <c r="K130" s="2"/>
+    </row>
+    <row r="131" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B131" s="2">
+        <v>127</v>
+      </c>
+      <c r="C131" s="31" t="s">
+        <v>105</v>
+      </c>
+      <c r="D131" s="31"/>
+      <c r="E131" s="31"/>
+      <c r="F131" s="31"/>
+      <c r="G131" s="31"/>
+      <c r="H131" s="31"/>
+      <c r="I131" s="31"/>
+      <c r="J131" s="31"/>
+      <c r="K131" s="2"/>
+    </row>
+    <row r="132" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B132" s="2">
+        <v>128</v>
+      </c>
+      <c r="C132" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="D132" s="31"/>
+      <c r="E132" s="31"/>
+      <c r="F132" s="31"/>
+      <c r="G132" s="31"/>
+      <c r="H132" s="31"/>
+      <c r="I132" s="31"/>
+      <c r="J132" s="31"/>
+      <c r="K132" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="67">
+  <mergeCells count="70">
+    <mergeCell ref="C130:J130"/>
+    <mergeCell ref="C131:J131"/>
+    <mergeCell ref="C132:J132"/>
+    <mergeCell ref="C18:J19"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="R2:T2"/>
+    <mergeCell ref="C4:J4"/>
+    <mergeCell ref="C5:J6"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="C7:J7"/>
+    <mergeCell ref="C8:J9"/>
+    <mergeCell ref="C10:J11"/>
+    <mergeCell ref="C12:J13"/>
+    <mergeCell ref="C14:J15"/>
+    <mergeCell ref="C16:J17"/>
+    <mergeCell ref="C42:J43"/>
+    <mergeCell ref="C20:J21"/>
+    <mergeCell ref="C22:J23"/>
+    <mergeCell ref="C24:J25"/>
+    <mergeCell ref="C26:J27"/>
+    <mergeCell ref="C28:J29"/>
+    <mergeCell ref="C30:J31"/>
+    <mergeCell ref="C32:J33"/>
+    <mergeCell ref="C34:J35"/>
+    <mergeCell ref="C36:J37"/>
+    <mergeCell ref="C38:J39"/>
+    <mergeCell ref="C40:J41"/>
+    <mergeCell ref="C66:J67"/>
+    <mergeCell ref="C44:J45"/>
+    <mergeCell ref="C46:J47"/>
+    <mergeCell ref="C48:J49"/>
+    <mergeCell ref="C50:J51"/>
+    <mergeCell ref="C52:J53"/>
+    <mergeCell ref="C54:J55"/>
+    <mergeCell ref="C56:J57"/>
+    <mergeCell ref="C58:J59"/>
+    <mergeCell ref="C60:J61"/>
+    <mergeCell ref="C62:J63"/>
+    <mergeCell ref="C64:J65"/>
+    <mergeCell ref="C90:J91"/>
+    <mergeCell ref="C68:J69"/>
+    <mergeCell ref="C70:J71"/>
+    <mergeCell ref="C72:J73"/>
+    <mergeCell ref="C74:J75"/>
+    <mergeCell ref="C76:J77"/>
+    <mergeCell ref="C78:J79"/>
+    <mergeCell ref="C80:J81"/>
+    <mergeCell ref="C82:J83"/>
+    <mergeCell ref="C84:J85"/>
+    <mergeCell ref="C86:J87"/>
+    <mergeCell ref="C88:J89"/>
+    <mergeCell ref="C114:J115"/>
+    <mergeCell ref="C92:J93"/>
+    <mergeCell ref="C94:J95"/>
+    <mergeCell ref="C96:J97"/>
+    <mergeCell ref="C98:J99"/>
+    <mergeCell ref="C100:J101"/>
+    <mergeCell ref="C102:J103"/>
+    <mergeCell ref="C104:J105"/>
+    <mergeCell ref="C106:J107"/>
+    <mergeCell ref="C108:J109"/>
+    <mergeCell ref="C110:J111"/>
+    <mergeCell ref="C112:J113"/>
     <mergeCell ref="C128:J129"/>
     <mergeCell ref="C116:J117"/>
     <mergeCell ref="C118:J119"/>
@@ -5426,66 +5561,6 @@
     <mergeCell ref="C122:J123"/>
     <mergeCell ref="C124:J125"/>
     <mergeCell ref="C126:J127"/>
-    <mergeCell ref="C104:J105"/>
-    <mergeCell ref="C106:J107"/>
-    <mergeCell ref="C108:J109"/>
-    <mergeCell ref="C110:J111"/>
-    <mergeCell ref="C112:J113"/>
-    <mergeCell ref="C114:J115"/>
-    <mergeCell ref="C92:J93"/>
-    <mergeCell ref="C94:J95"/>
-    <mergeCell ref="C96:J97"/>
-    <mergeCell ref="C98:J99"/>
-    <mergeCell ref="C100:J101"/>
-    <mergeCell ref="C102:J103"/>
-    <mergeCell ref="C80:J81"/>
-    <mergeCell ref="C82:J83"/>
-    <mergeCell ref="C84:J85"/>
-    <mergeCell ref="C86:J87"/>
-    <mergeCell ref="C88:J89"/>
-    <mergeCell ref="C90:J91"/>
-    <mergeCell ref="C68:J69"/>
-    <mergeCell ref="C70:J71"/>
-    <mergeCell ref="C72:J73"/>
-    <mergeCell ref="C74:J75"/>
-    <mergeCell ref="C76:J77"/>
-    <mergeCell ref="C78:J79"/>
-    <mergeCell ref="C56:J57"/>
-    <mergeCell ref="C58:J59"/>
-    <mergeCell ref="C60:J61"/>
-    <mergeCell ref="C62:J63"/>
-    <mergeCell ref="C64:J65"/>
-    <mergeCell ref="C66:J67"/>
-    <mergeCell ref="C44:J45"/>
-    <mergeCell ref="C46:J47"/>
-    <mergeCell ref="C48:J49"/>
-    <mergeCell ref="C50:J51"/>
-    <mergeCell ref="C52:J53"/>
-    <mergeCell ref="C54:J55"/>
-    <mergeCell ref="C32:J33"/>
-    <mergeCell ref="C34:J35"/>
-    <mergeCell ref="C36:J37"/>
-    <mergeCell ref="C38:J39"/>
-    <mergeCell ref="C40:J41"/>
-    <mergeCell ref="C42:J43"/>
-    <mergeCell ref="C20:J21"/>
-    <mergeCell ref="C22:J23"/>
-    <mergeCell ref="C24:J25"/>
-    <mergeCell ref="C26:J27"/>
-    <mergeCell ref="C28:J29"/>
-    <mergeCell ref="C30:J31"/>
-    <mergeCell ref="C8:J9"/>
-    <mergeCell ref="C10:J11"/>
-    <mergeCell ref="C12:J13"/>
-    <mergeCell ref="C14:J15"/>
-    <mergeCell ref="C16:J17"/>
-    <mergeCell ref="C18:J19"/>
-    <mergeCell ref="N2:P2"/>
-    <mergeCell ref="R2:T2"/>
-    <mergeCell ref="C4:J4"/>
-    <mergeCell ref="C5:J6"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="C7:J7"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[Mod] Display User ID in Status Screen
- from now on, If user log-in succeed, the User ID will displayed on the status screen.
- UI Changed : memo_Log component (adv -> tcx)
- Add DATA_TYPE_DEFINED ID (Making Game Room ID)
- Client Thread will take his screen status and User ID.
- Sign Up/In Message Changed (for server log info)
- DB Path has been changed (because now, I'm in home)
</commit_message>
<xml_diff>
--- a/T_Design.xlsx
+++ b/T_Design.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wave\010_Project\010_Game\Tetris\Server\010_Source\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wave\010_Project\010_Game\Tetris\Tetris_Server\020_SourceCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B336C0E8-C1A3-46C4-B826-E0D2E4B838BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3BE24F1-243C-41D8-8634-B23AF2F4C967}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="5" xr2:uid="{CBDAA684-FC25-4649-B038-1CECF5D4149C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CBDAA684-FC25-4649-B038-1CECF5D4149C}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="1" r:id="rId1"/>
@@ -26,12 +26,20 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="113">
   <si>
     <t>Byte</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -179,14 +187,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>In Game Whole Data</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>In Game My Data</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>0x0A</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -432,6 +432,18 @@
   </si>
   <si>
     <t>Message Type (0x02 Sign In)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x0C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>In Game Data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Make Game Room</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -630,7 +642,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -662,6 +674,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -715,9 +730,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -734,6 +746,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1065,10 +1080,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3CD6B57-0370-464C-92D1-8CCB08728235}">
-  <dimension ref="C2:I14"/>
+  <dimension ref="C2:I24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1081,16 +1096,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="G2" s="12" t="s">
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="G2" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
     </row>
     <row r="3" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C3" s="3" t="s">
@@ -1251,14 +1266,14 @@
         <v>34</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>36</v>
+        <v>112</v>
       </c>
       <c r="E11" s="2"/>
       <c r="G11" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>36</v>
+        <v>112</v>
       </c>
       <c r="I11" s="2"/>
     </row>
@@ -1266,53 +1281,141 @@
       <c r="C12" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>42</v>
+      <c r="D12" s="12" t="s">
+        <v>36</v>
       </c>
       <c r="E12" s="2"/>
       <c r="G12" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="H12" s="2" t="s">
-        <v>42</v>
+      <c r="H12" s="12" t="s">
+        <v>36</v>
       </c>
       <c r="I12" s="2"/>
     </row>
     <row r="13" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="12" t="s">
         <v>40</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>37</v>
       </c>
       <c r="E13" s="2"/>
       <c r="G13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H13" s="12" t="s">
         <v>40</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>37</v>
       </c>
       <c r="I13" s="2"/>
     </row>
     <row r="14" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C14" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E14" s="2">
+        <v>39</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="G14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H14" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="I14" s="2"/>
+    </row>
+    <row r="15" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C15" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="E15" s="12">
         <v>1300</v>
       </c>
-      <c r="G14" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I14" s="2">
+      <c r="G15" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="H15" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="I15" s="12">
         <v>300</v>
       </c>
+    </row>
+    <row r="16" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+    </row>
+    <row r="17" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+    </row>
+    <row r="18" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+    </row>
+    <row r="19" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+    </row>
+    <row r="20" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+    </row>
+    <row r="21" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+    </row>
+    <row r="22" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+    </row>
+    <row r="23" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+    </row>
+    <row r="24" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1347,18 +1450,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="N2" s="13" t="str">
+      <c r="N2" s="14" t="str">
         <f>Type!C2</f>
         <v>Server -&gt; Client</v>
       </c>
-      <c r="O2" s="13"/>
-      <c r="P2" s="13"/>
-      <c r="R2" s="13" t="str">
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
+      <c r="R2" s="14" t="str">
         <f>Type!G2</f>
         <v>Client -&gt; Server</v>
       </c>
-      <c r="S2" s="13"/>
-      <c r="T2" s="13"/>
+      <c r="S2" s="14"/>
+      <c r="T2" s="14"/>
     </row>
     <row r="3" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="6" t="s">
@@ -1420,16 +1523,16 @@
       <c r="B4" s="4">
         <v>0</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
       <c r="K4" s="4" t="s">
         <v>11</v>
       </c>
@@ -1462,17 +1565,17 @@
       <c r="B5" s="4">
         <v>1</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="23"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="24"/>
       <c r="N5" s="2" t="str">
         <f>IF(ISBLANK(Type!C5),"",Type!C5)</f>
         <v>0x02</v>
@@ -1502,15 +1605,15 @@
       <c r="B6" s="4">
         <v>2</v>
       </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="24"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="25"/>
       <c r="N6" s="2" t="str">
         <f>IF(ISBLANK(Type!C6),"",Type!C6)</f>
         <v>0x03</v>
@@ -1540,16 +1643,16 @@
       <c r="B7" s="4">
         <v>3</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="21"/>
-      <c r="J7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="23"/>
       <c r="K7" s="5"/>
       <c r="N7" s="2" t="str">
         <f>IF(ISBLANK(Type!C7),"",Type!C7)</f>
@@ -1709,7 +1812,7 @@
       </c>
       <c r="O11" s="2" t="str">
         <f>IF(ISBLANK(Type!D11),"",Type!D11)</f>
-        <v>Enter Game Room</v>
+        <v>Make Game Room</v>
       </c>
       <c r="P11" s="2" t="str">
         <f>IF(ISBLANK(Type!E11),"",Type!E11)</f>
@@ -1721,7 +1824,7 @@
       </c>
       <c r="S11" s="2" t="str">
         <f>IF(ISBLANK(Type!H11),"",Type!H11)</f>
-        <v>Enter Game Room</v>
+        <v>Make Game Room</v>
       </c>
       <c r="T11" s="2" t="str">
         <f>IF(ISBLANK(Type!I11),"",Type!I11)</f>
@@ -1747,7 +1850,7 @@
       </c>
       <c r="O12" s="2" t="str">
         <f>IF(ISBLANK(Type!D12),"",Type!D12)</f>
-        <v>Escape Game Room</v>
+        <v>Enter Game Room</v>
       </c>
       <c r="P12" s="2" t="str">
         <f>IF(ISBLANK(Type!E12),"",Type!E12)</f>
@@ -1759,7 +1862,7 @@
       </c>
       <c r="S12" s="2" t="str">
         <f>IF(ISBLANK(Type!H12),"",Type!H12)</f>
-        <v>Escape Game Room</v>
+        <v>Enter Game Room</v>
       </c>
       <c r="T12" s="2" t="str">
         <f>IF(ISBLANK(Type!I12),"",Type!I12)</f>
@@ -1785,7 +1888,7 @@
       </c>
       <c r="O13" s="2" t="str">
         <f>IF(ISBLANK(Type!D13),"",Type!D13)</f>
-        <v>Heart Beat</v>
+        <v>Escape Game Room</v>
       </c>
       <c r="P13" s="2" t="str">
         <f>IF(ISBLANK(Type!E13),"",Type!E13)</f>
@@ -1797,7 +1900,7 @@
       </c>
       <c r="S13" s="2" t="str">
         <f>IF(ISBLANK(Type!H13),"",Type!H13)</f>
-        <v>Heart Beat</v>
+        <v>Escape Game Room</v>
       </c>
       <c r="T13" s="2" t="str">
         <f>IF(ISBLANK(Type!I13),"",Type!I13)</f>
@@ -1823,11 +1926,11 @@
       </c>
       <c r="O14" s="2" t="str">
         <f>IF(ISBLANK(Type!D14),"",Type!D14)</f>
-        <v>In Game Whole Data</v>
-      </c>
-      <c r="P14" s="2">
+        <v>Heart Beat</v>
+      </c>
+      <c r="P14" s="2" t="str">
         <f>IF(ISBLANK(Type!E14),"",Type!E14)</f>
-        <v>1300</v>
+        <v/>
       </c>
       <c r="R14" s="2" t="str">
         <f>IF(ISBLANK(Type!G14),"",Type!G14)</f>
@@ -1835,11 +1938,11 @@
       </c>
       <c r="S14" s="2" t="str">
         <f>IF(ISBLANK(Type!H14),"",Type!H14)</f>
-        <v>In Game My Data</v>
-      </c>
-      <c r="T14" s="2">
+        <v>Heart Beat</v>
+      </c>
+      <c r="T14" s="2" t="str">
         <f>IF(ISBLANK(Type!I14),"",Type!I14)</f>
-        <v>300</v>
+        <v/>
       </c>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.3">
@@ -1857,27 +1960,27 @@
       <c r="K15" s="2"/>
       <c r="N15" s="2" t="str">
         <f>IF(ISBLANK(Type!C15),"",Type!C15)</f>
-        <v/>
+        <v>0x0C</v>
       </c>
       <c r="O15" s="2" t="str">
         <f>IF(ISBLANK(Type!D15),"",Type!D15)</f>
-        <v/>
-      </c>
-      <c r="P15" s="2" t="str">
+        <v>In Game Data</v>
+      </c>
+      <c r="P15" s="2">
         <f>IF(ISBLANK(Type!E15),"",Type!E15)</f>
-        <v/>
+        <v>1300</v>
       </c>
       <c r="R15" s="2" t="str">
         <f>IF(ISBLANK(Type!G15),"",Type!G15)</f>
-        <v/>
+        <v>0x0C</v>
       </c>
       <c r="S15" s="2" t="str">
         <f>IF(ISBLANK(Type!H15),"",Type!H15)</f>
-        <v/>
-      </c>
-      <c r="T15" s="2" t="str">
+        <v>In Game Data</v>
+      </c>
+      <c r="T15" s="2">
         <f>IF(ISBLANK(Type!I15),"",Type!I15)</f>
-        <v/>
+        <v>300</v>
       </c>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.3">
@@ -2262,18 +2365,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="N2" s="13" t="str">
+      <c r="N2" s="14" t="str">
         <f>Type!C2</f>
         <v>Server -&gt; Client</v>
       </c>
-      <c r="O2" s="13"/>
-      <c r="P2" s="13"/>
-      <c r="R2" s="13" t="str">
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
+      <c r="R2" s="14" t="str">
         <f>Type!G2</f>
         <v>Client -&gt; Server</v>
       </c>
-      <c r="S2" s="13"/>
-      <c r="T2" s="13"/>
+      <c r="S2" s="14"/>
+      <c r="T2" s="14"/>
     </row>
     <row r="3" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="8" t="s">
@@ -2335,16 +2438,16 @@
       <c r="B4" s="7">
         <v>0</v>
       </c>
-      <c r="C4" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
+      <c r="C4" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
       <c r="K4" s="7" t="s">
         <v>11</v>
       </c>
@@ -2377,17 +2480,17 @@
       <c r="B5" s="7">
         <v>1</v>
       </c>
-      <c r="C5" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="23"/>
+      <c r="C5" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="24"/>
       <c r="N5" s="2" t="str">
         <f>IF(ISBLANK(Type!C5),"",Type!C5)</f>
         <v>0x02</v>
@@ -2417,15 +2520,15 @@
       <c r="B6" s="7">
         <v>2</v>
       </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="24"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="25"/>
       <c r="N6" s="2" t="str">
         <f>IF(ISBLANK(Type!C6),"",Type!C6)</f>
         <v>0x03</v>
@@ -2455,16 +2558,16 @@
       <c r="B7" s="7">
         <v>3</v>
       </c>
-      <c r="C7" s="20" t="s">
-        <v>102</v>
-      </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="21"/>
-      <c r="J7" s="22"/>
+      <c r="C7" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="23"/>
       <c r="K7" s="5"/>
       <c r="N7" s="2" t="str">
         <f>IF(ISBLANK(Type!C7),"",Type!C7)</f>
@@ -2495,16 +2598,16 @@
       <c r="B8" s="2">
         <v>4</v>
       </c>
-      <c r="C8" s="25" t="s">
-        <v>104</v>
-      </c>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="27"/>
+      <c r="C8" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="28"/>
       <c r="K8" s="2"/>
       <c r="N8" s="2" t="str">
         <f>IF(ISBLANK(Type!C8),"",Type!C8)</f>
@@ -2590,7 +2693,7 @@
       </c>
       <c r="O11" s="2" t="str">
         <f>IF(ISBLANK(Type!D11),"",Type!D11)</f>
-        <v>Enter Game Room</v>
+        <v>Make Game Room</v>
       </c>
       <c r="P11" s="2" t="str">
         <f>IF(ISBLANK(Type!E11),"",Type!E11)</f>
@@ -2602,7 +2705,7 @@
       </c>
       <c r="S11" s="2" t="str">
         <f>IF(ISBLANK(Type!H11),"",Type!H11)</f>
-        <v>Enter Game Room</v>
+        <v>Make Game Room</v>
       </c>
       <c r="T11" s="2" t="str">
         <f>IF(ISBLANK(Type!I11),"",Type!I11)</f>
@@ -2616,7 +2719,7 @@
       </c>
       <c r="O12" s="2" t="str">
         <f>IF(ISBLANK(Type!D12),"",Type!D12)</f>
-        <v>Escape Game Room</v>
+        <v>Enter Game Room</v>
       </c>
       <c r="P12" s="2" t="str">
         <f>IF(ISBLANK(Type!E12),"",Type!E12)</f>
@@ -2628,7 +2731,7 @@
       </c>
       <c r="S12" s="2" t="str">
         <f>IF(ISBLANK(Type!H12),"",Type!H12)</f>
-        <v>Escape Game Room</v>
+        <v>Enter Game Room</v>
       </c>
       <c r="T12" s="2" t="str">
         <f>IF(ISBLANK(Type!I12),"",Type!I12)</f>
@@ -2642,7 +2745,7 @@
       </c>
       <c r="O13" s="2" t="str">
         <f>IF(ISBLANK(Type!D13),"",Type!D13)</f>
-        <v>Heart Beat</v>
+        <v>Escape Game Room</v>
       </c>
       <c r="P13" s="2" t="str">
         <f>IF(ISBLANK(Type!E13),"",Type!E13)</f>
@@ -2654,7 +2757,7 @@
       </c>
       <c r="S13" s="2" t="str">
         <f>IF(ISBLANK(Type!H13),"",Type!H13)</f>
-        <v>Heart Beat</v>
+        <v>Escape Game Room</v>
       </c>
       <c r="T13" s="2" t="str">
         <f>IF(ISBLANK(Type!I13),"",Type!I13)</f>
@@ -2668,11 +2771,11 @@
       </c>
       <c r="O14" s="2" t="str">
         <f>IF(ISBLANK(Type!D14),"",Type!D14)</f>
-        <v>In Game Whole Data</v>
-      </c>
-      <c r="P14" s="2">
+        <v>Heart Beat</v>
+      </c>
+      <c r="P14" s="2" t="str">
         <f>IF(ISBLANK(Type!E14),"",Type!E14)</f>
-        <v>1300</v>
+        <v/>
       </c>
       <c r="R14" s="2" t="str">
         <f>IF(ISBLANK(Type!G14),"",Type!G14)</f>
@@ -2680,37 +2783,37 @@
       </c>
       <c r="S14" s="2" t="str">
         <f>IF(ISBLANK(Type!H14),"",Type!H14)</f>
-        <v>In Game My Data</v>
-      </c>
-      <c r="T14" s="2">
+        <v>Heart Beat</v>
+      </c>
+      <c r="T14" s="2" t="str">
         <f>IF(ISBLANK(Type!I14),"",Type!I14)</f>
-        <v>300</v>
+        <v/>
       </c>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.3">
       <c r="N15" s="2" t="str">
         <f>IF(ISBLANK(Type!C15),"",Type!C15)</f>
-        <v/>
+        <v>0x0C</v>
       </c>
       <c r="O15" s="2" t="str">
         <f>IF(ISBLANK(Type!D15),"",Type!D15)</f>
-        <v/>
-      </c>
-      <c r="P15" s="2" t="str">
+        <v>In Game Data</v>
+      </c>
+      <c r="P15" s="2">
         <f>IF(ISBLANK(Type!E15),"",Type!E15)</f>
-        <v/>
+        <v>1300</v>
       </c>
       <c r="R15" s="2" t="str">
         <f>IF(ISBLANK(Type!G15),"",Type!G15)</f>
-        <v/>
+        <v>0x0C</v>
       </c>
       <c r="S15" s="2" t="str">
         <f>IF(ISBLANK(Type!H15),"",Type!H15)</f>
-        <v/>
-      </c>
-      <c r="T15" s="2" t="str">
+        <v>In Game Data</v>
+      </c>
+      <c r="T15" s="2">
         <f>IF(ISBLANK(Type!I15),"",Type!I15)</f>
-        <v/>
+        <v>300</v>
       </c>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.3">
@@ -2989,18 +3092,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="N2" s="13" t="str">
+      <c r="N2" s="14" t="str">
         <f>Type!C2</f>
         <v>Server -&gt; Client</v>
       </c>
-      <c r="O2" s="13"/>
-      <c r="P2" s="13"/>
-      <c r="R2" s="13" t="str">
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
+      <c r="R2" s="14" t="str">
         <f>Type!G2</f>
         <v>Client -&gt; Server</v>
       </c>
-      <c r="S2" s="13"/>
-      <c r="T2" s="13"/>
+      <c r="S2" s="14"/>
+      <c r="T2" s="14"/>
     </row>
     <row r="3" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="8" t="s">
@@ -3062,16 +3165,16 @@
       <c r="B4" s="7">
         <v>0</v>
       </c>
-      <c r="C4" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
+      <c r="C4" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
       <c r="K4" s="7" t="s">
         <v>11</v>
       </c>
@@ -3104,17 +3207,17 @@
       <c r="B5" s="7">
         <v>1</v>
       </c>
-      <c r="C5" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="23"/>
+      <c r="C5" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="24"/>
       <c r="N5" s="2" t="str">
         <f>IF(ISBLANK(Type!C5),"",Type!C5)</f>
         <v>0x02</v>
@@ -3144,15 +3247,15 @@
       <c r="B6" s="7">
         <v>2</v>
       </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="24"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="25"/>
       <c r="N6" s="2" t="str">
         <f>IF(ISBLANK(Type!C6),"",Type!C6)</f>
         <v>0x03</v>
@@ -3182,16 +3285,16 @@
       <c r="B7" s="7">
         <v>3</v>
       </c>
-      <c r="C7" s="20" t="s">
-        <v>100</v>
-      </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="21"/>
-      <c r="J7" s="22"/>
+      <c r="C7" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="23"/>
       <c r="K7" s="5"/>
       <c r="N7" s="2" t="str">
         <f>IF(ISBLANK(Type!C7),"",Type!C7)</f>
@@ -3223,7 +3326,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D8" s="30"/>
       <c r="E8" s="30"/>
@@ -3301,7 +3404,7 @@
         <v>6</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D10" s="30"/>
       <c r="E10" s="30"/>
@@ -3355,7 +3458,7 @@
       </c>
       <c r="O11" s="2" t="str">
         <f>IF(ISBLANK(Type!D11),"",Type!D11)</f>
-        <v>Enter Game Room</v>
+        <v>Make Game Room</v>
       </c>
       <c r="P11" s="2" t="str">
         <f>IF(ISBLANK(Type!E11),"",Type!E11)</f>
@@ -3367,7 +3470,7 @@
       </c>
       <c r="S11" s="2" t="str">
         <f>IF(ISBLANK(Type!H11),"",Type!H11)</f>
-        <v>Enter Game Room</v>
+        <v>Make Game Room</v>
       </c>
       <c r="T11" s="2" t="str">
         <f>IF(ISBLANK(Type!I11),"",Type!I11)</f>
@@ -3379,7 +3482,7 @@
         <v>8</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D12" s="30"/>
       <c r="E12" s="30"/>
@@ -3395,7 +3498,7 @@
       </c>
       <c r="O12" s="2" t="str">
         <f>IF(ISBLANK(Type!D12),"",Type!D12)</f>
-        <v>Escape Game Room</v>
+        <v>Enter Game Room</v>
       </c>
       <c r="P12" s="2" t="str">
         <f>IF(ISBLANK(Type!E12),"",Type!E12)</f>
@@ -3407,7 +3510,7 @@
       </c>
       <c r="S12" s="2" t="str">
         <f>IF(ISBLANK(Type!H12),"",Type!H12)</f>
-        <v>Escape Game Room</v>
+        <v>Enter Game Room</v>
       </c>
       <c r="T12" s="2" t="str">
         <f>IF(ISBLANK(Type!I12),"",Type!I12)</f>
@@ -3433,7 +3536,7 @@
       </c>
       <c r="O13" s="2" t="str">
         <f>IF(ISBLANK(Type!D13),"",Type!D13)</f>
-        <v>Heart Beat</v>
+        <v>Escape Game Room</v>
       </c>
       <c r="P13" s="2" t="str">
         <f>IF(ISBLANK(Type!E13),"",Type!E13)</f>
@@ -3445,7 +3548,7 @@
       </c>
       <c r="S13" s="2" t="str">
         <f>IF(ISBLANK(Type!H13),"",Type!H13)</f>
-        <v>Heart Beat</v>
+        <v>Escape Game Room</v>
       </c>
       <c r="T13" s="2" t="str">
         <f>IF(ISBLANK(Type!I13),"",Type!I13)</f>
@@ -3457,7 +3560,7 @@
         <v>10</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D14" s="30"/>
       <c r="E14" s="30"/>
@@ -3473,11 +3576,11 @@
       </c>
       <c r="O14" s="2" t="str">
         <f>IF(ISBLANK(Type!D14),"",Type!D14)</f>
-        <v>In Game Whole Data</v>
-      </c>
-      <c r="P14" s="2">
+        <v>Heart Beat</v>
+      </c>
+      <c r="P14" s="2" t="str">
         <f>IF(ISBLANK(Type!E14),"",Type!E14)</f>
-        <v>1300</v>
+        <v/>
       </c>
       <c r="R14" s="2" t="str">
         <f>IF(ISBLANK(Type!G14),"",Type!G14)</f>
@@ -3485,11 +3588,11 @@
       </c>
       <c r="S14" s="2" t="str">
         <f>IF(ISBLANK(Type!H14),"",Type!H14)</f>
-        <v>In Game My Data</v>
-      </c>
-      <c r="T14" s="2">
+        <v>Heart Beat</v>
+      </c>
+      <c r="T14" s="2" t="str">
         <f>IF(ISBLANK(Type!I14),"",Type!I14)</f>
-        <v>300</v>
+        <v/>
       </c>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.3">
@@ -3507,27 +3610,27 @@
       <c r="K15" s="2"/>
       <c r="N15" s="2" t="str">
         <f>IF(ISBLANK(Type!C15),"",Type!C15)</f>
-        <v/>
+        <v>0x0C</v>
       </c>
       <c r="O15" s="2" t="str">
         <f>IF(ISBLANK(Type!D15),"",Type!D15)</f>
-        <v/>
-      </c>
-      <c r="P15" s="2" t="str">
+        <v>In Game Data</v>
+      </c>
+      <c r="P15" s="2">
         <f>IF(ISBLANK(Type!E15),"",Type!E15)</f>
-        <v/>
+        <v>1300</v>
       </c>
       <c r="R15" s="2" t="str">
         <f>IF(ISBLANK(Type!G15),"",Type!G15)</f>
-        <v/>
+        <v>0x0C</v>
       </c>
       <c r="S15" s="2" t="str">
         <f>IF(ISBLANK(Type!H15),"",Type!H15)</f>
-        <v/>
-      </c>
-      <c r="T15" s="2" t="str">
+        <v>In Game Data</v>
+      </c>
+      <c r="T15" s="2">
         <f>IF(ISBLANK(Type!I15),"",Type!I15)</f>
-        <v/>
+        <v>300</v>
       </c>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.3">
@@ -3535,7 +3638,7 @@
         <v>12</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D16" s="30"/>
       <c r="E16" s="30"/>
@@ -3613,7 +3716,7 @@
         <v>14</v>
       </c>
       <c r="C18" s="29" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D18" s="30"/>
       <c r="E18" s="30"/>
@@ -3691,7 +3794,7 @@
         <v>16</v>
       </c>
       <c r="C20" s="29" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D20" s="30"/>
       <c r="E20" s="30"/>
@@ -3769,7 +3872,7 @@
         <v>18</v>
       </c>
       <c r="C22" s="29" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D22" s="30"/>
       <c r="E22" s="30"/>
@@ -3847,7 +3950,7 @@
         <v>20</v>
       </c>
       <c r="C24" s="29" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D24" s="30"/>
       <c r="E24" s="30"/>
@@ -3901,7 +4004,7 @@
         <v>22</v>
       </c>
       <c r="C26" s="29" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D26" s="30"/>
       <c r="E26" s="30"/>
@@ -3931,7 +4034,7 @@
         <v>24</v>
       </c>
       <c r="C28" s="29" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D28" s="30"/>
       <c r="E28" s="30"/>
@@ -3961,7 +4064,7 @@
         <v>26</v>
       </c>
       <c r="C30" s="29" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D30" s="30"/>
       <c r="E30" s="30"/>
@@ -3991,7 +4094,7 @@
         <v>28</v>
       </c>
       <c r="C32" s="29" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D32" s="30"/>
       <c r="E32" s="30"/>
@@ -4021,7 +4124,7 @@
         <v>30</v>
       </c>
       <c r="C34" s="29" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D34" s="30"/>
       <c r="E34" s="30"/>
@@ -4051,7 +4154,7 @@
         <v>32</v>
       </c>
       <c r="C36" s="29" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D36" s="30"/>
       <c r="E36" s="30"/>
@@ -4081,7 +4184,7 @@
         <v>34</v>
       </c>
       <c r="C38" s="29" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D38" s="30"/>
       <c r="E38" s="30"/>
@@ -4111,7 +4214,7 @@
         <v>36</v>
       </c>
       <c r="C40" s="29" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D40" s="30"/>
       <c r="E40" s="30"/>
@@ -4141,7 +4244,7 @@
         <v>38</v>
       </c>
       <c r="C42" s="29" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D42" s="30"/>
       <c r="E42" s="30"/>
@@ -4171,7 +4274,7 @@
         <v>40</v>
       </c>
       <c r="C44" s="29" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D44" s="30"/>
       <c r="E44" s="30"/>
@@ -4201,7 +4304,7 @@
         <v>42</v>
       </c>
       <c r="C46" s="29" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D46" s="30"/>
       <c r="E46" s="30"/>
@@ -4231,7 +4334,7 @@
         <v>44</v>
       </c>
       <c r="C48" s="29" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D48" s="30"/>
       <c r="E48" s="30"/>
@@ -4261,7 +4364,7 @@
         <v>46</v>
       </c>
       <c r="C50" s="29" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D50" s="30"/>
       <c r="E50" s="30"/>
@@ -4291,7 +4394,7 @@
         <v>48</v>
       </c>
       <c r="C52" s="29" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D52" s="30"/>
       <c r="E52" s="30"/>
@@ -4321,7 +4424,7 @@
         <v>50</v>
       </c>
       <c r="C54" s="29" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D54" s="30"/>
       <c r="E54" s="30"/>
@@ -4351,7 +4454,7 @@
         <v>52</v>
       </c>
       <c r="C56" s="29" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D56" s="30"/>
       <c r="E56" s="30"/>
@@ -4381,7 +4484,7 @@
         <v>54</v>
       </c>
       <c r="C58" s="29" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D58" s="30"/>
       <c r="E58" s="30"/>
@@ -4411,7 +4514,7 @@
         <v>56</v>
       </c>
       <c r="C60" s="29" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D60" s="30"/>
       <c r="E60" s="30"/>
@@ -4441,7 +4544,7 @@
         <v>58</v>
       </c>
       <c r="C62" s="29" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D62" s="30"/>
       <c r="E62" s="30"/>
@@ -4471,7 +4574,7 @@
         <v>60</v>
       </c>
       <c r="C64" s="29" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D64" s="30"/>
       <c r="E64" s="30"/>
@@ -4501,7 +4604,7 @@
         <v>62</v>
       </c>
       <c r="C66" s="29" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D66" s="30"/>
       <c r="E66" s="30"/>
@@ -4531,7 +4634,7 @@
         <v>64</v>
       </c>
       <c r="C68" s="29" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D68" s="30"/>
       <c r="E68" s="30"/>
@@ -4561,7 +4664,7 @@
         <v>66</v>
       </c>
       <c r="C70" s="29" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D70" s="30"/>
       <c r="E70" s="30"/>
@@ -4591,7 +4694,7 @@
         <v>68</v>
       </c>
       <c r="C72" s="29" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D72" s="30"/>
       <c r="E72" s="30"/>
@@ -4621,7 +4724,7 @@
         <v>70</v>
       </c>
       <c r="C74" s="29" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D74" s="30"/>
       <c r="E74" s="30"/>
@@ -4651,7 +4754,7 @@
         <v>72</v>
       </c>
       <c r="C76" s="29" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D76" s="30"/>
       <c r="E76" s="30"/>
@@ -4681,7 +4784,7 @@
         <v>74</v>
       </c>
       <c r="C78" s="29" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D78" s="30"/>
       <c r="E78" s="30"/>
@@ -4711,7 +4814,7 @@
         <v>76</v>
       </c>
       <c r="C80" s="29" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D80" s="30"/>
       <c r="E80" s="30"/>
@@ -4741,7 +4844,7 @@
         <v>78</v>
       </c>
       <c r="C82" s="29" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D82" s="30"/>
       <c r="E82" s="30"/>
@@ -4771,7 +4874,7 @@
         <v>80</v>
       </c>
       <c r="C84" s="29" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D84" s="30"/>
       <c r="E84" s="30"/>
@@ -4801,7 +4904,7 @@
         <v>82</v>
       </c>
       <c r="C86" s="29" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D86" s="30"/>
       <c r="E86" s="30"/>
@@ -4831,7 +4934,7 @@
         <v>84</v>
       </c>
       <c r="C88" s="29" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D88" s="30"/>
       <c r="E88" s="30"/>
@@ -4861,7 +4964,7 @@
         <v>86</v>
       </c>
       <c r="C90" s="29" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D90" s="30"/>
       <c r="E90" s="30"/>
@@ -4891,7 +4994,7 @@
         <v>88</v>
       </c>
       <c r="C92" s="29" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D92" s="30"/>
       <c r="E92" s="30"/>
@@ -4921,7 +5024,7 @@
         <v>90</v>
       </c>
       <c r="C94" s="29" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D94" s="30"/>
       <c r="E94" s="30"/>
@@ -4951,7 +5054,7 @@
         <v>92</v>
       </c>
       <c r="C96" s="29" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D96" s="30"/>
       <c r="E96" s="30"/>
@@ -4981,7 +5084,7 @@
         <v>94</v>
       </c>
       <c r="C98" s="29" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D98" s="30"/>
       <c r="E98" s="30"/>
@@ -5011,7 +5114,7 @@
         <v>96</v>
       </c>
       <c r="C100" s="29" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D100" s="30"/>
       <c r="E100" s="30"/>
@@ -5041,7 +5144,7 @@
         <v>98</v>
       </c>
       <c r="C102" s="29" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D102" s="30"/>
       <c r="E102" s="30"/>
@@ -5071,7 +5174,7 @@
         <v>100</v>
       </c>
       <c r="C104" s="29" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D104" s="30"/>
       <c r="E104" s="30"/>
@@ -5101,7 +5204,7 @@
         <v>102</v>
       </c>
       <c r="C106" s="29" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D106" s="30"/>
       <c r="E106" s="30"/>
@@ -5131,7 +5234,7 @@
         <v>104</v>
       </c>
       <c r="C108" s="29" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D108" s="30"/>
       <c r="E108" s="30"/>
@@ -5161,7 +5264,7 @@
         <v>106</v>
       </c>
       <c r="C110" s="29" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D110" s="30"/>
       <c r="E110" s="30"/>
@@ -5191,7 +5294,7 @@
         <v>108</v>
       </c>
       <c r="C112" s="29" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D112" s="30"/>
       <c r="E112" s="30"/>
@@ -5221,7 +5324,7 @@
         <v>110</v>
       </c>
       <c r="C114" s="29" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D114" s="30"/>
       <c r="E114" s="30"/>
@@ -5251,7 +5354,7 @@
         <v>112</v>
       </c>
       <c r="C116" s="29" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D116" s="30"/>
       <c r="E116" s="30"/>
@@ -5281,7 +5384,7 @@
         <v>114</v>
       </c>
       <c r="C118" s="29" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D118" s="30"/>
       <c r="E118" s="30"/>
@@ -5311,7 +5414,7 @@
         <v>116</v>
       </c>
       <c r="C120" s="29" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D120" s="30"/>
       <c r="E120" s="30"/>
@@ -5341,7 +5444,7 @@
         <v>118</v>
       </c>
       <c r="C122" s="29" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D122" s="30"/>
       <c r="E122" s="30"/>
@@ -5371,7 +5474,7 @@
         <v>120</v>
       </c>
       <c r="C124" s="29" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D124" s="30"/>
       <c r="E124" s="30"/>
@@ -5401,7 +5504,7 @@
         <v>122</v>
       </c>
       <c r="C126" s="29" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D126" s="30"/>
       <c r="E126" s="30"/>
@@ -5431,7 +5534,7 @@
         <v>124</v>
       </c>
       <c r="C128" s="29" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D128" s="30"/>
       <c r="E128" s="30"/>
@@ -5460,106 +5563,52 @@
       <c r="B130" s="2">
         <v>126</v>
       </c>
-      <c r="C130" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="D130" s="28"/>
-      <c r="E130" s="28"/>
-      <c r="F130" s="28"/>
-      <c r="G130" s="28"/>
-      <c r="H130" s="28"/>
-      <c r="I130" s="28"/>
-      <c r="J130" s="28"/>
+      <c r="C130" s="35" t="s">
+        <v>104</v>
+      </c>
+      <c r="D130" s="35"/>
+      <c r="E130" s="35"/>
+      <c r="F130" s="35"/>
+      <c r="G130" s="35"/>
+      <c r="H130" s="35"/>
+      <c r="I130" s="35"/>
+      <c r="J130" s="35"/>
       <c r="K130" s="2"/>
     </row>
     <row r="131" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B131" s="2">
         <v>127</v>
       </c>
-      <c r="C131" s="28" t="s">
-        <v>105</v>
-      </c>
-      <c r="D131" s="28"/>
-      <c r="E131" s="28"/>
-      <c r="F131" s="28"/>
-      <c r="G131" s="28"/>
-      <c r="H131" s="28"/>
-      <c r="I131" s="28"/>
-      <c r="J131" s="28"/>
+      <c r="C131" s="35" t="s">
+        <v>103</v>
+      </c>
+      <c r="D131" s="35"/>
+      <c r="E131" s="35"/>
+      <c r="F131" s="35"/>
+      <c r="G131" s="35"/>
+      <c r="H131" s="35"/>
+      <c r="I131" s="35"/>
+      <c r="J131" s="35"/>
       <c r="K131" s="2"/>
     </row>
     <row r="132" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B132" s="2">
         <v>128</v>
       </c>
-      <c r="C132" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="D132" s="28"/>
-      <c r="E132" s="28"/>
-      <c r="F132" s="28"/>
-      <c r="G132" s="28"/>
-      <c r="H132" s="28"/>
-      <c r="I132" s="28"/>
-      <c r="J132" s="28"/>
+      <c r="C132" s="35" t="s">
+        <v>105</v>
+      </c>
+      <c r="D132" s="35"/>
+      <c r="E132" s="35"/>
+      <c r="F132" s="35"/>
+      <c r="G132" s="35"/>
+      <c r="H132" s="35"/>
+      <c r="I132" s="35"/>
+      <c r="J132" s="35"/>
       <c r="K132" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="70">
-    <mergeCell ref="C128:J129"/>
-    <mergeCell ref="C116:J117"/>
-    <mergeCell ref="C118:J119"/>
-    <mergeCell ref="C120:J121"/>
-    <mergeCell ref="C122:J123"/>
-    <mergeCell ref="C124:J125"/>
-    <mergeCell ref="C126:J127"/>
-    <mergeCell ref="C114:J115"/>
-    <mergeCell ref="C92:J93"/>
-    <mergeCell ref="C94:J95"/>
-    <mergeCell ref="C96:J97"/>
-    <mergeCell ref="C98:J99"/>
-    <mergeCell ref="C100:J101"/>
-    <mergeCell ref="C102:J103"/>
-    <mergeCell ref="C104:J105"/>
-    <mergeCell ref="C106:J107"/>
-    <mergeCell ref="C108:J109"/>
-    <mergeCell ref="C110:J111"/>
-    <mergeCell ref="C112:J113"/>
-    <mergeCell ref="C90:J91"/>
-    <mergeCell ref="C68:J69"/>
-    <mergeCell ref="C70:J71"/>
-    <mergeCell ref="C72:J73"/>
-    <mergeCell ref="C74:J75"/>
-    <mergeCell ref="C76:J77"/>
-    <mergeCell ref="C78:J79"/>
-    <mergeCell ref="C80:J81"/>
-    <mergeCell ref="C82:J83"/>
-    <mergeCell ref="C84:J85"/>
-    <mergeCell ref="C86:J87"/>
-    <mergeCell ref="C88:J89"/>
-    <mergeCell ref="C40:J41"/>
-    <mergeCell ref="C66:J67"/>
-    <mergeCell ref="C44:J45"/>
-    <mergeCell ref="C46:J47"/>
-    <mergeCell ref="C48:J49"/>
-    <mergeCell ref="C50:J51"/>
-    <mergeCell ref="C52:J53"/>
-    <mergeCell ref="C54:J55"/>
-    <mergeCell ref="C56:J57"/>
-    <mergeCell ref="C58:J59"/>
-    <mergeCell ref="C60:J61"/>
-    <mergeCell ref="C62:J63"/>
-    <mergeCell ref="C64:J65"/>
-    <mergeCell ref="C30:J31"/>
-    <mergeCell ref="C32:J33"/>
-    <mergeCell ref="C34:J35"/>
-    <mergeCell ref="C36:J37"/>
-    <mergeCell ref="C38:J39"/>
-    <mergeCell ref="R2:T2"/>
-    <mergeCell ref="C4:J4"/>
-    <mergeCell ref="C5:J6"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="C7:J7"/>
     <mergeCell ref="C130:J130"/>
     <mergeCell ref="C131:J131"/>
     <mergeCell ref="C132:J132"/>
@@ -5576,6 +5625,60 @@
     <mergeCell ref="C24:J25"/>
     <mergeCell ref="C26:J27"/>
     <mergeCell ref="C28:J29"/>
+    <mergeCell ref="R2:T2"/>
+    <mergeCell ref="C4:J4"/>
+    <mergeCell ref="C5:J6"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="C7:J7"/>
+    <mergeCell ref="C30:J31"/>
+    <mergeCell ref="C32:J33"/>
+    <mergeCell ref="C34:J35"/>
+    <mergeCell ref="C36:J37"/>
+    <mergeCell ref="C38:J39"/>
+    <mergeCell ref="C40:J41"/>
+    <mergeCell ref="C66:J67"/>
+    <mergeCell ref="C44:J45"/>
+    <mergeCell ref="C46:J47"/>
+    <mergeCell ref="C48:J49"/>
+    <mergeCell ref="C50:J51"/>
+    <mergeCell ref="C52:J53"/>
+    <mergeCell ref="C54:J55"/>
+    <mergeCell ref="C56:J57"/>
+    <mergeCell ref="C58:J59"/>
+    <mergeCell ref="C60:J61"/>
+    <mergeCell ref="C62:J63"/>
+    <mergeCell ref="C64:J65"/>
+    <mergeCell ref="C90:J91"/>
+    <mergeCell ref="C68:J69"/>
+    <mergeCell ref="C70:J71"/>
+    <mergeCell ref="C72:J73"/>
+    <mergeCell ref="C74:J75"/>
+    <mergeCell ref="C76:J77"/>
+    <mergeCell ref="C78:J79"/>
+    <mergeCell ref="C80:J81"/>
+    <mergeCell ref="C82:J83"/>
+    <mergeCell ref="C84:J85"/>
+    <mergeCell ref="C86:J87"/>
+    <mergeCell ref="C88:J89"/>
+    <mergeCell ref="C114:J115"/>
+    <mergeCell ref="C92:J93"/>
+    <mergeCell ref="C94:J95"/>
+    <mergeCell ref="C96:J97"/>
+    <mergeCell ref="C98:J99"/>
+    <mergeCell ref="C100:J101"/>
+    <mergeCell ref="C102:J103"/>
+    <mergeCell ref="C104:J105"/>
+    <mergeCell ref="C106:J107"/>
+    <mergeCell ref="C108:J109"/>
+    <mergeCell ref="C110:J111"/>
+    <mergeCell ref="C112:J113"/>
+    <mergeCell ref="C128:J129"/>
+    <mergeCell ref="C116:J117"/>
+    <mergeCell ref="C118:J119"/>
+    <mergeCell ref="C120:J121"/>
+    <mergeCell ref="C122:J123"/>
+    <mergeCell ref="C124:J125"/>
+    <mergeCell ref="C126:J127"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5589,7 +5692,7 @@
   </sheetPr>
   <dimension ref="B2:T24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8:J8"/>
     </sheetView>
   </sheetViews>
@@ -5608,18 +5711,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="N2" s="13" t="str">
+      <c r="N2" s="14" t="str">
         <f>Type!C2</f>
         <v>Server -&gt; Client</v>
       </c>
-      <c r="O2" s="13"/>
-      <c r="P2" s="13"/>
-      <c r="R2" s="13" t="str">
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
+      <c r="R2" s="14" t="str">
         <f>Type!G2</f>
         <v>Client -&gt; Server</v>
       </c>
-      <c r="S2" s="13"/>
-      <c r="T2" s="13"/>
+      <c r="S2" s="14"/>
+      <c r="T2" s="14"/>
     </row>
     <row r="3" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="10" t="s">
@@ -5681,16 +5784,16 @@
       <c r="B4" s="9">
         <v>0</v>
       </c>
-      <c r="C4" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
+      <c r="C4" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
       <c r="K4" s="9" t="s">
         <v>11</v>
       </c>
@@ -5723,17 +5826,17 @@
       <c r="B5" s="9">
         <v>1</v>
       </c>
-      <c r="C5" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="23"/>
+      <c r="C5" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="24"/>
       <c r="N5" s="11" t="str">
         <f>IF(ISBLANK(Type!C5),"",Type!C5)</f>
         <v>0x02</v>
@@ -5763,15 +5866,15 @@
       <c r="B6" s="9">
         <v>2</v>
       </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="24"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="25"/>
       <c r="N6" s="11" t="str">
         <f>IF(ISBLANK(Type!C6),"",Type!C6)</f>
         <v>0x03</v>
@@ -5801,16 +5904,16 @@
       <c r="B7" s="9">
         <v>3</v>
       </c>
-      <c r="C7" s="20" t="s">
-        <v>111</v>
-      </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="21"/>
-      <c r="J7" s="22"/>
+      <c r="C7" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="23"/>
       <c r="K7" s="5"/>
       <c r="N7" s="11" t="str">
         <f>IF(ISBLANK(Type!C7),"",Type!C7)</f>
@@ -5841,16 +5944,16 @@
       <c r="B8" s="11">
         <v>4</v>
       </c>
-      <c r="C8" s="25" t="s">
-        <v>109</v>
-      </c>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="27"/>
+      <c r="C8" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="28"/>
       <c r="K8" s="11"/>
       <c r="N8" s="11" t="str">
         <f>IF(ISBLANK(Type!C8),"",Type!C8)</f>
@@ -5936,7 +6039,7 @@
       </c>
       <c r="O11" s="11" t="str">
         <f>IF(ISBLANK(Type!D11),"",Type!D11)</f>
-        <v>Enter Game Room</v>
+        <v>Make Game Room</v>
       </c>
       <c r="P11" s="11" t="str">
         <f>IF(ISBLANK(Type!E11),"",Type!E11)</f>
@@ -5948,7 +6051,7 @@
       </c>
       <c r="S11" s="11" t="str">
         <f>IF(ISBLANK(Type!H11),"",Type!H11)</f>
-        <v>Enter Game Room</v>
+        <v>Make Game Room</v>
       </c>
       <c r="T11" s="11" t="str">
         <f>IF(ISBLANK(Type!I11),"",Type!I11)</f>
@@ -5962,7 +6065,7 @@
       </c>
       <c r="O12" s="11" t="str">
         <f>IF(ISBLANK(Type!D12),"",Type!D12)</f>
-        <v>Escape Game Room</v>
+        <v>Enter Game Room</v>
       </c>
       <c r="P12" s="11" t="str">
         <f>IF(ISBLANK(Type!E12),"",Type!E12)</f>
@@ -5974,7 +6077,7 @@
       </c>
       <c r="S12" s="11" t="str">
         <f>IF(ISBLANK(Type!H12),"",Type!H12)</f>
-        <v>Escape Game Room</v>
+        <v>Enter Game Room</v>
       </c>
       <c r="T12" s="11" t="str">
         <f>IF(ISBLANK(Type!I12),"",Type!I12)</f>
@@ -5988,7 +6091,7 @@
       </c>
       <c r="O13" s="11" t="str">
         <f>IF(ISBLANK(Type!D13),"",Type!D13)</f>
-        <v>Heart Beat</v>
+        <v>Escape Game Room</v>
       </c>
       <c r="P13" s="11" t="str">
         <f>IF(ISBLANK(Type!E13),"",Type!E13)</f>
@@ -6000,7 +6103,7 @@
       </c>
       <c r="S13" s="11" t="str">
         <f>IF(ISBLANK(Type!H13),"",Type!H13)</f>
-        <v>Heart Beat</v>
+        <v>Escape Game Room</v>
       </c>
       <c r="T13" s="11" t="str">
         <f>IF(ISBLANK(Type!I13),"",Type!I13)</f>
@@ -6014,11 +6117,11 @@
       </c>
       <c r="O14" s="11" t="str">
         <f>IF(ISBLANK(Type!D14),"",Type!D14)</f>
-        <v>In Game Whole Data</v>
-      </c>
-      <c r="P14" s="11">
+        <v>Heart Beat</v>
+      </c>
+      <c r="P14" s="11" t="str">
         <f>IF(ISBLANK(Type!E14),"",Type!E14)</f>
-        <v>1300</v>
+        <v/>
       </c>
       <c r="R14" s="11" t="str">
         <f>IF(ISBLANK(Type!G14),"",Type!G14)</f>
@@ -6026,37 +6129,37 @@
       </c>
       <c r="S14" s="11" t="str">
         <f>IF(ISBLANK(Type!H14),"",Type!H14)</f>
-        <v>In Game My Data</v>
-      </c>
-      <c r="T14" s="11">
+        <v>Heart Beat</v>
+      </c>
+      <c r="T14" s="11" t="str">
         <f>IF(ISBLANK(Type!I14),"",Type!I14)</f>
-        <v>300</v>
+        <v/>
       </c>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.3">
       <c r="N15" s="11" t="str">
         <f>IF(ISBLANK(Type!C15),"",Type!C15)</f>
-        <v/>
+        <v>0x0C</v>
       </c>
       <c r="O15" s="11" t="str">
         <f>IF(ISBLANK(Type!D15),"",Type!D15)</f>
-        <v/>
-      </c>
-      <c r="P15" s="11" t="str">
+        <v>In Game Data</v>
+      </c>
+      <c r="P15" s="11">
         <f>IF(ISBLANK(Type!E15),"",Type!E15)</f>
-        <v/>
+        <v>1300</v>
       </c>
       <c r="R15" s="11" t="str">
         <f>IF(ISBLANK(Type!G15),"",Type!G15)</f>
-        <v/>
+        <v>0x0C</v>
       </c>
       <c r="S15" s="11" t="str">
         <f>IF(ISBLANK(Type!H15),"",Type!H15)</f>
-        <v/>
-      </c>
-      <c r="T15" s="11" t="str">
+        <v>In Game Data</v>
+      </c>
+      <c r="T15" s="11">
         <f>IF(ISBLANK(Type!I15),"",Type!I15)</f>
-        <v/>
+        <v>300</v>
       </c>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.3">
@@ -6335,18 +6438,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="N2" s="13" t="str">
+      <c r="N2" s="14" t="str">
         <f>Type!C2</f>
         <v>Server -&gt; Client</v>
       </c>
-      <c r="O2" s="13"/>
-      <c r="P2" s="13"/>
-      <c r="R2" s="13" t="str">
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
+      <c r="R2" s="14" t="str">
         <f>Type!G2</f>
         <v>Client -&gt; Server</v>
       </c>
-      <c r="S2" s="13"/>
-      <c r="T2" s="13"/>
+      <c r="S2" s="14"/>
+      <c r="T2" s="14"/>
     </row>
     <row r="3" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="10" t="s">
@@ -6408,16 +6511,16 @@
       <c r="B4" s="9">
         <v>0</v>
       </c>
-      <c r="C4" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
+      <c r="C4" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
       <c r="K4" s="9" t="s">
         <v>11</v>
       </c>
@@ -6450,17 +6553,17 @@
       <c r="B5" s="9">
         <v>1</v>
       </c>
-      <c r="C5" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="23"/>
+      <c r="C5" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="24"/>
       <c r="N5" s="11" t="str">
         <f>IF(ISBLANK(Type!C5),"",Type!C5)</f>
         <v>0x02</v>
@@ -6490,15 +6593,15 @@
       <c r="B6" s="9">
         <v>2</v>
       </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="24"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="25"/>
       <c r="N6" s="11" t="str">
         <f>IF(ISBLANK(Type!C6),"",Type!C6)</f>
         <v>0x03</v>
@@ -6528,16 +6631,16 @@
       <c r="B7" s="9">
         <v>3</v>
       </c>
-      <c r="C7" s="20" t="s">
-        <v>110</v>
-      </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="21"/>
-      <c r="J7" s="22"/>
+      <c r="C7" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="23"/>
       <c r="K7" s="5"/>
       <c r="N7" s="11" t="str">
         <f>IF(ISBLANK(Type!C7),"",Type!C7)</f>
@@ -6569,7 +6672,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D8" s="30"/>
       <c r="E8" s="30"/>
@@ -6647,7 +6750,7 @@
         <v>6</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D10" s="30"/>
       <c r="E10" s="30"/>
@@ -6701,7 +6804,7 @@
       </c>
       <c r="O11" s="11" t="str">
         <f>IF(ISBLANK(Type!D11),"",Type!D11)</f>
-        <v>Enter Game Room</v>
+        <v>Make Game Room</v>
       </c>
       <c r="P11" s="11" t="str">
         <f>IF(ISBLANK(Type!E11),"",Type!E11)</f>
@@ -6713,7 +6816,7 @@
       </c>
       <c r="S11" s="11" t="str">
         <f>IF(ISBLANK(Type!H11),"",Type!H11)</f>
-        <v>Enter Game Room</v>
+        <v>Make Game Room</v>
       </c>
       <c r="T11" s="11" t="str">
         <f>IF(ISBLANK(Type!I11),"",Type!I11)</f>
@@ -6725,7 +6828,7 @@
         <v>8</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D12" s="30"/>
       <c r="E12" s="30"/>
@@ -6741,7 +6844,7 @@
       </c>
       <c r="O12" s="11" t="str">
         <f>IF(ISBLANK(Type!D12),"",Type!D12)</f>
-        <v>Escape Game Room</v>
+        <v>Enter Game Room</v>
       </c>
       <c r="P12" s="11" t="str">
         <f>IF(ISBLANK(Type!E12),"",Type!E12)</f>
@@ -6753,7 +6856,7 @@
       </c>
       <c r="S12" s="11" t="str">
         <f>IF(ISBLANK(Type!H12),"",Type!H12)</f>
-        <v>Escape Game Room</v>
+        <v>Enter Game Room</v>
       </c>
       <c r="T12" s="11" t="str">
         <f>IF(ISBLANK(Type!I12),"",Type!I12)</f>
@@ -6779,7 +6882,7 @@
       </c>
       <c r="O13" s="11" t="str">
         <f>IF(ISBLANK(Type!D13),"",Type!D13)</f>
-        <v>Heart Beat</v>
+        <v>Escape Game Room</v>
       </c>
       <c r="P13" s="11" t="str">
         <f>IF(ISBLANK(Type!E13),"",Type!E13)</f>
@@ -6791,7 +6894,7 @@
       </c>
       <c r="S13" s="11" t="str">
         <f>IF(ISBLANK(Type!H13),"",Type!H13)</f>
-        <v>Heart Beat</v>
+        <v>Escape Game Room</v>
       </c>
       <c r="T13" s="11" t="str">
         <f>IF(ISBLANK(Type!I13),"",Type!I13)</f>
@@ -6803,7 +6906,7 @@
         <v>10</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D14" s="30"/>
       <c r="E14" s="30"/>
@@ -6819,11 +6922,11 @@
       </c>
       <c r="O14" s="11" t="str">
         <f>IF(ISBLANK(Type!D14),"",Type!D14)</f>
-        <v>In Game Whole Data</v>
-      </c>
-      <c r="P14" s="11">
+        <v>Heart Beat</v>
+      </c>
+      <c r="P14" s="11" t="str">
         <f>IF(ISBLANK(Type!E14),"",Type!E14)</f>
-        <v>1300</v>
+        <v/>
       </c>
       <c r="R14" s="11" t="str">
         <f>IF(ISBLANK(Type!G14),"",Type!G14)</f>
@@ -6831,11 +6934,11 @@
       </c>
       <c r="S14" s="11" t="str">
         <f>IF(ISBLANK(Type!H14),"",Type!H14)</f>
-        <v>In Game My Data</v>
-      </c>
-      <c r="T14" s="11">
+        <v>Heart Beat</v>
+      </c>
+      <c r="T14" s="11" t="str">
         <f>IF(ISBLANK(Type!I14),"",Type!I14)</f>
-        <v>300</v>
+        <v/>
       </c>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.3">
@@ -6853,27 +6956,27 @@
       <c r="K15" s="11"/>
       <c r="N15" s="11" t="str">
         <f>IF(ISBLANK(Type!C15),"",Type!C15)</f>
-        <v/>
+        <v>0x0C</v>
       </c>
       <c r="O15" s="11" t="str">
         <f>IF(ISBLANK(Type!D15),"",Type!D15)</f>
-        <v/>
-      </c>
-      <c r="P15" s="11" t="str">
+        <v>In Game Data</v>
+      </c>
+      <c r="P15" s="11">
         <f>IF(ISBLANK(Type!E15),"",Type!E15)</f>
-        <v/>
+        <v>1300</v>
       </c>
       <c r="R15" s="11" t="str">
         <f>IF(ISBLANK(Type!G15),"",Type!G15)</f>
-        <v/>
+        <v>0x0C</v>
       </c>
       <c r="S15" s="11" t="str">
         <f>IF(ISBLANK(Type!H15),"",Type!H15)</f>
-        <v/>
-      </c>
-      <c r="T15" s="11" t="str">
+        <v>In Game Data</v>
+      </c>
+      <c r="T15" s="11">
         <f>IF(ISBLANK(Type!I15),"",Type!I15)</f>
-        <v/>
+        <v>300</v>
       </c>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.3">
@@ -6881,7 +6984,7 @@
         <v>12</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D16" s="30"/>
       <c r="E16" s="30"/>
@@ -6959,7 +7062,7 @@
         <v>14</v>
       </c>
       <c r="C18" s="29" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D18" s="30"/>
       <c r="E18" s="30"/>
@@ -7037,7 +7140,7 @@
         <v>16</v>
       </c>
       <c r="C20" s="29" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D20" s="30"/>
       <c r="E20" s="30"/>
@@ -7115,7 +7218,7 @@
         <v>18</v>
       </c>
       <c r="C22" s="29" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D22" s="30"/>
       <c r="E22" s="30"/>
@@ -7193,7 +7296,7 @@
         <v>20</v>
       </c>
       <c r="C24" s="29" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D24" s="30"/>
       <c r="E24" s="30"/>
@@ -7247,7 +7350,7 @@
         <v>22</v>
       </c>
       <c r="C26" s="29" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D26" s="30"/>
       <c r="E26" s="30"/>
@@ -7277,7 +7380,7 @@
         <v>24</v>
       </c>
       <c r="C28" s="29" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D28" s="30"/>
       <c r="E28" s="30"/>
@@ -7307,7 +7410,7 @@
         <v>26</v>
       </c>
       <c r="C30" s="29" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D30" s="30"/>
       <c r="E30" s="30"/>
@@ -7337,7 +7440,7 @@
         <v>28</v>
       </c>
       <c r="C32" s="29" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D32" s="30"/>
       <c r="E32" s="30"/>
@@ -7367,7 +7470,7 @@
         <v>30</v>
       </c>
       <c r="C34" s="29" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D34" s="30"/>
       <c r="E34" s="30"/>
@@ -7397,7 +7500,7 @@
         <v>32</v>
       </c>
       <c r="C36" s="29" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D36" s="30"/>
       <c r="E36" s="30"/>
@@ -7427,7 +7530,7 @@
         <v>34</v>
       </c>
       <c r="C38" s="29" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D38" s="30"/>
       <c r="E38" s="30"/>
@@ -7457,7 +7560,7 @@
         <v>36</v>
       </c>
       <c r="C40" s="29" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D40" s="30"/>
       <c r="E40" s="30"/>
@@ -7487,7 +7590,7 @@
         <v>38</v>
       </c>
       <c r="C42" s="29" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D42" s="30"/>
       <c r="E42" s="30"/>
@@ -7517,7 +7620,7 @@
         <v>40</v>
       </c>
       <c r="C44" s="29" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D44" s="30"/>
       <c r="E44" s="30"/>
@@ -7547,7 +7650,7 @@
         <v>42</v>
       </c>
       <c r="C46" s="29" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D46" s="30"/>
       <c r="E46" s="30"/>
@@ -7577,7 +7680,7 @@
         <v>44</v>
       </c>
       <c r="C48" s="29" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D48" s="30"/>
       <c r="E48" s="30"/>
@@ -7607,7 +7710,7 @@
         <v>46</v>
       </c>
       <c r="C50" s="29" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D50" s="30"/>
       <c r="E50" s="30"/>
@@ -7637,7 +7740,7 @@
         <v>48</v>
       </c>
       <c r="C52" s="29" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D52" s="30"/>
       <c r="E52" s="30"/>
@@ -7667,7 +7770,7 @@
         <v>50</v>
       </c>
       <c r="C54" s="29" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D54" s="30"/>
       <c r="E54" s="30"/>
@@ -7697,7 +7800,7 @@
         <v>52</v>
       </c>
       <c r="C56" s="29" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D56" s="30"/>
       <c r="E56" s="30"/>
@@ -7727,7 +7830,7 @@
         <v>54</v>
       </c>
       <c r="C58" s="29" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D58" s="30"/>
       <c r="E58" s="30"/>
@@ -7757,7 +7860,7 @@
         <v>56</v>
       </c>
       <c r="C60" s="29" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D60" s="30"/>
       <c r="E60" s="30"/>
@@ -7787,7 +7890,7 @@
         <v>58</v>
       </c>
       <c r="C62" s="29" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D62" s="30"/>
       <c r="E62" s="30"/>
@@ -7817,7 +7920,7 @@
         <v>60</v>
       </c>
       <c r="C64" s="29" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D64" s="30"/>
       <c r="E64" s="30"/>
@@ -7847,7 +7950,7 @@
         <v>62</v>
       </c>
       <c r="C66" s="29" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D66" s="30"/>
       <c r="E66" s="30"/>
@@ -7877,7 +7980,7 @@
         <v>64</v>
       </c>
       <c r="C68" s="29" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D68" s="30"/>
       <c r="E68" s="30"/>
@@ -7907,7 +8010,7 @@
         <v>66</v>
       </c>
       <c r="C70" s="29" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D70" s="30"/>
       <c r="E70" s="30"/>
@@ -7937,7 +8040,7 @@
         <v>68</v>
       </c>
       <c r="C72" s="29" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D72" s="30"/>
       <c r="E72" s="30"/>
@@ -7967,7 +8070,7 @@
         <v>70</v>
       </c>
       <c r="C74" s="29" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D74" s="30"/>
       <c r="E74" s="30"/>
@@ -7997,7 +8100,7 @@
         <v>72</v>
       </c>
       <c r="C76" s="29" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D76" s="30"/>
       <c r="E76" s="30"/>
@@ -8027,7 +8130,7 @@
         <v>74</v>
       </c>
       <c r="C78" s="29" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D78" s="30"/>
       <c r="E78" s="30"/>
@@ -8057,7 +8160,7 @@
         <v>76</v>
       </c>
       <c r="C80" s="29" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D80" s="30"/>
       <c r="E80" s="30"/>
@@ -8087,7 +8190,7 @@
         <v>78</v>
       </c>
       <c r="C82" s="29" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D82" s="30"/>
       <c r="E82" s="30"/>
@@ -8117,7 +8220,7 @@
         <v>80</v>
       </c>
       <c r="C84" s="29" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D84" s="30"/>
       <c r="E84" s="30"/>
@@ -8147,7 +8250,7 @@
         <v>82</v>
       </c>
       <c r="C86" s="29" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D86" s="30"/>
       <c r="E86" s="30"/>
@@ -8177,7 +8280,7 @@
         <v>84</v>
       </c>
       <c r="C88" s="29" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D88" s="30"/>
       <c r="E88" s="30"/>
@@ -8207,7 +8310,7 @@
         <v>86</v>
       </c>
       <c r="C90" s="29" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D90" s="30"/>
       <c r="E90" s="30"/>
@@ -8237,7 +8340,7 @@
         <v>88</v>
       </c>
       <c r="C92" s="29" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D92" s="30"/>
       <c r="E92" s="30"/>
@@ -8267,7 +8370,7 @@
         <v>90</v>
       </c>
       <c r="C94" s="29" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D94" s="30"/>
       <c r="E94" s="30"/>
@@ -8297,7 +8400,7 @@
         <v>92</v>
       </c>
       <c r="C96" s="29" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D96" s="30"/>
       <c r="E96" s="30"/>
@@ -8327,7 +8430,7 @@
         <v>94</v>
       </c>
       <c r="C98" s="29" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D98" s="30"/>
       <c r="E98" s="30"/>
@@ -8357,7 +8460,7 @@
         <v>96</v>
       </c>
       <c r="C100" s="29" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D100" s="30"/>
       <c r="E100" s="30"/>
@@ -8387,7 +8490,7 @@
         <v>98</v>
       </c>
       <c r="C102" s="29" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D102" s="30"/>
       <c r="E102" s="30"/>
@@ -8417,7 +8520,7 @@
         <v>100</v>
       </c>
       <c r="C104" s="29" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D104" s="30"/>
       <c r="E104" s="30"/>
@@ -8447,7 +8550,7 @@
         <v>102</v>
       </c>
       <c r="C106" s="29" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D106" s="30"/>
       <c r="E106" s="30"/>
@@ -8477,7 +8580,7 @@
         <v>104</v>
       </c>
       <c r="C108" s="29" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D108" s="30"/>
       <c r="E108" s="30"/>
@@ -8507,7 +8610,7 @@
         <v>106</v>
       </c>
       <c r="C110" s="29" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D110" s="30"/>
       <c r="E110" s="30"/>
@@ -8537,7 +8640,7 @@
         <v>108</v>
       </c>
       <c r="C112" s="29" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D112" s="30"/>
       <c r="E112" s="30"/>
@@ -8567,7 +8670,7 @@
         <v>110</v>
       </c>
       <c r="C114" s="29" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D114" s="30"/>
       <c r="E114" s="30"/>
@@ -8597,7 +8700,7 @@
         <v>112</v>
       </c>
       <c r="C116" s="29" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D116" s="30"/>
       <c r="E116" s="30"/>
@@ -8627,7 +8730,7 @@
         <v>114</v>
       </c>
       <c r="C118" s="29" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D118" s="30"/>
       <c r="E118" s="30"/>
@@ -8657,7 +8760,7 @@
         <v>116</v>
       </c>
       <c r="C120" s="29" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D120" s="30"/>
       <c r="E120" s="30"/>
@@ -8687,7 +8790,7 @@
         <v>118</v>
       </c>
       <c r="C122" s="29" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D122" s="30"/>
       <c r="E122" s="30"/>
@@ -8717,7 +8820,7 @@
         <v>120</v>
       </c>
       <c r="C124" s="29" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D124" s="30"/>
       <c r="E124" s="30"/>
@@ -8747,7 +8850,7 @@
         <v>122</v>
       </c>
       <c r="C126" s="29" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D126" s="30"/>
       <c r="E126" s="30"/>
@@ -8777,7 +8880,7 @@
         <v>124</v>
       </c>
       <c r="C128" s="29" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D128" s="30"/>
       <c r="E128" s="30"/>
@@ -8806,52 +8909,112 @@
       <c r="B130" s="11">
         <v>126</v>
       </c>
-      <c r="C130" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="D130" s="28"/>
-      <c r="E130" s="28"/>
-      <c r="F130" s="28"/>
-      <c r="G130" s="28"/>
-      <c r="H130" s="28"/>
-      <c r="I130" s="28"/>
-      <c r="J130" s="28"/>
+      <c r="C130" s="35" t="s">
+        <v>104</v>
+      </c>
+      <c r="D130" s="35"/>
+      <c r="E130" s="35"/>
+      <c r="F130" s="35"/>
+      <c r="G130" s="35"/>
+      <c r="H130" s="35"/>
+      <c r="I130" s="35"/>
+      <c r="J130" s="35"/>
       <c r="K130" s="11"/>
     </row>
     <row r="131" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B131" s="11">
         <v>127</v>
       </c>
-      <c r="C131" s="28" t="s">
-        <v>105</v>
-      </c>
-      <c r="D131" s="28"/>
-      <c r="E131" s="28"/>
-      <c r="F131" s="28"/>
-      <c r="G131" s="28"/>
-      <c r="H131" s="28"/>
-      <c r="I131" s="28"/>
-      <c r="J131" s="28"/>
+      <c r="C131" s="35" t="s">
+        <v>103</v>
+      </c>
+      <c r="D131" s="35"/>
+      <c r="E131" s="35"/>
+      <c r="F131" s="35"/>
+      <c r="G131" s="35"/>
+      <c r="H131" s="35"/>
+      <c r="I131" s="35"/>
+      <c r="J131" s="35"/>
       <c r="K131" s="11"/>
     </row>
     <row r="132" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B132" s="11">
         <v>128</v>
       </c>
-      <c r="C132" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="D132" s="28"/>
-      <c r="E132" s="28"/>
-      <c r="F132" s="28"/>
-      <c r="G132" s="28"/>
-      <c r="H132" s="28"/>
-      <c r="I132" s="28"/>
-      <c r="J132" s="28"/>
+      <c r="C132" s="35" t="s">
+        <v>105</v>
+      </c>
+      <c r="D132" s="35"/>
+      <c r="E132" s="35"/>
+      <c r="F132" s="35"/>
+      <c r="G132" s="35"/>
+      <c r="H132" s="35"/>
+      <c r="I132" s="35"/>
+      <c r="J132" s="35"/>
       <c r="K132" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="70">
+    <mergeCell ref="C18:J19"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="R2:T2"/>
+    <mergeCell ref="C4:J4"/>
+    <mergeCell ref="C5:J6"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="C7:J7"/>
+    <mergeCell ref="C8:J9"/>
+    <mergeCell ref="C10:J11"/>
+    <mergeCell ref="C12:J13"/>
+    <mergeCell ref="C14:J15"/>
+    <mergeCell ref="C16:J17"/>
+    <mergeCell ref="C42:J43"/>
+    <mergeCell ref="C20:J21"/>
+    <mergeCell ref="C22:J23"/>
+    <mergeCell ref="C24:J25"/>
+    <mergeCell ref="C26:J27"/>
+    <mergeCell ref="C28:J29"/>
+    <mergeCell ref="C30:J31"/>
+    <mergeCell ref="C32:J33"/>
+    <mergeCell ref="C34:J35"/>
+    <mergeCell ref="C36:J37"/>
+    <mergeCell ref="C38:J39"/>
+    <mergeCell ref="C40:J41"/>
+    <mergeCell ref="C66:J67"/>
+    <mergeCell ref="C44:J45"/>
+    <mergeCell ref="C46:J47"/>
+    <mergeCell ref="C48:J49"/>
+    <mergeCell ref="C50:J51"/>
+    <mergeCell ref="C52:J53"/>
+    <mergeCell ref="C54:J55"/>
+    <mergeCell ref="C56:J57"/>
+    <mergeCell ref="C58:J59"/>
+    <mergeCell ref="C60:J61"/>
+    <mergeCell ref="C62:J63"/>
+    <mergeCell ref="C64:J65"/>
+    <mergeCell ref="C90:J91"/>
+    <mergeCell ref="C68:J69"/>
+    <mergeCell ref="C70:J71"/>
+    <mergeCell ref="C72:J73"/>
+    <mergeCell ref="C74:J75"/>
+    <mergeCell ref="C76:J77"/>
+    <mergeCell ref="C78:J79"/>
+    <mergeCell ref="C80:J81"/>
+    <mergeCell ref="C82:J83"/>
+    <mergeCell ref="C84:J85"/>
+    <mergeCell ref="C86:J87"/>
+    <mergeCell ref="C88:J89"/>
+    <mergeCell ref="C114:J115"/>
+    <mergeCell ref="C92:J93"/>
+    <mergeCell ref="C94:J95"/>
+    <mergeCell ref="C96:J97"/>
+    <mergeCell ref="C98:J99"/>
+    <mergeCell ref="C100:J101"/>
+    <mergeCell ref="C102:J103"/>
+    <mergeCell ref="C104:J105"/>
+    <mergeCell ref="C106:J107"/>
+    <mergeCell ref="C108:J109"/>
+    <mergeCell ref="C110:J111"/>
+    <mergeCell ref="C112:J113"/>
     <mergeCell ref="C128:J129"/>
     <mergeCell ref="C130:J130"/>
     <mergeCell ref="C131:J131"/>
@@ -8862,66 +9025,6 @@
     <mergeCell ref="C122:J123"/>
     <mergeCell ref="C124:J125"/>
     <mergeCell ref="C126:J127"/>
-    <mergeCell ref="C104:J105"/>
-    <mergeCell ref="C106:J107"/>
-    <mergeCell ref="C108:J109"/>
-    <mergeCell ref="C110:J111"/>
-    <mergeCell ref="C112:J113"/>
-    <mergeCell ref="C114:J115"/>
-    <mergeCell ref="C92:J93"/>
-    <mergeCell ref="C94:J95"/>
-    <mergeCell ref="C96:J97"/>
-    <mergeCell ref="C98:J99"/>
-    <mergeCell ref="C100:J101"/>
-    <mergeCell ref="C102:J103"/>
-    <mergeCell ref="C80:J81"/>
-    <mergeCell ref="C82:J83"/>
-    <mergeCell ref="C84:J85"/>
-    <mergeCell ref="C86:J87"/>
-    <mergeCell ref="C88:J89"/>
-    <mergeCell ref="C90:J91"/>
-    <mergeCell ref="C68:J69"/>
-    <mergeCell ref="C70:J71"/>
-    <mergeCell ref="C72:J73"/>
-    <mergeCell ref="C74:J75"/>
-    <mergeCell ref="C76:J77"/>
-    <mergeCell ref="C78:J79"/>
-    <mergeCell ref="C56:J57"/>
-    <mergeCell ref="C58:J59"/>
-    <mergeCell ref="C60:J61"/>
-    <mergeCell ref="C62:J63"/>
-    <mergeCell ref="C64:J65"/>
-    <mergeCell ref="C66:J67"/>
-    <mergeCell ref="C44:J45"/>
-    <mergeCell ref="C46:J47"/>
-    <mergeCell ref="C48:J49"/>
-    <mergeCell ref="C50:J51"/>
-    <mergeCell ref="C52:J53"/>
-    <mergeCell ref="C54:J55"/>
-    <mergeCell ref="C32:J33"/>
-    <mergeCell ref="C34:J35"/>
-    <mergeCell ref="C36:J37"/>
-    <mergeCell ref="C38:J39"/>
-    <mergeCell ref="C40:J41"/>
-    <mergeCell ref="C42:J43"/>
-    <mergeCell ref="C20:J21"/>
-    <mergeCell ref="C22:J23"/>
-    <mergeCell ref="C24:J25"/>
-    <mergeCell ref="C26:J27"/>
-    <mergeCell ref="C28:J29"/>
-    <mergeCell ref="C30:J31"/>
-    <mergeCell ref="C8:J9"/>
-    <mergeCell ref="C10:J11"/>
-    <mergeCell ref="C12:J13"/>
-    <mergeCell ref="C14:J15"/>
-    <mergeCell ref="C16:J17"/>
-    <mergeCell ref="C18:J19"/>
-    <mergeCell ref="N2:P2"/>
-    <mergeCell ref="R2:T2"/>
-    <mergeCell ref="C4:J4"/>
-    <mergeCell ref="C5:J6"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="C7:J7"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[Add] Protocol (Game End Signal)
- 게임 종료에 대한 Signal 추가
- 그리고 기존 내용 일부 수정 ( GameRoom Outside State 에 0이 Empty 고 1이 Waiting, 2 가 게임중 인데, 이게 좀 프로토콜 문서에 제대로 업데이트가 되어 있찌 않았었음)
- CheckGameIsOver() 함수를 추가하여, 게임이 끝났는지를 검사함.
- 이 함수는 단순히 현재 게임이 끝났는지 여부를 bool 값으로 리턴함.
- 또한, 현재 커밋에서는 개인전의 경우에만 적용되도록 함.
- 팀전에는 아직...
- 기존 소스는 일단 주석 처리하였음.
- 다음 커밋에서는 싱글모드에서도 잘 되게 하고, 또한, 플레이어가 (게임도중) 중간에 나갈 경우에도 이 함수를 호출하도록 하자.
- 그나자나.. 게임이 시작되더라도 현재 게임방의 시작 사용자가 몇명인지를 카운트 해야하려나?
- 일단 커밋하자. 끝.

P.S. define 에 주석이 잘못되어 있던 것 수정함 : 0 이 Empty 상태고 1이 Waiting 2 가 Gaming 상태인데 이게 업데이트 되어 있지 않았었음. (이번 커밋에서 프로토콜 문서 수정한 것과 같은 맥락임)
</commit_message>
<xml_diff>
--- a/T_Design.xlsx
+++ b/T_Design.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wave\010_Project\010_Game\Tetris\Server\010_Source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FCC7B8B-57CF-406E-8889-648D7AB7AEEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D1A9E1-7C3C-445A-98C8-63D73B8112E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="926" activeTab="3" xr2:uid="{CBDAA684-FC25-4649-B038-1CECF5D4149C}"/>
+    <workbookView xWindow="-30795" yWindow="2535" windowWidth="28800" windowHeight="14685" tabRatio="926" firstSheet="1" activeTab="13" xr2:uid="{CBDAA684-FC25-4649-B038-1CECF5D4149C}"/>
   </bookViews>
   <sheets>
     <sheet name="VersionInfo(SC)" sheetId="24" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1019" uniqueCount="428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1019" uniqueCount="429">
   <si>
     <t>Byte</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -653,10 +653,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>State (0:Wait, 1:Game)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Room Title
 - Unicode 13 Character
 - 13 * 2 + 2(NULL) = 28 Byte</t>
@@ -1539,6 +1535,14 @@
   </si>
   <si>
     <t>Minor Version</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Game End Signal (1:Game End)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>State (1:Wait, 2:Game)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2623,7 +2627,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="52" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D4" s="52"/>
       <c r="E4" s="52"/>
@@ -2665,7 +2669,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="53" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D5" s="54"/>
       <c r="E5" s="54"/>
@@ -2743,7 +2747,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="61" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D7" s="62"/>
       <c r="E7" s="62"/>
@@ -2783,7 +2787,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="48" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D8" s="49"/>
       <c r="E8" s="49"/>
@@ -2823,7 +2827,7 @@
         <v>5</v>
       </c>
       <c r="C9" s="48" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D9" s="49"/>
       <c r="E9" s="49"/>
@@ -3304,8 +3308,8 @@
   </sheetPr>
   <dimension ref="B2:T58"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13:K40"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9:J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -6181,7 +6185,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="48" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D8" s="49"/>
       <c r="E8" s="49"/>
@@ -8035,8 +8039,8 @@
   </sheetPr>
   <dimension ref="B2:T87"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="C88" sqref="C88"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9:J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -8170,7 +8174,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="53" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D5" s="54"/>
       <c r="E5" s="54"/>
@@ -8288,7 +8292,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="93" t="s">
-        <v>162</v>
+        <v>428</v>
       </c>
       <c r="D8" s="93"/>
       <c r="E8" s="93"/>
@@ -8298,7 +8302,7 @@
       <c r="I8" s="93"/>
       <c r="J8" s="93"/>
       <c r="K8" s="129" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="N8" s="26" t="str">
         <f>IF(ISBLANK(Type!C8),"",Type!C8)</f>
@@ -8370,7 +8374,7 @@
         <v>6</v>
       </c>
       <c r="C10" s="93" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D10" s="93"/>
       <c r="E10" s="93"/>
@@ -8450,7 +8454,7 @@
         <v>8</v>
       </c>
       <c r="C12" s="129" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D12" s="129"/>
       <c r="E12" s="129"/>
@@ -8490,7 +8494,7 @@
         <v>9</v>
       </c>
       <c r="C13" s="129" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D13" s="93"/>
       <c r="E13" s="93"/>
@@ -9172,7 +9176,7 @@
         <v>37</v>
       </c>
       <c r="C41" s="117" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D41" s="117"/>
       <c r="E41" s="117"/>
@@ -9182,7 +9186,7 @@
       <c r="I41" s="117"/>
       <c r="J41" s="117"/>
       <c r="K41" s="118" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="42" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -9190,7 +9194,7 @@
         <v>38</v>
       </c>
       <c r="C42" s="118" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D42" s="118"/>
       <c r="E42" s="118"/>
@@ -9612,7 +9616,7 @@
         <v>68</v>
       </c>
       <c r="C72" s="117" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D72" s="117"/>
       <c r="E72" s="117"/>
@@ -9628,7 +9632,7 @@
         <v>69</v>
       </c>
       <c r="C73" s="117" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D73" s="117"/>
       <c r="E73" s="117"/>
@@ -9644,7 +9648,7 @@
         <v>70</v>
       </c>
       <c r="C74" s="117" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D74" s="117"/>
       <c r="E74" s="117"/>
@@ -9660,7 +9664,7 @@
         <v>71</v>
       </c>
       <c r="C75" s="117" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D75" s="117"/>
       <c r="E75" s="117"/>
@@ -9676,7 +9680,7 @@
         <v>72</v>
       </c>
       <c r="C76" s="117" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D76" s="117"/>
       <c r="E76" s="117"/>
@@ -9692,7 +9696,7 @@
         <v>73</v>
       </c>
       <c r="C77" s="121" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D77" s="122"/>
       <c r="E77" s="122"/>
@@ -9702,7 +9706,7 @@
       <c r="I77" s="122"/>
       <c r="J77" s="123"/>
       <c r="K77" s="127" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="78" spans="2:11" x14ac:dyDescent="0.3">
@@ -9725,7 +9729,7 @@
         <v>109</v>
       </c>
       <c r="C79" s="92" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D79" s="75"/>
       <c r="E79" s="75"/>
@@ -9735,7 +9739,7 @@
       <c r="I79" s="75"/>
       <c r="J79" s="76"/>
       <c r="K79" s="119" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="80" spans="2:11" x14ac:dyDescent="0.3">
@@ -9759,7 +9763,7 @@
         <v>145</v>
       </c>
       <c r="C81" s="121" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D81" s="122"/>
       <c r="E81" s="122"/>
@@ -9769,7 +9773,7 @@
       <c r="I81" s="122"/>
       <c r="J81" s="123"/>
       <c r="K81" s="127" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="82" spans="2:11" x14ac:dyDescent="0.3">
@@ -9793,7 +9797,7 @@
         <v>181</v>
       </c>
       <c r="C83" s="92" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D83" s="75"/>
       <c r="E83" s="75"/>
@@ -9803,7 +9807,7 @@
       <c r="I83" s="75"/>
       <c r="J83" s="76"/>
       <c r="K83" s="119" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="84" spans="2:11" x14ac:dyDescent="0.3">
@@ -9827,7 +9831,7 @@
         <v>217</v>
       </c>
       <c r="C85" s="121" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D85" s="122"/>
       <c r="E85" s="122"/>
@@ -9837,7 +9841,7 @@
       <c r="I85" s="122"/>
       <c r="J85" s="123"/>
       <c r="K85" s="127" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="86" spans="2:11" x14ac:dyDescent="0.3">
@@ -9860,7 +9864,7 @@
         <v>253</v>
       </c>
       <c r="C87" s="114" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D87" s="115"/>
       <c r="E87" s="115"/>
@@ -10132,7 +10136,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="61" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D7" s="62"/>
       <c r="E7" s="62"/>
@@ -10172,7 +10176,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="48" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D8" s="49"/>
       <c r="E8" s="49"/>
@@ -10212,7 +10216,7 @@
         <v>5</v>
       </c>
       <c r="C9" s="48" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D9" s="49"/>
       <c r="E9" s="49"/>
@@ -10874,7 +10878,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="61" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D7" s="62"/>
       <c r="E7" s="62"/>
@@ -10914,7 +10918,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="48" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D8" s="49"/>
       <c r="E8" s="49"/>
@@ -11601,7 +11605,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="61" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D7" s="62"/>
       <c r="E7" s="62"/>
@@ -11641,7 +11645,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="48" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D8" s="49"/>
       <c r="E8" s="49"/>
@@ -12116,7 +12120,7 @@
   <dimension ref="B2:T33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9:J9"/>
+      <selection activeCell="C14" sqref="C14:J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -12250,7 +12254,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="53" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D5" s="54"/>
       <c r="E5" s="54"/>
@@ -12328,7 +12332,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="61" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D7" s="62"/>
       <c r="E7" s="62"/>
@@ -12368,7 +12372,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="48" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D8" s="49"/>
       <c r="E8" s="49"/>
@@ -12408,7 +12412,7 @@
         <v>5</v>
       </c>
       <c r="C9" s="48" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D9" s="49"/>
       <c r="E9" s="49"/>
@@ -12448,7 +12452,7 @@
         <v>6</v>
       </c>
       <c r="C10" s="48" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D10" s="49"/>
       <c r="E10" s="49"/>
@@ -12488,7 +12492,7 @@
         <v>7</v>
       </c>
       <c r="C11" s="48" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D11" s="49"/>
       <c r="E11" s="49"/>
@@ -12528,7 +12532,7 @@
         <v>8</v>
       </c>
       <c r="C12" s="48" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D12" s="49"/>
       <c r="E12" s="49"/>
@@ -12568,7 +12572,7 @@
         <v>9</v>
       </c>
       <c r="C13" s="48" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D13" s="49"/>
       <c r="E13" s="49"/>
@@ -12608,7 +12612,7 @@
         <v>10</v>
       </c>
       <c r="C14" s="48" t="s">
-        <v>59</v>
+        <v>427</v>
       </c>
       <c r="D14" s="49"/>
       <c r="E14" s="49"/>
@@ -13370,7 +13374,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="53" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D5" s="54"/>
       <c r="E5" s="54"/>
@@ -13448,7 +13452,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="61" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D7" s="62"/>
       <c r="E7" s="62"/>
@@ -13488,7 +13492,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="48" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D8" s="49"/>
       <c r="E8" s="49"/>
@@ -13528,7 +13532,7 @@
         <v>5</v>
       </c>
       <c r="C9" s="48" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D9" s="49"/>
       <c r="E9" s="49"/>
@@ -13568,7 +13572,7 @@
         <v>6</v>
       </c>
       <c r="C10" s="48" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D10" s="49"/>
       <c r="E10" s="49"/>
@@ -13608,7 +13612,7 @@
         <v>7</v>
       </c>
       <c r="C11" s="48" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D11" s="49"/>
       <c r="E11" s="49"/>
@@ -13648,7 +13652,7 @@
         <v>8</v>
       </c>
       <c r="C12" s="48" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D12" s="49"/>
       <c r="E12" s="49"/>
@@ -13688,7 +13692,7 @@
         <v>9</v>
       </c>
       <c r="C13" s="48" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D13" s="49"/>
       <c r="E13" s="49"/>
@@ -14448,7 +14452,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="52" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D4" s="52"/>
       <c r="E4" s="52"/>
@@ -14490,7 +14494,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="53" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D5" s="54"/>
       <c r="E5" s="54"/>
@@ -14568,7 +14572,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="61" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D7" s="62"/>
       <c r="E7" s="62"/>
@@ -15201,7 +15205,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="53" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D5" s="54"/>
       <c r="E5" s="54"/>
@@ -15279,7 +15283,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="61" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D7" s="62"/>
       <c r="E7" s="62"/>
@@ -15319,7 +15323,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="48" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D8" s="49"/>
       <c r="E8" s="49"/>
@@ -15559,7 +15563,7 @@
         <v>10</v>
       </c>
       <c r="C14" s="131" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D14" s="132"/>
       <c r="E14" s="132"/>
@@ -15599,7 +15603,7 @@
         <v>11</v>
       </c>
       <c r="C15" s="131" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D15" s="132"/>
       <c r="E15" s="132"/>
@@ -15639,7 +15643,7 @@
         <v>12</v>
       </c>
       <c r="C16" s="131" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D16" s="132"/>
       <c r="E16" s="132"/>
@@ -15679,7 +15683,7 @@
         <v>13</v>
       </c>
       <c r="C17" s="131" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D17" s="132"/>
       <c r="E17" s="132"/>
@@ -15719,7 +15723,7 @@
         <v>14</v>
       </c>
       <c r="C18" s="131" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D18" s="132"/>
       <c r="E18" s="132"/>
@@ -15759,7 +15763,7 @@
         <v>15</v>
       </c>
       <c r="C19" s="131" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D19" s="132"/>
       <c r="E19" s="132"/>
@@ -15799,7 +15803,7 @@
         <v>16</v>
       </c>
       <c r="C20" s="131" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D20" s="132"/>
       <c r="E20" s="132"/>
@@ -15839,7 +15843,7 @@
         <v>17</v>
       </c>
       <c r="C21" s="131" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D21" s="132"/>
       <c r="E21" s="132"/>
@@ -15879,7 +15883,7 @@
         <v>18</v>
       </c>
       <c r="C22" s="131" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D22" s="132"/>
       <c r="E22" s="132"/>
@@ -15919,7 +15923,7 @@
         <v>19</v>
       </c>
       <c r="C23" s="131" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D23" s="132"/>
       <c r="E23" s="132"/>
@@ -15959,7 +15963,7 @@
         <v>20</v>
       </c>
       <c r="C24" s="131" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D24" s="132"/>
       <c r="E24" s="132"/>
@@ -15999,7 +16003,7 @@
         <v>21</v>
       </c>
       <c r="C25" s="131" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D25" s="132"/>
       <c r="E25" s="132"/>
@@ -16015,7 +16019,7 @@
         <v>22</v>
       </c>
       <c r="C26" s="131" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D26" s="132"/>
       <c r="E26" s="132"/>
@@ -16031,7 +16035,7 @@
         <v>23</v>
       </c>
       <c r="C27" s="131" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D27" s="132"/>
       <c r="E27" s="132"/>
@@ -16047,7 +16051,7 @@
         <v>24</v>
       </c>
       <c r="C28" s="131" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D28" s="132"/>
       <c r="E28" s="132"/>
@@ -16063,7 +16067,7 @@
         <v>25</v>
       </c>
       <c r="C29" s="131" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D29" s="132"/>
       <c r="E29" s="132"/>
@@ -16079,7 +16083,7 @@
         <v>26</v>
       </c>
       <c r="C30" s="131" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D30" s="132"/>
       <c r="E30" s="132"/>
@@ -16095,7 +16099,7 @@
         <v>27</v>
       </c>
       <c r="C31" s="131" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D31" s="132"/>
       <c r="E31" s="132"/>
@@ -16111,7 +16115,7 @@
         <v>28</v>
       </c>
       <c r="C32" s="131" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D32" s="132"/>
       <c r="E32" s="132"/>
@@ -16127,7 +16131,7 @@
         <v>29</v>
       </c>
       <c r="C33" s="131" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D33" s="132"/>
       <c r="E33" s="132"/>
@@ -16143,7 +16147,7 @@
         <v>30</v>
       </c>
       <c r="C34" s="71" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D34" s="72"/>
       <c r="E34" s="72"/>
@@ -16159,7 +16163,7 @@
         <v>31</v>
       </c>
       <c r="C35" s="71" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D35" s="72"/>
       <c r="E35" s="72"/>
@@ -16175,7 +16179,7 @@
         <v>32</v>
       </c>
       <c r="C36" s="71" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D36" s="72"/>
       <c r="E36" s="72"/>
@@ -16191,7 +16195,7 @@
         <v>33</v>
       </c>
       <c r="C37" s="71" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D37" s="72"/>
       <c r="E37" s="72"/>
@@ -16207,7 +16211,7 @@
         <v>34</v>
       </c>
       <c r="C38" s="71" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D38" s="72"/>
       <c r="E38" s="72"/>
@@ -16223,7 +16227,7 @@
         <v>35</v>
       </c>
       <c r="C39" s="71" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D39" s="72"/>
       <c r="E39" s="72"/>
@@ -16239,7 +16243,7 @@
         <v>36</v>
       </c>
       <c r="C40" s="71" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D40" s="72"/>
       <c r="E40" s="72"/>
@@ -16255,7 +16259,7 @@
         <v>37</v>
       </c>
       <c r="C41" s="71" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D41" s="72"/>
       <c r="E41" s="72"/>
@@ -16271,7 +16275,7 @@
         <v>38</v>
       </c>
       <c r="C42" s="71" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D42" s="72"/>
       <c r="E42" s="72"/>
@@ -16287,7 +16291,7 @@
         <v>39</v>
       </c>
       <c r="C43" s="71" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D43" s="72"/>
       <c r="E43" s="72"/>
@@ -16303,7 +16307,7 @@
         <v>40</v>
       </c>
       <c r="C44" s="71" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D44" s="72"/>
       <c r="E44" s="72"/>
@@ -16319,7 +16323,7 @@
         <v>41</v>
       </c>
       <c r="C45" s="71" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D45" s="72"/>
       <c r="E45" s="72"/>
@@ -16335,7 +16339,7 @@
         <v>42</v>
       </c>
       <c r="C46" s="71" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D46" s="72"/>
       <c r="E46" s="72"/>
@@ -16351,7 +16355,7 @@
         <v>43</v>
       </c>
       <c r="C47" s="71" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D47" s="72"/>
       <c r="E47" s="72"/>
@@ -16367,7 +16371,7 @@
         <v>44</v>
       </c>
       <c r="C48" s="71" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D48" s="72"/>
       <c r="E48" s="72"/>
@@ -16383,7 +16387,7 @@
         <v>45</v>
       </c>
       <c r="C49" s="71" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D49" s="72"/>
       <c r="E49" s="72"/>
@@ -16399,7 +16403,7 @@
         <v>46</v>
       </c>
       <c r="C50" s="71" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D50" s="72"/>
       <c r="E50" s="72"/>
@@ -16415,7 +16419,7 @@
         <v>47</v>
       </c>
       <c r="C51" s="71" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D51" s="72"/>
       <c r="E51" s="72"/>
@@ -16431,7 +16435,7 @@
         <v>48</v>
       </c>
       <c r="C52" s="71" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D52" s="72"/>
       <c r="E52" s="72"/>
@@ -16447,7 +16451,7 @@
         <v>49</v>
       </c>
       <c r="C53" s="71" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D53" s="72"/>
       <c r="E53" s="72"/>
@@ -16463,7 +16467,7 @@
         <v>50</v>
       </c>
       <c r="C54" s="131" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D54" s="132"/>
       <c r="E54" s="132"/>
@@ -16479,7 +16483,7 @@
         <v>51</v>
       </c>
       <c r="C55" s="131" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D55" s="132"/>
       <c r="E55" s="132"/>
@@ -16495,7 +16499,7 @@
         <v>52</v>
       </c>
       <c r="C56" s="131" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D56" s="132"/>
       <c r="E56" s="132"/>
@@ -16511,7 +16515,7 @@
         <v>53</v>
       </c>
       <c r="C57" s="131" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D57" s="132"/>
       <c r="E57" s="132"/>
@@ -16527,7 +16531,7 @@
         <v>54</v>
       </c>
       <c r="C58" s="131" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D58" s="132"/>
       <c r="E58" s="132"/>
@@ -16543,7 +16547,7 @@
         <v>55</v>
       </c>
       <c r="C59" s="131" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D59" s="132"/>
       <c r="E59" s="132"/>
@@ -16559,7 +16563,7 @@
         <v>56</v>
       </c>
       <c r="C60" s="131" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D60" s="132"/>
       <c r="E60" s="132"/>
@@ -16575,7 +16579,7 @@
         <v>57</v>
       </c>
       <c r="C61" s="131" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D61" s="132"/>
       <c r="E61" s="132"/>
@@ -16591,7 +16595,7 @@
         <v>58</v>
       </c>
       <c r="C62" s="131" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D62" s="132"/>
       <c r="E62" s="132"/>
@@ -16607,7 +16611,7 @@
         <v>59</v>
       </c>
       <c r="C63" s="131" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D63" s="132"/>
       <c r="E63" s="132"/>
@@ -16623,7 +16627,7 @@
         <v>60</v>
       </c>
       <c r="C64" s="131" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D64" s="132"/>
       <c r="E64" s="132"/>
@@ -16639,7 +16643,7 @@
         <v>61</v>
       </c>
       <c r="C65" s="131" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D65" s="132"/>
       <c r="E65" s="132"/>
@@ -16655,7 +16659,7 @@
         <v>62</v>
       </c>
       <c r="C66" s="131" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D66" s="132"/>
       <c r="E66" s="132"/>
@@ -16671,7 +16675,7 @@
         <v>63</v>
       </c>
       <c r="C67" s="131" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D67" s="132"/>
       <c r="E67" s="132"/>
@@ -16687,7 +16691,7 @@
         <v>64</v>
       </c>
       <c r="C68" s="131" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D68" s="132"/>
       <c r="E68" s="132"/>
@@ -16703,7 +16707,7 @@
         <v>65</v>
       </c>
       <c r="C69" s="131" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D69" s="132"/>
       <c r="E69" s="132"/>
@@ -16719,7 +16723,7 @@
         <v>66</v>
       </c>
       <c r="C70" s="131" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D70" s="132"/>
       <c r="E70" s="132"/>
@@ -16735,7 +16739,7 @@
         <v>67</v>
       </c>
       <c r="C71" s="131" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D71" s="132"/>
       <c r="E71" s="132"/>
@@ -16751,7 +16755,7 @@
         <v>68</v>
       </c>
       <c r="C72" s="131" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D72" s="132"/>
       <c r="E72" s="132"/>
@@ -16767,7 +16771,7 @@
         <v>69</v>
       </c>
       <c r="C73" s="131" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D73" s="132"/>
       <c r="E73" s="132"/>
@@ -16783,7 +16787,7 @@
         <v>70</v>
       </c>
       <c r="C74" s="71" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D74" s="72"/>
       <c r="E74" s="72"/>
@@ -16799,7 +16803,7 @@
         <v>71</v>
       </c>
       <c r="C75" s="71" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D75" s="72"/>
       <c r="E75" s="72"/>
@@ -16815,7 +16819,7 @@
         <v>72</v>
       </c>
       <c r="C76" s="71" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D76" s="72"/>
       <c r="E76" s="72"/>
@@ -16831,7 +16835,7 @@
         <v>73</v>
       </c>
       <c r="C77" s="71" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D77" s="72"/>
       <c r="E77" s="72"/>
@@ -16847,7 +16851,7 @@
         <v>74</v>
       </c>
       <c r="C78" s="71" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D78" s="72"/>
       <c r="E78" s="72"/>
@@ -16863,7 +16867,7 @@
         <v>75</v>
       </c>
       <c r="C79" s="71" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D79" s="72"/>
       <c r="E79" s="72"/>
@@ -16879,7 +16883,7 @@
         <v>76</v>
       </c>
       <c r="C80" s="71" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D80" s="72"/>
       <c r="E80" s="72"/>
@@ -16895,7 +16899,7 @@
         <v>77</v>
       </c>
       <c r="C81" s="71" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D81" s="72"/>
       <c r="E81" s="72"/>
@@ -16911,7 +16915,7 @@
         <v>78</v>
       </c>
       <c r="C82" s="71" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D82" s="72"/>
       <c r="E82" s="72"/>
@@ -16927,7 +16931,7 @@
         <v>79</v>
       </c>
       <c r="C83" s="71" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D83" s="72"/>
       <c r="E83" s="72"/>
@@ -16943,7 +16947,7 @@
         <v>80</v>
       </c>
       <c r="C84" s="71" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D84" s="72"/>
       <c r="E84" s="72"/>
@@ -16959,7 +16963,7 @@
         <v>81</v>
       </c>
       <c r="C85" s="71" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D85" s="72"/>
       <c r="E85" s="72"/>
@@ -16975,7 +16979,7 @@
         <v>82</v>
       </c>
       <c r="C86" s="71" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D86" s="72"/>
       <c r="E86" s="72"/>
@@ -16991,7 +16995,7 @@
         <v>83</v>
       </c>
       <c r="C87" s="71" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D87" s="72"/>
       <c r="E87" s="72"/>
@@ -17007,7 +17011,7 @@
         <v>84</v>
       </c>
       <c r="C88" s="71" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D88" s="72"/>
       <c r="E88" s="72"/>
@@ -17023,7 +17027,7 @@
         <v>85</v>
       </c>
       <c r="C89" s="71" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D89" s="72"/>
       <c r="E89" s="72"/>
@@ -17039,7 +17043,7 @@
         <v>86</v>
       </c>
       <c r="C90" s="71" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D90" s="72"/>
       <c r="E90" s="72"/>
@@ -17055,7 +17059,7 @@
         <v>87</v>
       </c>
       <c r="C91" s="71" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D91" s="72"/>
       <c r="E91" s="72"/>
@@ -17071,7 +17075,7 @@
         <v>88</v>
       </c>
       <c r="C92" s="71" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D92" s="72"/>
       <c r="E92" s="72"/>
@@ -17087,7 +17091,7 @@
         <v>89</v>
       </c>
       <c r="C93" s="71" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D93" s="72"/>
       <c r="E93" s="72"/>
@@ -17103,7 +17107,7 @@
         <v>90</v>
       </c>
       <c r="C94" s="131" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D94" s="132"/>
       <c r="E94" s="132"/>
@@ -17119,7 +17123,7 @@
         <v>91</v>
       </c>
       <c r="C95" s="131" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D95" s="132"/>
       <c r="E95" s="132"/>
@@ -17135,7 +17139,7 @@
         <v>92</v>
       </c>
       <c r="C96" s="131" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D96" s="132"/>
       <c r="E96" s="132"/>
@@ -17151,7 +17155,7 @@
         <v>93</v>
       </c>
       <c r="C97" s="131" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D97" s="132"/>
       <c r="E97" s="132"/>
@@ -17167,7 +17171,7 @@
         <v>94</v>
       </c>
       <c r="C98" s="131" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D98" s="132"/>
       <c r="E98" s="132"/>
@@ -17183,7 +17187,7 @@
         <v>95</v>
       </c>
       <c r="C99" s="131" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D99" s="132"/>
       <c r="E99" s="132"/>
@@ -17199,7 +17203,7 @@
         <v>96</v>
       </c>
       <c r="C100" s="131" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D100" s="132"/>
       <c r="E100" s="132"/>
@@ -17215,7 +17219,7 @@
         <v>97</v>
       </c>
       <c r="C101" s="131" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D101" s="132"/>
       <c r="E101" s="132"/>
@@ -17231,7 +17235,7 @@
         <v>98</v>
       </c>
       <c r="C102" s="131" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D102" s="132"/>
       <c r="E102" s="132"/>
@@ -17247,7 +17251,7 @@
         <v>99</v>
       </c>
       <c r="C103" s="131" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D103" s="132"/>
       <c r="E103" s="132"/>
@@ -17263,7 +17267,7 @@
         <v>100</v>
       </c>
       <c r="C104" s="131" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D104" s="132"/>
       <c r="E104" s="132"/>
@@ -17279,7 +17283,7 @@
         <v>101</v>
       </c>
       <c r="C105" s="131" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D105" s="132"/>
       <c r="E105" s="132"/>
@@ -17295,7 +17299,7 @@
         <v>102</v>
       </c>
       <c r="C106" s="131" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D106" s="132"/>
       <c r="E106" s="132"/>
@@ -17311,7 +17315,7 @@
         <v>103</v>
       </c>
       <c r="C107" s="131" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D107" s="132"/>
       <c r="E107" s="132"/>
@@ -17327,7 +17331,7 @@
         <v>104</v>
       </c>
       <c r="C108" s="131" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D108" s="132"/>
       <c r="E108" s="132"/>
@@ -17343,7 +17347,7 @@
         <v>105</v>
       </c>
       <c r="C109" s="131" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D109" s="132"/>
       <c r="E109" s="132"/>
@@ -17359,7 +17363,7 @@
         <v>106</v>
       </c>
       <c r="C110" s="131" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D110" s="132"/>
       <c r="E110" s="132"/>
@@ -17375,7 +17379,7 @@
         <v>107</v>
       </c>
       <c r="C111" s="131" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D111" s="132"/>
       <c r="E111" s="132"/>
@@ -17391,7 +17395,7 @@
         <v>108</v>
       </c>
       <c r="C112" s="131" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D112" s="132"/>
       <c r="E112" s="132"/>
@@ -17407,7 +17411,7 @@
         <v>109</v>
       </c>
       <c r="C113" s="131" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D113" s="132"/>
       <c r="E113" s="132"/>
@@ -17423,7 +17427,7 @@
         <v>110</v>
       </c>
       <c r="C114" s="71" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D114" s="72"/>
       <c r="E114" s="72"/>
@@ -17439,7 +17443,7 @@
         <v>111</v>
       </c>
       <c r="C115" s="71" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D115" s="72"/>
       <c r="E115" s="72"/>
@@ -17455,7 +17459,7 @@
         <v>112</v>
       </c>
       <c r="C116" s="71" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D116" s="72"/>
       <c r="E116" s="72"/>
@@ -17471,7 +17475,7 @@
         <v>113</v>
       </c>
       <c r="C117" s="71" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D117" s="72"/>
       <c r="E117" s="72"/>
@@ -17487,7 +17491,7 @@
         <v>114</v>
       </c>
       <c r="C118" s="71" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D118" s="72"/>
       <c r="E118" s="72"/>
@@ -17503,7 +17507,7 @@
         <v>115</v>
       </c>
       <c r="C119" s="71" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D119" s="72"/>
       <c r="E119" s="72"/>
@@ -17519,7 +17523,7 @@
         <v>116</v>
       </c>
       <c r="C120" s="71" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D120" s="72"/>
       <c r="E120" s="72"/>
@@ -17535,7 +17539,7 @@
         <v>117</v>
       </c>
       <c r="C121" s="71" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D121" s="72"/>
       <c r="E121" s="72"/>
@@ -17551,7 +17555,7 @@
         <v>118</v>
       </c>
       <c r="C122" s="71" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D122" s="72"/>
       <c r="E122" s="72"/>
@@ -17567,7 +17571,7 @@
         <v>119</v>
       </c>
       <c r="C123" s="71" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D123" s="72"/>
       <c r="E123" s="72"/>
@@ -17583,7 +17587,7 @@
         <v>120</v>
       </c>
       <c r="C124" s="71" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D124" s="72"/>
       <c r="E124" s="72"/>
@@ -17599,7 +17603,7 @@
         <v>121</v>
       </c>
       <c r="C125" s="71" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D125" s="72"/>
       <c r="E125" s="72"/>
@@ -17615,7 +17619,7 @@
         <v>122</v>
       </c>
       <c r="C126" s="71" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D126" s="72"/>
       <c r="E126" s="72"/>
@@ -17631,7 +17635,7 @@
         <v>123</v>
       </c>
       <c r="C127" s="71" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D127" s="72"/>
       <c r="E127" s="72"/>
@@ -17647,7 +17651,7 @@
         <v>124</v>
       </c>
       <c r="C128" s="71" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D128" s="72"/>
       <c r="E128" s="72"/>
@@ -17663,7 +17667,7 @@
         <v>125</v>
       </c>
       <c r="C129" s="71" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D129" s="72"/>
       <c r="E129" s="72"/>
@@ -17679,7 +17683,7 @@
         <v>126</v>
       </c>
       <c r="C130" s="71" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D130" s="72"/>
       <c r="E130" s="72"/>
@@ -17695,7 +17699,7 @@
         <v>127</v>
       </c>
       <c r="C131" s="71" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D131" s="72"/>
       <c r="E131" s="72"/>
@@ -17711,7 +17715,7 @@
         <v>128</v>
       </c>
       <c r="C132" s="71" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D132" s="72"/>
       <c r="E132" s="72"/>
@@ -17727,7 +17731,7 @@
         <v>129</v>
       </c>
       <c r="C133" s="71" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D133" s="72"/>
       <c r="E133" s="72"/>
@@ -17743,7 +17747,7 @@
         <v>130</v>
       </c>
       <c r="C134" s="131" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D134" s="132"/>
       <c r="E134" s="132"/>
@@ -17759,7 +17763,7 @@
         <v>131</v>
       </c>
       <c r="C135" s="131" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D135" s="132"/>
       <c r="E135" s="132"/>
@@ -17775,7 +17779,7 @@
         <v>132</v>
       </c>
       <c r="C136" s="131" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D136" s="132"/>
       <c r="E136" s="132"/>
@@ -17791,7 +17795,7 @@
         <v>133</v>
       </c>
       <c r="C137" s="131" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D137" s="132"/>
       <c r="E137" s="132"/>
@@ -17807,7 +17811,7 @@
         <v>134</v>
       </c>
       <c r="C138" s="131" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D138" s="132"/>
       <c r="E138" s="132"/>
@@ -17823,7 +17827,7 @@
         <v>135</v>
       </c>
       <c r="C139" s="131" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D139" s="132"/>
       <c r="E139" s="132"/>
@@ -17839,7 +17843,7 @@
         <v>136</v>
       </c>
       <c r="C140" s="131" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D140" s="132"/>
       <c r="E140" s="132"/>
@@ -17855,7 +17859,7 @@
         <v>137</v>
       </c>
       <c r="C141" s="131" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D141" s="132"/>
       <c r="E141" s="132"/>
@@ -17871,7 +17875,7 @@
         <v>138</v>
       </c>
       <c r="C142" s="131" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D142" s="132"/>
       <c r="E142" s="132"/>
@@ -17887,7 +17891,7 @@
         <v>139</v>
       </c>
       <c r="C143" s="131" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D143" s="132"/>
       <c r="E143" s="132"/>
@@ -17903,7 +17907,7 @@
         <v>140</v>
       </c>
       <c r="C144" s="131" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D144" s="132"/>
       <c r="E144" s="132"/>
@@ -17919,7 +17923,7 @@
         <v>141</v>
       </c>
       <c r="C145" s="131" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D145" s="132"/>
       <c r="E145" s="132"/>
@@ -17935,7 +17939,7 @@
         <v>142</v>
       </c>
       <c r="C146" s="131" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D146" s="132"/>
       <c r="E146" s="132"/>
@@ -17951,7 +17955,7 @@
         <v>143</v>
       </c>
       <c r="C147" s="131" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D147" s="132"/>
       <c r="E147" s="132"/>
@@ -17967,7 +17971,7 @@
         <v>144</v>
       </c>
       <c r="C148" s="131" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D148" s="132"/>
       <c r="E148" s="132"/>
@@ -17983,7 +17987,7 @@
         <v>145</v>
       </c>
       <c r="C149" s="131" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D149" s="132"/>
       <c r="E149" s="132"/>
@@ -17999,7 +18003,7 @@
         <v>146</v>
       </c>
       <c r="C150" s="131" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D150" s="132"/>
       <c r="E150" s="132"/>
@@ -18015,7 +18019,7 @@
         <v>147</v>
       </c>
       <c r="C151" s="131" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D151" s="132"/>
       <c r="E151" s="132"/>
@@ -18031,7 +18035,7 @@
         <v>148</v>
       </c>
       <c r="C152" s="131" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D152" s="132"/>
       <c r="E152" s="132"/>
@@ -18047,7 +18051,7 @@
         <v>149</v>
       </c>
       <c r="C153" s="131" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D153" s="132"/>
       <c r="E153" s="132"/>
@@ -18063,7 +18067,7 @@
         <v>150</v>
       </c>
       <c r="C154" s="71" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D154" s="72"/>
       <c r="E154" s="72"/>
@@ -18079,7 +18083,7 @@
         <v>151</v>
       </c>
       <c r="C155" s="71" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D155" s="72"/>
       <c r="E155" s="72"/>
@@ -18095,7 +18099,7 @@
         <v>152</v>
       </c>
       <c r="C156" s="71" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D156" s="72"/>
       <c r="E156" s="72"/>
@@ -18111,7 +18115,7 @@
         <v>153</v>
       </c>
       <c r="C157" s="71" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D157" s="72"/>
       <c r="E157" s="72"/>
@@ -18127,7 +18131,7 @@
         <v>154</v>
       </c>
       <c r="C158" s="71" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D158" s="72"/>
       <c r="E158" s="72"/>
@@ -18143,7 +18147,7 @@
         <v>155</v>
       </c>
       <c r="C159" s="71" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D159" s="72"/>
       <c r="E159" s="72"/>
@@ -18159,7 +18163,7 @@
         <v>156</v>
       </c>
       <c r="C160" s="71" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D160" s="72"/>
       <c r="E160" s="72"/>
@@ -18175,7 +18179,7 @@
         <v>157</v>
       </c>
       <c r="C161" s="71" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D161" s="72"/>
       <c r="E161" s="72"/>
@@ -18191,7 +18195,7 @@
         <v>158</v>
       </c>
       <c r="C162" s="71" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D162" s="72"/>
       <c r="E162" s="72"/>
@@ -18207,7 +18211,7 @@
         <v>159</v>
       </c>
       <c r="C163" s="71" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D163" s="72"/>
       <c r="E163" s="72"/>
@@ -18223,7 +18227,7 @@
         <v>160</v>
       </c>
       <c r="C164" s="71" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D164" s="72"/>
       <c r="E164" s="72"/>
@@ -18239,7 +18243,7 @@
         <v>161</v>
       </c>
       <c r="C165" s="71" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D165" s="72"/>
       <c r="E165" s="72"/>
@@ -18255,7 +18259,7 @@
         <v>162</v>
       </c>
       <c r="C166" s="71" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D166" s="72"/>
       <c r="E166" s="72"/>
@@ -18271,7 +18275,7 @@
         <v>163</v>
       </c>
       <c r="C167" s="71" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D167" s="72"/>
       <c r="E167" s="72"/>
@@ -18287,7 +18291,7 @@
         <v>164</v>
       </c>
       <c r="C168" s="71" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D168" s="72"/>
       <c r="E168" s="72"/>
@@ -18303,7 +18307,7 @@
         <v>165</v>
       </c>
       <c r="C169" s="71" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D169" s="72"/>
       <c r="E169" s="72"/>
@@ -18319,7 +18323,7 @@
         <v>166</v>
       </c>
       <c r="C170" s="71" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D170" s="72"/>
       <c r="E170" s="72"/>
@@ -18335,7 +18339,7 @@
         <v>167</v>
       </c>
       <c r="C171" s="71" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D171" s="72"/>
       <c r="E171" s="72"/>
@@ -18351,7 +18355,7 @@
         <v>168</v>
       </c>
       <c r="C172" s="71" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D172" s="72"/>
       <c r="E172" s="72"/>
@@ -18367,7 +18371,7 @@
         <v>169</v>
       </c>
       <c r="C173" s="71" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D173" s="72"/>
       <c r="E173" s="72"/>
@@ -18383,7 +18387,7 @@
         <v>170</v>
       </c>
       <c r="C174" s="131" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D174" s="132"/>
       <c r="E174" s="132"/>
@@ -18399,7 +18403,7 @@
         <v>171</v>
       </c>
       <c r="C175" s="131" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D175" s="132"/>
       <c r="E175" s="132"/>
@@ -18415,7 +18419,7 @@
         <v>172</v>
       </c>
       <c r="C176" s="131" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D176" s="132"/>
       <c r="E176" s="132"/>
@@ -18431,7 +18435,7 @@
         <v>173</v>
       </c>
       <c r="C177" s="131" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D177" s="132"/>
       <c r="E177" s="132"/>
@@ -18447,7 +18451,7 @@
         <v>174</v>
       </c>
       <c r="C178" s="131" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D178" s="132"/>
       <c r="E178" s="132"/>
@@ -18463,7 +18467,7 @@
         <v>175</v>
       </c>
       <c r="C179" s="131" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D179" s="132"/>
       <c r="E179" s="132"/>
@@ -18479,7 +18483,7 @@
         <v>176</v>
       </c>
       <c r="C180" s="131" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D180" s="132"/>
       <c r="E180" s="132"/>
@@ -18495,7 +18499,7 @@
         <v>177</v>
       </c>
       <c r="C181" s="131" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D181" s="132"/>
       <c r="E181" s="132"/>
@@ -18511,7 +18515,7 @@
         <v>178</v>
       </c>
       <c r="C182" s="131" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D182" s="132"/>
       <c r="E182" s="132"/>
@@ -18527,7 +18531,7 @@
         <v>179</v>
       </c>
       <c r="C183" s="131" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D183" s="132"/>
       <c r="E183" s="132"/>
@@ -18543,7 +18547,7 @@
         <v>180</v>
       </c>
       <c r="C184" s="131" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D184" s="132"/>
       <c r="E184" s="132"/>
@@ -18559,7 +18563,7 @@
         <v>181</v>
       </c>
       <c r="C185" s="131" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D185" s="132"/>
       <c r="E185" s="132"/>
@@ -18575,7 +18579,7 @@
         <v>182</v>
       </c>
       <c r="C186" s="131" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D186" s="132"/>
       <c r="E186" s="132"/>
@@ -18591,7 +18595,7 @@
         <v>183</v>
       </c>
       <c r="C187" s="131" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D187" s="132"/>
       <c r="E187" s="132"/>
@@ -18607,7 +18611,7 @@
         <v>184</v>
       </c>
       <c r="C188" s="131" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D188" s="132"/>
       <c r="E188" s="132"/>
@@ -18623,7 +18627,7 @@
         <v>185</v>
       </c>
       <c r="C189" s="131" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D189" s="132"/>
       <c r="E189" s="132"/>
@@ -18639,7 +18643,7 @@
         <v>186</v>
       </c>
       <c r="C190" s="131" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D190" s="132"/>
       <c r="E190" s="132"/>
@@ -18655,7 +18659,7 @@
         <v>187</v>
       </c>
       <c r="C191" s="131" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D191" s="132"/>
       <c r="E191" s="132"/>
@@ -18671,7 +18675,7 @@
         <v>188</v>
       </c>
       <c r="C192" s="131" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D192" s="132"/>
       <c r="E192" s="132"/>
@@ -18687,7 +18691,7 @@
         <v>189</v>
       </c>
       <c r="C193" s="131" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D193" s="132"/>
       <c r="E193" s="132"/>
@@ -18703,7 +18707,7 @@
         <v>190</v>
       </c>
       <c r="C194" s="71" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D194" s="72"/>
       <c r="E194" s="72"/>
@@ -18719,7 +18723,7 @@
         <v>191</v>
       </c>
       <c r="C195" s="71" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D195" s="72"/>
       <c r="E195" s="72"/>
@@ -18735,7 +18739,7 @@
         <v>192</v>
       </c>
       <c r="C196" s="71" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D196" s="72"/>
       <c r="E196" s="72"/>
@@ -18751,7 +18755,7 @@
         <v>193</v>
       </c>
       <c r="C197" s="71" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D197" s="72"/>
       <c r="E197" s="72"/>
@@ -18767,7 +18771,7 @@
         <v>194</v>
       </c>
       <c r="C198" s="71" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D198" s="72"/>
       <c r="E198" s="72"/>
@@ -18783,7 +18787,7 @@
         <v>195</v>
       </c>
       <c r="C199" s="71" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D199" s="72"/>
       <c r="E199" s="72"/>
@@ -18799,7 +18803,7 @@
         <v>196</v>
       </c>
       <c r="C200" s="71" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D200" s="72"/>
       <c r="E200" s="72"/>
@@ -18815,7 +18819,7 @@
         <v>197</v>
       </c>
       <c r="C201" s="71" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D201" s="72"/>
       <c r="E201" s="72"/>
@@ -18831,7 +18835,7 @@
         <v>198</v>
       </c>
       <c r="C202" s="71" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D202" s="72"/>
       <c r="E202" s="72"/>
@@ -18847,7 +18851,7 @@
         <v>199</v>
       </c>
       <c r="C203" s="71" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D203" s="72"/>
       <c r="E203" s="72"/>
@@ -18863,7 +18867,7 @@
         <v>200</v>
       </c>
       <c r="C204" s="71" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D204" s="72"/>
       <c r="E204" s="72"/>
@@ -18879,7 +18883,7 @@
         <v>201</v>
       </c>
       <c r="C205" s="71" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D205" s="72"/>
       <c r="E205" s="72"/>
@@ -18895,7 +18899,7 @@
         <v>202</v>
       </c>
       <c r="C206" s="71" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D206" s="72"/>
       <c r="E206" s="72"/>
@@ -18911,7 +18915,7 @@
         <v>203</v>
       </c>
       <c r="C207" s="71" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D207" s="72"/>
       <c r="E207" s="72"/>
@@ -18927,7 +18931,7 @@
         <v>204</v>
       </c>
       <c r="C208" s="71" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D208" s="72"/>
       <c r="E208" s="72"/>
@@ -18943,7 +18947,7 @@
         <v>205</v>
       </c>
       <c r="C209" s="71" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D209" s="72"/>
       <c r="E209" s="72"/>
@@ -18959,7 +18963,7 @@
         <v>206</v>
       </c>
       <c r="C210" s="71" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D210" s="72"/>
       <c r="E210" s="72"/>
@@ -18975,7 +18979,7 @@
         <v>207</v>
       </c>
       <c r="C211" s="71" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D211" s="72"/>
       <c r="E211" s="72"/>
@@ -18991,7 +18995,7 @@
         <v>208</v>
       </c>
       <c r="C212" s="71" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D212" s="72"/>
       <c r="E212" s="72"/>
@@ -19007,7 +19011,7 @@
         <v>209</v>
       </c>
       <c r="C213" s="71" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D213" s="72"/>
       <c r="E213" s="72"/>
@@ -19023,7 +19027,7 @@
         <v>210</v>
       </c>
       <c r="C214" s="64" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D214" s="65"/>
       <c r="E214" s="65"/>
@@ -19053,7 +19057,7 @@
         <v>410</v>
       </c>
       <c r="C216" s="64" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D216" s="65"/>
       <c r="E216" s="65"/>
@@ -19083,7 +19087,7 @@
         <v>610</v>
       </c>
       <c r="C218" s="64" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D218" s="65"/>
       <c r="E218" s="65"/>
@@ -19113,7 +19117,7 @@
         <v>810</v>
       </c>
       <c r="C220" s="64" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D220" s="65"/>
       <c r="E220" s="65"/>
@@ -19143,7 +19147,7 @@
         <v>1010</v>
       </c>
       <c r="C222" s="64" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D222" s="65"/>
       <c r="E222" s="65"/>
@@ -19173,7 +19177,7 @@
         <v>1210</v>
       </c>
       <c r="C224" s="64" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D224" s="65"/>
       <c r="E224" s="65"/>
@@ -19567,7 +19571,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="53" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D5" s="54"/>
       <c r="E5" s="54"/>
@@ -19645,7 +19649,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="61" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D7" s="62"/>
       <c r="E7" s="62"/>
@@ -19685,7 +19689,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="48" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D8" s="49"/>
       <c r="E8" s="49"/>
@@ -19725,7 +19729,7 @@
         <v>5</v>
       </c>
       <c r="C9" s="48" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D9" s="49"/>
       <c r="E9" s="49"/>
@@ -19925,7 +19929,7 @@
         <v>10</v>
       </c>
       <c r="C14" s="131" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D14" s="132"/>
       <c r="E14" s="132"/>
@@ -19965,7 +19969,7 @@
         <v>11</v>
       </c>
       <c r="C15" s="131" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D15" s="132"/>
       <c r="E15" s="132"/>
@@ -20005,7 +20009,7 @@
         <v>12</v>
       </c>
       <c r="C16" s="131" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D16" s="132"/>
       <c r="E16" s="132"/>
@@ -20045,7 +20049,7 @@
         <v>13</v>
       </c>
       <c r="C17" s="131" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D17" s="132"/>
       <c r="E17" s="132"/>
@@ -20085,7 +20089,7 @@
         <v>14</v>
       </c>
       <c r="C18" s="131" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D18" s="132"/>
       <c r="E18" s="132"/>
@@ -20125,7 +20129,7 @@
         <v>15</v>
       </c>
       <c r="C19" s="131" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D19" s="132"/>
       <c r="E19" s="132"/>
@@ -20165,7 +20169,7 @@
         <v>16</v>
       </c>
       <c r="C20" s="131" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D20" s="132"/>
       <c r="E20" s="132"/>
@@ -20205,7 +20209,7 @@
         <v>17</v>
       </c>
       <c r="C21" s="131" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D21" s="132"/>
       <c r="E21" s="132"/>
@@ -20245,7 +20249,7 @@
         <v>18</v>
       </c>
       <c r="C22" s="131" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D22" s="132"/>
       <c r="E22" s="132"/>
@@ -20285,7 +20289,7 @@
         <v>19</v>
       </c>
       <c r="C23" s="131" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D23" s="132"/>
       <c r="E23" s="132"/>
@@ -20325,7 +20329,7 @@
         <v>20</v>
       </c>
       <c r="C24" s="131" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D24" s="132"/>
       <c r="E24" s="132"/>
@@ -20365,7 +20369,7 @@
         <v>21</v>
       </c>
       <c r="C25" s="131" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D25" s="132"/>
       <c r="E25" s="132"/>
@@ -20381,7 +20385,7 @@
         <v>22</v>
       </c>
       <c r="C26" s="131" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D26" s="132"/>
       <c r="E26" s="132"/>
@@ -20397,7 +20401,7 @@
         <v>23</v>
       </c>
       <c r="C27" s="131" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D27" s="132"/>
       <c r="E27" s="132"/>
@@ -20413,7 +20417,7 @@
         <v>24</v>
       </c>
       <c r="C28" s="131" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D28" s="132"/>
       <c r="E28" s="132"/>
@@ -20429,7 +20433,7 @@
         <v>25</v>
       </c>
       <c r="C29" s="131" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D29" s="132"/>
       <c r="E29" s="132"/>
@@ -20445,7 +20449,7 @@
         <v>26</v>
       </c>
       <c r="C30" s="131" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D30" s="132"/>
       <c r="E30" s="132"/>
@@ -20461,7 +20465,7 @@
         <v>27</v>
       </c>
       <c r="C31" s="131" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D31" s="132"/>
       <c r="E31" s="132"/>
@@ -20477,7 +20481,7 @@
         <v>28</v>
       </c>
       <c r="C32" s="131" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D32" s="132"/>
       <c r="E32" s="132"/>
@@ -20493,7 +20497,7 @@
         <v>29</v>
       </c>
       <c r="C33" s="131" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D33" s="132"/>
       <c r="E33" s="132"/>
@@ -20509,7 +20513,7 @@
         <v>30</v>
       </c>
       <c r="C34" s="71" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D34" s="72"/>
       <c r="E34" s="72"/>
@@ -20525,7 +20529,7 @@
         <v>31</v>
       </c>
       <c r="C35" s="71" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D35" s="72"/>
       <c r="E35" s="72"/>
@@ -20541,7 +20545,7 @@
         <v>32</v>
       </c>
       <c r="C36" s="71" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D36" s="72"/>
       <c r="E36" s="72"/>
@@ -20557,7 +20561,7 @@
         <v>33</v>
       </c>
       <c r="C37" s="71" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D37" s="72"/>
       <c r="E37" s="72"/>
@@ -20573,7 +20577,7 @@
         <v>34</v>
       </c>
       <c r="C38" s="71" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D38" s="72"/>
       <c r="E38" s="72"/>
@@ -20589,7 +20593,7 @@
         <v>35</v>
       </c>
       <c r="C39" s="71" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D39" s="72"/>
       <c r="E39" s="72"/>
@@ -20605,7 +20609,7 @@
         <v>36</v>
       </c>
       <c r="C40" s="71" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D40" s="72"/>
       <c r="E40" s="72"/>
@@ -20621,7 +20625,7 @@
         <v>37</v>
       </c>
       <c r="C41" s="71" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D41" s="72"/>
       <c r="E41" s="72"/>
@@ -20637,7 +20641,7 @@
         <v>38</v>
       </c>
       <c r="C42" s="71" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D42" s="72"/>
       <c r="E42" s="72"/>
@@ -20653,7 +20657,7 @@
         <v>39</v>
       </c>
       <c r="C43" s="71" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D43" s="72"/>
       <c r="E43" s="72"/>
@@ -20669,7 +20673,7 @@
         <v>40</v>
       </c>
       <c r="C44" s="71" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D44" s="72"/>
       <c r="E44" s="72"/>
@@ -20685,7 +20689,7 @@
         <v>41</v>
       </c>
       <c r="C45" s="71" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D45" s="72"/>
       <c r="E45" s="72"/>
@@ -20701,7 +20705,7 @@
         <v>42</v>
       </c>
       <c r="C46" s="71" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D46" s="72"/>
       <c r="E46" s="72"/>
@@ -20717,7 +20721,7 @@
         <v>43</v>
       </c>
       <c r="C47" s="71" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D47" s="72"/>
       <c r="E47" s="72"/>
@@ -20733,7 +20737,7 @@
         <v>44</v>
       </c>
       <c r="C48" s="71" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D48" s="72"/>
       <c r="E48" s="72"/>
@@ -20749,7 +20753,7 @@
         <v>45</v>
       </c>
       <c r="C49" s="71" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D49" s="72"/>
       <c r="E49" s="72"/>
@@ -20765,7 +20769,7 @@
         <v>46</v>
       </c>
       <c r="C50" s="71" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D50" s="72"/>
       <c r="E50" s="72"/>
@@ -20781,7 +20785,7 @@
         <v>47</v>
       </c>
       <c r="C51" s="71" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D51" s="72"/>
       <c r="E51" s="72"/>
@@ -20797,7 +20801,7 @@
         <v>48</v>
       </c>
       <c r="C52" s="71" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D52" s="72"/>
       <c r="E52" s="72"/>
@@ -20813,7 +20817,7 @@
         <v>49</v>
       </c>
       <c r="C53" s="71" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D53" s="72"/>
       <c r="E53" s="72"/>
@@ -20829,7 +20833,7 @@
         <v>50</v>
       </c>
       <c r="C54" s="131" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D54" s="132"/>
       <c r="E54" s="132"/>
@@ -20845,7 +20849,7 @@
         <v>51</v>
       </c>
       <c r="C55" s="131" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D55" s="132"/>
       <c r="E55" s="132"/>
@@ -20861,7 +20865,7 @@
         <v>52</v>
       </c>
       <c r="C56" s="131" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D56" s="132"/>
       <c r="E56" s="132"/>
@@ -20877,7 +20881,7 @@
         <v>53</v>
       </c>
       <c r="C57" s="131" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D57" s="132"/>
       <c r="E57" s="132"/>
@@ -20893,7 +20897,7 @@
         <v>54</v>
       </c>
       <c r="C58" s="131" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D58" s="132"/>
       <c r="E58" s="132"/>
@@ -20909,7 +20913,7 @@
         <v>55</v>
       </c>
       <c r="C59" s="131" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D59" s="132"/>
       <c r="E59" s="132"/>
@@ -20925,7 +20929,7 @@
         <v>56</v>
       </c>
       <c r="C60" s="131" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D60" s="132"/>
       <c r="E60" s="132"/>
@@ -20941,7 +20945,7 @@
         <v>57</v>
       </c>
       <c r="C61" s="131" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D61" s="132"/>
       <c r="E61" s="132"/>
@@ -20957,7 +20961,7 @@
         <v>58</v>
       </c>
       <c r="C62" s="131" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D62" s="132"/>
       <c r="E62" s="132"/>
@@ -20973,7 +20977,7 @@
         <v>59</v>
       </c>
       <c r="C63" s="131" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D63" s="132"/>
       <c r="E63" s="132"/>
@@ -20989,7 +20993,7 @@
         <v>60</v>
       </c>
       <c r="C64" s="131" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D64" s="132"/>
       <c r="E64" s="132"/>
@@ -21005,7 +21009,7 @@
         <v>61</v>
       </c>
       <c r="C65" s="131" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D65" s="132"/>
       <c r="E65" s="132"/>
@@ -21021,7 +21025,7 @@
         <v>62</v>
       </c>
       <c r="C66" s="131" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D66" s="132"/>
       <c r="E66" s="132"/>
@@ -21037,7 +21041,7 @@
         <v>63</v>
       </c>
       <c r="C67" s="131" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D67" s="132"/>
       <c r="E67" s="132"/>
@@ -21053,7 +21057,7 @@
         <v>64</v>
       </c>
       <c r="C68" s="131" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D68" s="132"/>
       <c r="E68" s="132"/>
@@ -21069,7 +21073,7 @@
         <v>65</v>
       </c>
       <c r="C69" s="131" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D69" s="132"/>
       <c r="E69" s="132"/>
@@ -21085,7 +21089,7 @@
         <v>66</v>
       </c>
       <c r="C70" s="131" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D70" s="132"/>
       <c r="E70" s="132"/>
@@ -21101,7 +21105,7 @@
         <v>67</v>
       </c>
       <c r="C71" s="131" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D71" s="132"/>
       <c r="E71" s="132"/>
@@ -21117,7 +21121,7 @@
         <v>68</v>
       </c>
       <c r="C72" s="131" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D72" s="132"/>
       <c r="E72" s="132"/>
@@ -21133,7 +21137,7 @@
         <v>69</v>
       </c>
       <c r="C73" s="131" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D73" s="132"/>
       <c r="E73" s="132"/>
@@ -21149,7 +21153,7 @@
         <v>70</v>
       </c>
       <c r="C74" s="71" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D74" s="72"/>
       <c r="E74" s="72"/>
@@ -21165,7 +21169,7 @@
         <v>71</v>
       </c>
       <c r="C75" s="71" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D75" s="72"/>
       <c r="E75" s="72"/>
@@ -21181,7 +21185,7 @@
         <v>72</v>
       </c>
       <c r="C76" s="71" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D76" s="72"/>
       <c r="E76" s="72"/>
@@ -21197,7 +21201,7 @@
         <v>73</v>
       </c>
       <c r="C77" s="71" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D77" s="72"/>
       <c r="E77" s="72"/>
@@ -21213,7 +21217,7 @@
         <v>74</v>
       </c>
       <c r="C78" s="71" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D78" s="72"/>
       <c r="E78" s="72"/>
@@ -21229,7 +21233,7 @@
         <v>75</v>
       </c>
       <c r="C79" s="71" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D79" s="72"/>
       <c r="E79" s="72"/>
@@ -21245,7 +21249,7 @@
         <v>76</v>
       </c>
       <c r="C80" s="71" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D80" s="72"/>
       <c r="E80" s="72"/>
@@ -21261,7 +21265,7 @@
         <v>77</v>
       </c>
       <c r="C81" s="71" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D81" s="72"/>
       <c r="E81" s="72"/>
@@ -21277,7 +21281,7 @@
         <v>78</v>
       </c>
       <c r="C82" s="71" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D82" s="72"/>
       <c r="E82" s="72"/>
@@ -21293,7 +21297,7 @@
         <v>79</v>
       </c>
       <c r="C83" s="71" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D83" s="72"/>
       <c r="E83" s="72"/>
@@ -21309,7 +21313,7 @@
         <v>80</v>
       </c>
       <c r="C84" s="71" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D84" s="72"/>
       <c r="E84" s="72"/>
@@ -21325,7 +21329,7 @@
         <v>81</v>
       </c>
       <c r="C85" s="71" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D85" s="72"/>
       <c r="E85" s="72"/>
@@ -21341,7 +21345,7 @@
         <v>82</v>
       </c>
       <c r="C86" s="71" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D86" s="72"/>
       <c r="E86" s="72"/>
@@ -21357,7 +21361,7 @@
         <v>83</v>
       </c>
       <c r="C87" s="71" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D87" s="72"/>
       <c r="E87" s="72"/>
@@ -21373,7 +21377,7 @@
         <v>84</v>
       </c>
       <c r="C88" s="71" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D88" s="72"/>
       <c r="E88" s="72"/>
@@ -21389,7 +21393,7 @@
         <v>85</v>
       </c>
       <c r="C89" s="71" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D89" s="72"/>
       <c r="E89" s="72"/>
@@ -21405,7 +21409,7 @@
         <v>86</v>
       </c>
       <c r="C90" s="71" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D90" s="72"/>
       <c r="E90" s="72"/>
@@ -21421,7 +21425,7 @@
         <v>87</v>
       </c>
       <c r="C91" s="71" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D91" s="72"/>
       <c r="E91" s="72"/>
@@ -21437,7 +21441,7 @@
         <v>88</v>
       </c>
       <c r="C92" s="71" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D92" s="72"/>
       <c r="E92" s="72"/>
@@ -21453,7 +21457,7 @@
         <v>89</v>
       </c>
       <c r="C93" s="71" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D93" s="72"/>
       <c r="E93" s="72"/>
@@ -21469,7 +21473,7 @@
         <v>90</v>
       </c>
       <c r="C94" s="131" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D94" s="132"/>
       <c r="E94" s="132"/>
@@ -21485,7 +21489,7 @@
         <v>91</v>
       </c>
       <c r="C95" s="131" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D95" s="132"/>
       <c r="E95" s="132"/>
@@ -21501,7 +21505,7 @@
         <v>92</v>
       </c>
       <c r="C96" s="131" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D96" s="132"/>
       <c r="E96" s="132"/>
@@ -21517,7 +21521,7 @@
         <v>93</v>
       </c>
       <c r="C97" s="131" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D97" s="132"/>
       <c r="E97" s="132"/>
@@ -21533,7 +21537,7 @@
         <v>94</v>
       </c>
       <c r="C98" s="131" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D98" s="132"/>
       <c r="E98" s="132"/>
@@ -21549,7 +21553,7 @@
         <v>95</v>
       </c>
       <c r="C99" s="131" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D99" s="132"/>
       <c r="E99" s="132"/>
@@ -21565,7 +21569,7 @@
         <v>96</v>
       </c>
       <c r="C100" s="131" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D100" s="132"/>
       <c r="E100" s="132"/>
@@ -21581,7 +21585,7 @@
         <v>97</v>
       </c>
       <c r="C101" s="131" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D101" s="132"/>
       <c r="E101" s="132"/>
@@ -21597,7 +21601,7 @@
         <v>98</v>
       </c>
       <c r="C102" s="131" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D102" s="132"/>
       <c r="E102" s="132"/>
@@ -21613,7 +21617,7 @@
         <v>99</v>
       </c>
       <c r="C103" s="131" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D103" s="132"/>
       <c r="E103" s="132"/>
@@ -21629,7 +21633,7 @@
         <v>100</v>
       </c>
       <c r="C104" s="131" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D104" s="132"/>
       <c r="E104" s="132"/>
@@ -21645,7 +21649,7 @@
         <v>101</v>
       </c>
       <c r="C105" s="131" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D105" s="132"/>
       <c r="E105" s="132"/>
@@ -21661,7 +21665,7 @@
         <v>102</v>
       </c>
       <c r="C106" s="131" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D106" s="132"/>
       <c r="E106" s="132"/>
@@ -21677,7 +21681,7 @@
         <v>103</v>
       </c>
       <c r="C107" s="131" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D107" s="132"/>
       <c r="E107" s="132"/>
@@ -21693,7 +21697,7 @@
         <v>104</v>
       </c>
       <c r="C108" s="131" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D108" s="132"/>
       <c r="E108" s="132"/>
@@ -21709,7 +21713,7 @@
         <v>105</v>
       </c>
       <c r="C109" s="131" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D109" s="132"/>
       <c r="E109" s="132"/>
@@ -21725,7 +21729,7 @@
         <v>106</v>
       </c>
       <c r="C110" s="131" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D110" s="132"/>
       <c r="E110" s="132"/>
@@ -21741,7 +21745,7 @@
         <v>107</v>
       </c>
       <c r="C111" s="131" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D111" s="132"/>
       <c r="E111" s="132"/>
@@ -21757,7 +21761,7 @@
         <v>108</v>
       </c>
       <c r="C112" s="131" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D112" s="132"/>
       <c r="E112" s="132"/>
@@ -21773,7 +21777,7 @@
         <v>109</v>
       </c>
       <c r="C113" s="131" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D113" s="132"/>
       <c r="E113" s="132"/>
@@ -21789,7 +21793,7 @@
         <v>110</v>
       </c>
       <c r="C114" s="71" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D114" s="72"/>
       <c r="E114" s="72"/>
@@ -21805,7 +21809,7 @@
         <v>111</v>
       </c>
       <c r="C115" s="71" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D115" s="72"/>
       <c r="E115" s="72"/>
@@ -21821,7 +21825,7 @@
         <v>112</v>
       </c>
       <c r="C116" s="71" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D116" s="72"/>
       <c r="E116" s="72"/>
@@ -21837,7 +21841,7 @@
         <v>113</v>
       </c>
       <c r="C117" s="71" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D117" s="72"/>
       <c r="E117" s="72"/>
@@ -21853,7 +21857,7 @@
         <v>114</v>
       </c>
       <c r="C118" s="71" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D118" s="72"/>
       <c r="E118" s="72"/>
@@ -21869,7 +21873,7 @@
         <v>115</v>
       </c>
       <c r="C119" s="71" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D119" s="72"/>
       <c r="E119" s="72"/>
@@ -21885,7 +21889,7 @@
         <v>116</v>
       </c>
       <c r="C120" s="71" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D120" s="72"/>
       <c r="E120" s="72"/>
@@ -21901,7 +21905,7 @@
         <v>117</v>
       </c>
       <c r="C121" s="71" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D121" s="72"/>
       <c r="E121" s="72"/>
@@ -21917,7 +21921,7 @@
         <v>118</v>
       </c>
       <c r="C122" s="71" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D122" s="72"/>
       <c r="E122" s="72"/>
@@ -21933,7 +21937,7 @@
         <v>119</v>
       </c>
       <c r="C123" s="71" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D123" s="72"/>
       <c r="E123" s="72"/>
@@ -21949,7 +21953,7 @@
         <v>120</v>
       </c>
       <c r="C124" s="71" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D124" s="72"/>
       <c r="E124" s="72"/>
@@ -21965,7 +21969,7 @@
         <v>121</v>
       </c>
       <c r="C125" s="71" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D125" s="72"/>
       <c r="E125" s="72"/>
@@ -21981,7 +21985,7 @@
         <v>122</v>
       </c>
       <c r="C126" s="71" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D126" s="72"/>
       <c r="E126" s="72"/>
@@ -21997,7 +22001,7 @@
         <v>123</v>
       </c>
       <c r="C127" s="71" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D127" s="72"/>
       <c r="E127" s="72"/>
@@ -22013,7 +22017,7 @@
         <v>124</v>
       </c>
       <c r="C128" s="71" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D128" s="72"/>
       <c r="E128" s="72"/>
@@ -22029,7 +22033,7 @@
         <v>125</v>
       </c>
       <c r="C129" s="71" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D129" s="72"/>
       <c r="E129" s="72"/>
@@ -22045,7 +22049,7 @@
         <v>126</v>
       </c>
       <c r="C130" s="71" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D130" s="72"/>
       <c r="E130" s="72"/>
@@ -22061,7 +22065,7 @@
         <v>127</v>
       </c>
       <c r="C131" s="71" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D131" s="72"/>
       <c r="E131" s="72"/>
@@ -22077,7 +22081,7 @@
         <v>128</v>
       </c>
       <c r="C132" s="71" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D132" s="72"/>
       <c r="E132" s="72"/>
@@ -22093,7 +22097,7 @@
         <v>129</v>
       </c>
       <c r="C133" s="71" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D133" s="72"/>
       <c r="E133" s="72"/>
@@ -22109,7 +22113,7 @@
         <v>130</v>
       </c>
       <c r="C134" s="131" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D134" s="132"/>
       <c r="E134" s="132"/>
@@ -22125,7 +22129,7 @@
         <v>131</v>
       </c>
       <c r="C135" s="131" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D135" s="132"/>
       <c r="E135" s="132"/>
@@ -22141,7 +22145,7 @@
         <v>132</v>
       </c>
       <c r="C136" s="131" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D136" s="132"/>
       <c r="E136" s="132"/>
@@ -22157,7 +22161,7 @@
         <v>133</v>
       </c>
       <c r="C137" s="131" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D137" s="132"/>
       <c r="E137" s="132"/>
@@ -22173,7 +22177,7 @@
         <v>134</v>
       </c>
       <c r="C138" s="131" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D138" s="132"/>
       <c r="E138" s="132"/>
@@ -22189,7 +22193,7 @@
         <v>135</v>
       </c>
       <c r="C139" s="131" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D139" s="132"/>
       <c r="E139" s="132"/>
@@ -22205,7 +22209,7 @@
         <v>136</v>
       </c>
       <c r="C140" s="131" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D140" s="132"/>
       <c r="E140" s="132"/>
@@ -22221,7 +22225,7 @@
         <v>137</v>
       </c>
       <c r="C141" s="131" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D141" s="132"/>
       <c r="E141" s="132"/>
@@ -22237,7 +22241,7 @@
         <v>138</v>
       </c>
       <c r="C142" s="131" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D142" s="132"/>
       <c r="E142" s="132"/>
@@ -22253,7 +22257,7 @@
         <v>139</v>
       </c>
       <c r="C143" s="131" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D143" s="132"/>
       <c r="E143" s="132"/>
@@ -22269,7 +22273,7 @@
         <v>140</v>
       </c>
       <c r="C144" s="131" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D144" s="132"/>
       <c r="E144" s="132"/>
@@ -22285,7 +22289,7 @@
         <v>141</v>
       </c>
       <c r="C145" s="131" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D145" s="132"/>
       <c r="E145" s="132"/>
@@ -22301,7 +22305,7 @@
         <v>142</v>
       </c>
       <c r="C146" s="131" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D146" s="132"/>
       <c r="E146" s="132"/>
@@ -22317,7 +22321,7 @@
         <v>143</v>
       </c>
       <c r="C147" s="131" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D147" s="132"/>
       <c r="E147" s="132"/>
@@ -22333,7 +22337,7 @@
         <v>144</v>
       </c>
       <c r="C148" s="131" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D148" s="132"/>
       <c r="E148" s="132"/>
@@ -22349,7 +22353,7 @@
         <v>145</v>
       </c>
       <c r="C149" s="131" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D149" s="132"/>
       <c r="E149" s="132"/>
@@ -22365,7 +22369,7 @@
         <v>146</v>
       </c>
       <c r="C150" s="131" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D150" s="132"/>
       <c r="E150" s="132"/>
@@ -22381,7 +22385,7 @@
         <v>147</v>
       </c>
       <c r="C151" s="131" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D151" s="132"/>
       <c r="E151" s="132"/>
@@ -22397,7 +22401,7 @@
         <v>148</v>
       </c>
       <c r="C152" s="131" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D152" s="132"/>
       <c r="E152" s="132"/>
@@ -22413,7 +22417,7 @@
         <v>149</v>
       </c>
       <c r="C153" s="131" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D153" s="132"/>
       <c r="E153" s="132"/>
@@ -22429,7 +22433,7 @@
         <v>150</v>
       </c>
       <c r="C154" s="71" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D154" s="72"/>
       <c r="E154" s="72"/>
@@ -22445,7 +22449,7 @@
         <v>151</v>
       </c>
       <c r="C155" s="71" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D155" s="72"/>
       <c r="E155" s="72"/>
@@ -22461,7 +22465,7 @@
         <v>152</v>
       </c>
       <c r="C156" s="71" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D156" s="72"/>
       <c r="E156" s="72"/>
@@ -22477,7 +22481,7 @@
         <v>153</v>
       </c>
       <c r="C157" s="71" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D157" s="72"/>
       <c r="E157" s="72"/>
@@ -22493,7 +22497,7 @@
         <v>154</v>
       </c>
       <c r="C158" s="71" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D158" s="72"/>
       <c r="E158" s="72"/>
@@ -22509,7 +22513,7 @@
         <v>155</v>
       </c>
       <c r="C159" s="71" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D159" s="72"/>
       <c r="E159" s="72"/>
@@ -22525,7 +22529,7 @@
         <v>156</v>
       </c>
       <c r="C160" s="71" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D160" s="72"/>
       <c r="E160" s="72"/>
@@ -22541,7 +22545,7 @@
         <v>157</v>
       </c>
       <c r="C161" s="71" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D161" s="72"/>
       <c r="E161" s="72"/>
@@ -22557,7 +22561,7 @@
         <v>158</v>
       </c>
       <c r="C162" s="71" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D162" s="72"/>
       <c r="E162" s="72"/>
@@ -22573,7 +22577,7 @@
         <v>159</v>
       </c>
       <c r="C163" s="71" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D163" s="72"/>
       <c r="E163" s="72"/>
@@ -22589,7 +22593,7 @@
         <v>160</v>
       </c>
       <c r="C164" s="71" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D164" s="72"/>
       <c r="E164" s="72"/>
@@ -22605,7 +22609,7 @@
         <v>161</v>
       </c>
       <c r="C165" s="71" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D165" s="72"/>
       <c r="E165" s="72"/>
@@ -22621,7 +22625,7 @@
         <v>162</v>
       </c>
       <c r="C166" s="71" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D166" s="72"/>
       <c r="E166" s="72"/>
@@ -22637,7 +22641,7 @@
         <v>163</v>
       </c>
       <c r="C167" s="71" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D167" s="72"/>
       <c r="E167" s="72"/>
@@ -22653,7 +22657,7 @@
         <v>164</v>
       </c>
       <c r="C168" s="71" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D168" s="72"/>
       <c r="E168" s="72"/>
@@ -22669,7 +22673,7 @@
         <v>165</v>
       </c>
       <c r="C169" s="71" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D169" s="72"/>
       <c r="E169" s="72"/>
@@ -22685,7 +22689,7 @@
         <v>166</v>
       </c>
       <c r="C170" s="71" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D170" s="72"/>
       <c r="E170" s="72"/>
@@ -22701,7 +22705,7 @@
         <v>167</v>
       </c>
       <c r="C171" s="71" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D171" s="72"/>
       <c r="E171" s="72"/>
@@ -22717,7 +22721,7 @@
         <v>168</v>
       </c>
       <c r="C172" s="71" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D172" s="72"/>
       <c r="E172" s="72"/>
@@ -22733,7 +22737,7 @@
         <v>169</v>
       </c>
       <c r="C173" s="71" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D173" s="72"/>
       <c r="E173" s="72"/>
@@ -22749,7 +22753,7 @@
         <v>170</v>
       </c>
       <c r="C174" s="131" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D174" s="132"/>
       <c r="E174" s="132"/>
@@ -22765,7 +22769,7 @@
         <v>171</v>
       </c>
       <c r="C175" s="131" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D175" s="132"/>
       <c r="E175" s="132"/>
@@ -22781,7 +22785,7 @@
         <v>172</v>
       </c>
       <c r="C176" s="131" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D176" s="132"/>
       <c r="E176" s="132"/>
@@ -22797,7 +22801,7 @@
         <v>173</v>
       </c>
       <c r="C177" s="131" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D177" s="132"/>
       <c r="E177" s="132"/>
@@ -22813,7 +22817,7 @@
         <v>174</v>
       </c>
       <c r="C178" s="131" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D178" s="132"/>
       <c r="E178" s="132"/>
@@ -22829,7 +22833,7 @@
         <v>175</v>
       </c>
       <c r="C179" s="131" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D179" s="132"/>
       <c r="E179" s="132"/>
@@ -22845,7 +22849,7 @@
         <v>176</v>
       </c>
       <c r="C180" s="131" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D180" s="132"/>
       <c r="E180" s="132"/>
@@ -22861,7 +22865,7 @@
         <v>177</v>
       </c>
       <c r="C181" s="131" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D181" s="132"/>
       <c r="E181" s="132"/>
@@ -22877,7 +22881,7 @@
         <v>178</v>
       </c>
       <c r="C182" s="131" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D182" s="132"/>
       <c r="E182" s="132"/>
@@ -22893,7 +22897,7 @@
         <v>179</v>
       </c>
       <c r="C183" s="131" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D183" s="132"/>
       <c r="E183" s="132"/>
@@ -22909,7 +22913,7 @@
         <v>180</v>
       </c>
       <c r="C184" s="131" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D184" s="132"/>
       <c r="E184" s="132"/>
@@ -22925,7 +22929,7 @@
         <v>181</v>
       </c>
       <c r="C185" s="131" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D185" s="132"/>
       <c r="E185" s="132"/>
@@ -22941,7 +22945,7 @@
         <v>182</v>
       </c>
       <c r="C186" s="131" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D186" s="132"/>
       <c r="E186" s="132"/>
@@ -22957,7 +22961,7 @@
         <v>183</v>
       </c>
       <c r="C187" s="131" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D187" s="132"/>
       <c r="E187" s="132"/>
@@ -22973,7 +22977,7 @@
         <v>184</v>
       </c>
       <c r="C188" s="131" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D188" s="132"/>
       <c r="E188" s="132"/>
@@ -22989,7 +22993,7 @@
         <v>185</v>
       </c>
       <c r="C189" s="131" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D189" s="132"/>
       <c r="E189" s="132"/>
@@ -23005,7 +23009,7 @@
         <v>186</v>
       </c>
       <c r="C190" s="131" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D190" s="132"/>
       <c r="E190" s="132"/>
@@ -23021,7 +23025,7 @@
         <v>187</v>
       </c>
       <c r="C191" s="131" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D191" s="132"/>
       <c r="E191" s="132"/>
@@ -23037,7 +23041,7 @@
         <v>188</v>
       </c>
       <c r="C192" s="131" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D192" s="132"/>
       <c r="E192" s="132"/>
@@ -23053,7 +23057,7 @@
         <v>189</v>
       </c>
       <c r="C193" s="131" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D193" s="132"/>
       <c r="E193" s="132"/>
@@ -23069,7 +23073,7 @@
         <v>190</v>
       </c>
       <c r="C194" s="71" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D194" s="72"/>
       <c r="E194" s="72"/>
@@ -23085,7 +23089,7 @@
         <v>191</v>
       </c>
       <c r="C195" s="71" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D195" s="72"/>
       <c r="E195" s="72"/>
@@ -23101,7 +23105,7 @@
         <v>192</v>
       </c>
       <c r="C196" s="71" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D196" s="72"/>
       <c r="E196" s="72"/>
@@ -23117,7 +23121,7 @@
         <v>193</v>
       </c>
       <c r="C197" s="71" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D197" s="72"/>
       <c r="E197" s="72"/>
@@ -23133,7 +23137,7 @@
         <v>194</v>
       </c>
       <c r="C198" s="71" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D198" s="72"/>
       <c r="E198" s="72"/>
@@ -23149,7 +23153,7 @@
         <v>195</v>
       </c>
       <c r="C199" s="71" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D199" s="72"/>
       <c r="E199" s="72"/>
@@ -23165,7 +23169,7 @@
         <v>196</v>
       </c>
       <c r="C200" s="71" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D200" s="72"/>
       <c r="E200" s="72"/>
@@ -23181,7 +23185,7 @@
         <v>197</v>
       </c>
       <c r="C201" s="71" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D201" s="72"/>
       <c r="E201" s="72"/>
@@ -23197,7 +23201,7 @@
         <v>198</v>
       </c>
       <c r="C202" s="71" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D202" s="72"/>
       <c r="E202" s="72"/>
@@ -23213,7 +23217,7 @@
         <v>199</v>
       </c>
       <c r="C203" s="71" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D203" s="72"/>
       <c r="E203" s="72"/>
@@ -23229,7 +23233,7 @@
         <v>200</v>
       </c>
       <c r="C204" s="71" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D204" s="72"/>
       <c r="E204" s="72"/>
@@ -23245,7 +23249,7 @@
         <v>201</v>
       </c>
       <c r="C205" s="71" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D205" s="72"/>
       <c r="E205" s="72"/>
@@ -23261,7 +23265,7 @@
         <v>202</v>
       </c>
       <c r="C206" s="71" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D206" s="72"/>
       <c r="E206" s="72"/>
@@ -23277,7 +23281,7 @@
         <v>203</v>
       </c>
       <c r="C207" s="71" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D207" s="72"/>
       <c r="E207" s="72"/>
@@ -23293,7 +23297,7 @@
         <v>204</v>
       </c>
       <c r="C208" s="71" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D208" s="72"/>
       <c r="E208" s="72"/>
@@ -23309,7 +23313,7 @@
         <v>205</v>
       </c>
       <c r="C209" s="71" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D209" s="72"/>
       <c r="E209" s="72"/>
@@ -23325,7 +23329,7 @@
         <v>206</v>
       </c>
       <c r="C210" s="71" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D210" s="72"/>
       <c r="E210" s="72"/>
@@ -23341,7 +23345,7 @@
         <v>207</v>
       </c>
       <c r="C211" s="71" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D211" s="72"/>
       <c r="E211" s="72"/>
@@ -23357,7 +23361,7 @@
         <v>208</v>
       </c>
       <c r="C212" s="71" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D212" s="72"/>
       <c r="E212" s="72"/>
@@ -23373,7 +23377,7 @@
         <v>209</v>
       </c>
       <c r="C213" s="71" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D213" s="72"/>
       <c r="E213" s="72"/>
@@ -24887,7 +24891,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3CD6B57-0370-464C-92D1-8CCB08728235}">
   <dimension ref="C2:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -25228,19 +25232,19 @@
     </row>
     <row r="21" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C21" s="47" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D21" s="47" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E21" s="47">
         <v>7</v>
       </c>
       <c r="G21" s="12" t="s">
+        <v>417</v>
+      </c>
+      <c r="H21" s="12" t="s">
         <v>418</v>
-      </c>
-      <c r="H21" s="12" t="s">
-        <v>419</v>
       </c>
       <c r="I21" s="12">
         <v>4</v>
@@ -29681,7 +29685,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="53" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D5" s="54"/>
       <c r="E5" s="54"/>
@@ -29839,7 +29843,7 @@
         <v>5</v>
       </c>
       <c r="C9" s="70" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D9" s="70"/>
       <c r="E9" s="70"/>
@@ -29879,7 +29883,7 @@
         <v>6</v>
       </c>
       <c r="C10" s="70" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D10" s="70"/>
       <c r="E10" s="70"/>
@@ -29919,7 +29923,7 @@
         <v>7</v>
       </c>
       <c r="C11" s="70" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D11" s="70"/>
       <c r="E11" s="70"/>
@@ -29997,7 +30001,7 @@
         <v>9</v>
       </c>
       <c r="C13" s="70" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D13" s="70"/>
       <c r="E13" s="70"/>
@@ -30075,7 +30079,7 @@
         <v>11</v>
       </c>
       <c r="C15" s="70" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D15" s="70"/>
       <c r="E15" s="70"/>

</xml_diff>